<commit_message>
Added data importer to DF format
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitza\Desktop\automated shifts assignment\Automated-shifts-assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Desktop\לימודים\Shibutzi\Automated-shifts-assignment\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B5C4A9-0F07-4000-8618-3DB3A45830F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{241C700C-B428-4812-A429-555BCE3AB957}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
     <sheet name="Tasks" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="155">
   <si>
     <t>id</t>
   </si>
@@ -46,12 +45,6 @@
     <t>tasks availeble</t>
   </si>
   <si>
-    <t>TIME - (Start,End)</t>
-  </si>
-  <si>
-    <t>Competible with</t>
-  </si>
-  <si>
     <t>pazam: 1-youngest etc</t>
   </si>
   <si>
@@ -196,78 +189,6 @@
     <t>T18</t>
   </si>
   <si>
-    <t>T19</t>
-  </si>
-  <si>
-    <t>T20</t>
-  </si>
-  <si>
-    <t>T21</t>
-  </si>
-  <si>
-    <t>T22</t>
-  </si>
-  <si>
-    <t>T23</t>
-  </si>
-  <si>
-    <t>T24</t>
-  </si>
-  <si>
-    <t>T25</t>
-  </si>
-  <si>
-    <t>T26</t>
-  </si>
-  <si>
-    <t>T27</t>
-  </si>
-  <si>
-    <t>T28</t>
-  </si>
-  <si>
-    <t>T29</t>
-  </si>
-  <si>
-    <t>T30</t>
-  </si>
-  <si>
-    <t>T31</t>
-  </si>
-  <si>
-    <t>T32</t>
-  </si>
-  <si>
-    <t>T33</t>
-  </si>
-  <si>
-    <t>T34</t>
-  </si>
-  <si>
-    <t>T35</t>
-  </si>
-  <si>
-    <t>T36</t>
-  </si>
-  <si>
-    <t>T37</t>
-  </si>
-  <si>
-    <t>T38</t>
-  </si>
-  <si>
-    <t>T39</t>
-  </si>
-  <si>
-    <t>T40</t>
-  </si>
-  <si>
-    <t>T41</t>
-  </si>
-  <si>
-    <t>T42</t>
-  </si>
-  <si>
     <t>bakut day 1</t>
   </si>
   <si>
@@ -298,24 +219,9 @@
     <t xml:space="preserve">ftt </t>
   </si>
   <si>
-    <t>08:00-20:00</t>
-  </si>
-  <si>
-    <t>08:00-14:00</t>
-  </si>
-  <si>
-    <t>08:00-18:00</t>
-  </si>
-  <si>
     <t>marzuk</t>
   </si>
   <si>
-    <t>08:15-19:00</t>
-  </si>
-  <si>
-    <t>08:30-17:30</t>
-  </si>
-  <si>
     <t>equip operator</t>
   </si>
   <si>
@@ -394,27 +300,6 @@
     <t>ITAY AVENSH</t>
   </si>
   <si>
-    <t xml:space="preserve">YEARA </t>
-  </si>
-  <si>
-    <t>REUT</t>
-  </si>
-  <si>
-    <t>BAR S</t>
-  </si>
-  <si>
-    <t>YOSSI</t>
-  </si>
-  <si>
-    <t>ITAY HEVER</t>
-  </si>
-  <si>
-    <t>NADAV P</t>
-  </si>
-  <si>
-    <t>DANA S</t>
-  </si>
-  <si>
     <t>NOYA</t>
   </si>
   <si>
@@ -514,27 +399,6 @@
     <t>O42</t>
   </si>
   <si>
-    <t>O43</t>
-  </si>
-  <si>
-    <t>O44</t>
-  </si>
-  <si>
-    <t>O45</t>
-  </si>
-  <si>
-    <t>O46</t>
-  </si>
-  <si>
-    <t>O47</t>
-  </si>
-  <si>
-    <t>O48</t>
-  </si>
-  <si>
-    <t>O49</t>
-  </si>
-  <si>
     <t>AVIA KLINE</t>
   </si>
   <si>
@@ -619,33 +483,39 @@
     <t>T1, T2, T5</t>
   </si>
   <si>
-    <t xml:space="preserve">DAY-LENGTH </t>
-  </si>
-  <si>
-    <t>COST</t>
-  </si>
-  <si>
     <t>MIN</t>
   </si>
   <si>
     <t>MAX</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>start-hour</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>Compatible</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -682,10 +552,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -999,21 +870,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2FC051-7E27-4761-B6CF-78CE51777849}">
-  <dimension ref="A1:G50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="3" width="26.21875" customWidth="1"/>
-    <col min="4" max="4" width="52.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.125" customWidth="1"/>
+    <col min="3" max="3" width="26.25" customWidth="1"/>
+    <col min="4" max="4" width="52.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1021,30 +892,30 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>196</v>
+        <v>149</v>
       </c>
       <c r="F1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>173</v>
+        <v>128</v>
       </c>
       <c r="E2">
         <v>8</v>
@@ -1052,22 +923,19 @@
       <c r="F2">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>127</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>173</v>
+        <v>128</v>
       </c>
       <c r="E3">
         <v>8</v>
@@ -1075,22 +943,19 @@
       <c r="F3">
         <v>14</v>
       </c>
-      <c r="G3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>173</v>
+        <v>128</v>
       </c>
       <c r="E4">
         <v>8</v>
@@ -1098,22 +963,19 @@
       <c r="F4">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>175</v>
+        <v>130</v>
       </c>
       <c r="E5">
         <v>8</v>
@@ -1121,22 +983,19 @@
       <c r="F5">
         <v>14</v>
       </c>
-      <c r="G5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>175</v>
+        <v>130</v>
       </c>
       <c r="E6">
         <v>8</v>
@@ -1144,22 +1003,19 @@
       <c r="F6">
         <v>14</v>
       </c>
-      <c r="G6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>175</v>
+        <v>130</v>
       </c>
       <c r="E7">
         <v>8</v>
@@ -1167,22 +1023,19 @@
       <c r="F7">
         <v>14</v>
       </c>
-      <c r="G7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>173</v>
+        <v>128</v>
       </c>
       <c r="E8">
         <v>8</v>
@@ -1190,22 +1043,19 @@
       <c r="F8">
         <v>14</v>
       </c>
-      <c r="G8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>173</v>
+        <v>128</v>
       </c>
       <c r="E9">
         <v>8</v>
@@ -1214,18 +1064,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>173</v>
+        <v>128</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -1234,18 +1084,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>173</v>
+        <v>128</v>
       </c>
       <c r="E11">
         <v>6</v>
@@ -1254,18 +1104,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>173</v>
+        <v>128</v>
       </c>
       <c r="E12">
         <v>6</v>
@@ -1274,18 +1124,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>88</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>175</v>
+        <v>130</v>
       </c>
       <c r="E13">
         <v>6</v>
@@ -1294,18 +1144,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>176</v>
+        <v>131</v>
       </c>
       <c r="E14">
         <v>6</v>
@@ -1314,18 +1164,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>179</v>
+        <v>134</v>
       </c>
       <c r="E15">
         <v>4</v>
@@ -1334,18 +1184,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="C16">
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>180</v>
+        <v>135</v>
       </c>
       <c r="E16">
         <v>4.5</v>
@@ -1354,18 +1204,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>181</v>
+        <v>136</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -1374,18 +1224,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C18">
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>181</v>
+        <v>136</v>
       </c>
       <c r="E18">
         <v>4</v>
@@ -1394,18 +1244,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>182</v>
+        <v>137</v>
       </c>
       <c r="E19">
         <v>4</v>
@@ -1414,18 +1264,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="C20">
         <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>177</v>
+        <v>132</v>
       </c>
       <c r="E20">
         <v>4</v>
@@ -1434,18 +1284,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="C21">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E21">
         <v>2</v>
@@ -1454,158 +1304,158 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>134</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>138</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="B22" t="s">
-        <v>105</v>
-      </c>
-      <c r="C22">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>179</v>
-      </c>
-      <c r="E22">
-        <v>4</v>
-      </c>
-      <c r="F22">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>129</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B23" t="s">
-        <v>106</v>
-      </c>
-      <c r="C23">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>183</v>
-      </c>
-      <c r="E23">
-        <v>4</v>
-      </c>
-      <c r="F23">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>129</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+      <c r="F25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>137</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>129</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
         <v>132</v>
       </c>
-      <c r="C24">
-        <v>4</v>
-      </c>
-      <c r="D24" t="s">
-        <v>174</v>
-      </c>
-      <c r="E24">
-        <v>4</v>
-      </c>
-      <c r="F24">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" t="s">
-        <v>133</v>
-      </c>
-      <c r="C25">
-        <v>4</v>
-      </c>
-      <c r="D25" t="s">
-        <v>174</v>
-      </c>
-      <c r="E25">
-        <v>4</v>
-      </c>
-      <c r="F25">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" t="s">
-        <v>134</v>
-      </c>
-      <c r="C26">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>182</v>
-      </c>
-      <c r="E26">
-        <v>4</v>
-      </c>
-      <c r="F26">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>31</v>
       </c>
-      <c r="B27" t="s">
-        <v>135</v>
-      </c>
-      <c r="C27">
-        <v>4</v>
-      </c>
-      <c r="D27" t="s">
-        <v>174</v>
-      </c>
-      <c r="E27">
-        <v>4</v>
-      </c>
-      <c r="F27">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" t="s">
-        <v>136</v>
-      </c>
-      <c r="C28">
-        <v>4</v>
-      </c>
-      <c r="D28" t="s">
-        <v>177</v>
-      </c>
-      <c r="E28">
-        <v>4</v>
-      </c>
-      <c r="F28">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>33</v>
-      </c>
       <c r="B29" t="s">
-        <v>137</v>
+        <v>99</v>
       </c>
       <c r="C29">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>184</v>
+        <v>139</v>
       </c>
       <c r="E29">
         <v>3</v>
@@ -1614,18 +1464,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>138</v>
+        <v>100</v>
       </c>
       <c r="C30">
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>178</v>
+        <v>133</v>
       </c>
       <c r="E30">
         <v>2</v>
@@ -1634,18 +1484,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>145</v>
+        <v>107</v>
       </c>
       <c r="B31" t="s">
-        <v>139</v>
+        <v>101</v>
       </c>
       <c r="C31">
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="E31">
         <v>4</v>
@@ -1654,18 +1504,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>146</v>
+        <v>108</v>
       </c>
       <c r="B32" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="C32">
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>186</v>
+        <v>141</v>
       </c>
       <c r="E32">
         <v>2</v>
@@ -1674,18 +1524,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>147</v>
+        <v>109</v>
       </c>
       <c r="B33" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="C33">
         <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>179</v>
+        <v>134</v>
       </c>
       <c r="E33">
         <v>2.5</v>
@@ -1694,18 +1544,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="B34" t="s">
-        <v>141</v>
+        <v>103</v>
       </c>
       <c r="C34">
         <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>187</v>
+        <v>142</v>
       </c>
       <c r="E34">
         <v>2.5</v>
@@ -1714,18 +1564,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="B35" t="s">
-        <v>142</v>
+        <v>104</v>
       </c>
       <c r="C35">
         <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>187</v>
+        <v>142</v>
       </c>
       <c r="E35">
         <v>2.5</v>
@@ -1734,18 +1584,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="B36" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="C36">
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>188</v>
+        <v>143</v>
       </c>
       <c r="E36">
         <v>3</v>
@@ -1754,18 +1604,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="B37" t="s">
-        <v>144</v>
+        <v>106</v>
       </c>
       <c r="C37">
         <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>189</v>
+        <v>144</v>
       </c>
       <c r="E37">
         <v>2</v>
@@ -1774,18 +1624,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>152</v>
+        <v>114</v>
       </c>
       <c r="B38" t="s">
-        <v>166</v>
+        <v>121</v>
       </c>
       <c r="C38">
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>190</v>
+        <v>145</v>
       </c>
       <c r="E38">
         <v>2</v>
@@ -1794,18 +1644,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>153</v>
+        <v>115</v>
       </c>
       <c r="B39" t="s">
-        <v>167</v>
+        <v>122</v>
       </c>
       <c r="C39">
         <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>191</v>
+        <v>146</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -1814,18 +1664,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>155</v>
+        <v>117</v>
       </c>
       <c r="B40" t="s">
-        <v>168</v>
+        <v>123</v>
       </c>
       <c r="C40">
         <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>192</v>
+        <v>147</v>
       </c>
       <c r="E40">
         <v>3</v>
@@ -1834,18 +1684,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>156</v>
+        <v>118</v>
       </c>
       <c r="B41" t="s">
-        <v>169</v>
+        <v>124</v>
       </c>
       <c r="C41">
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>191</v>
+        <v>146</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -1854,18 +1704,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>157</v>
+        <v>119</v>
       </c>
       <c r="B42" t="s">
-        <v>170</v>
+        <v>125</v>
       </c>
       <c r="C42">
         <v>9</v>
       </c>
       <c r="D42" t="s">
-        <v>189</v>
+        <v>144</v>
       </c>
       <c r="E42">
         <v>2</v>
@@ -1874,18 +1724,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>158</v>
+        <v>120</v>
       </c>
       <c r="B43" t="s">
-        <v>171</v>
+        <v>126</v>
       </c>
       <c r="C43">
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>193</v>
+        <v>148</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -1894,40 +1744,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>165</v>
-      </c>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1936,22 +1754,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8936557-B087-4F9F-9B32-E00C4EB10571}">
-  <dimension ref="A1:F43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="28.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="2" max="3" width="21.375" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="28.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1959,473 +1776,357 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>152</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>153</v>
       </c>
       <c r="E1" t="s">
-        <v>194</v>
+        <v>154</v>
       </c>
       <c r="F1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
+        <v>52</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
+        <v>53</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D4">
+        <v>24</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
+        <v>54</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D5">
+        <v>24</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
+        <v>55</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
+        <v>56</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D7">
+        <v>24</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
+        <v>57</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
+        <v>58</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D9">
+        <v>24</v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D10" t="s">
-        <v>99</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>68</v>
       </c>
       <c r="F10">
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
-      </c>
-      <c r="C12" t="s">
-        <v>89</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" t="s">
-        <v>101</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
+        <v>60</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D13">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>70</v>
       </c>
       <c r="F13">
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C14" t="s">
-        <v>91</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
+        <v>61</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D14">
+        <v>9</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
-      </c>
-      <c r="C15" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" t="s">
-        <v>102</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
+        <v>62</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D15">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>71</v>
       </c>
       <c r="F15">
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
-      </c>
-      <c r="C16" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" t="s">
-        <v>102</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D16">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>71</v>
       </c>
       <c r="F16">
         <v>0.25</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" t="s">
-        <v>102</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
+        <v>66</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D17">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>71</v>
       </c>
       <c r="F17">
         <v>0.25</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
-      </c>
-      <c r="C18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" t="s">
-        <v>102</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
+        <v>67</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D18">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>71</v>
       </c>
       <c r="F18">
         <v>0.25</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>100</v>
-      </c>
-      <c r="C19" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" t="s">
-        <v>103</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
+        <v>69</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D19">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>72</v>
       </c>
       <c r="F19">
         <v>0.25</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>76</v>
-      </c>
+    <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C1048576" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added wants for operators in db
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Desktop\לימודים\Shibutzi\Automated-shifts-assignment\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noabe\Desktop\omri\auto-shifts\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2DDD12-E5DF-4E2F-B0D4-09A0D71AF2F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
@@ -20,21 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="201">
   <si>
     <t>id</t>
   </si>
@@ -499,12 +491,150 @@
   </si>
   <si>
     <t>Compatible</t>
+  </si>
+  <si>
+    <t>1,26,27</t>
+  </si>
+  <si>
+    <t>9,17,26,27</t>
+  </si>
+  <si>
+    <t>5,6,19,20</t>
+  </si>
+  <si>
+    <t>10,18,23</t>
+  </si>
+  <si>
+    <t>9,12,13,26,27</t>
+  </si>
+  <si>
+    <t>14,25,31</t>
+  </si>
+  <si>
+    <t>1,3,12,13,24</t>
+  </si>
+  <si>
+    <t>2,11,17,23</t>
+  </si>
+  <si>
+    <t>12,13,26,27</t>
+  </si>
+  <si>
+    <t>5,6,12,13</t>
+  </si>
+  <si>
+    <t>2,9</t>
+  </si>
+  <si>
+    <t>8,12,13,26,27</t>
+  </si>
+  <si>
+    <t>5,6,26,27</t>
+  </si>
+  <si>
+    <t>4,9,15,22,29</t>
+  </si>
+  <si>
+    <t>26,27</t>
+  </si>
+  <si>
+    <t>2,9,15,23</t>
+  </si>
+  <si>
+    <t>2,9,18,23,30</t>
+  </si>
+  <si>
+    <t>9,25</t>
+  </si>
+  <si>
+    <t>4,9,16</t>
+  </si>
+  <si>
+    <t>9,18,23,30</t>
+  </si>
+  <si>
+    <t>11,12,13</t>
+  </si>
+  <si>
+    <t>11,14,23</t>
+  </si>
+  <si>
+    <t>19,20,26,27</t>
+  </si>
+  <si>
+    <t>19,20,26,27,30</t>
+  </si>
+  <si>
+    <t>7,17,26,27</t>
+  </si>
+  <si>
+    <t>3,23,29</t>
+  </si>
+  <si>
+    <t>2,9,16,23</t>
+  </si>
+  <si>
+    <t>1,3,4,5,6,9,16,23,26,27</t>
+  </si>
+  <si>
+    <t>3,14,17</t>
+  </si>
+  <si>
+    <t>3,5,6,17,25,26,27</t>
+  </si>
+  <si>
+    <t>3,10,21,23,26,27,28</t>
+  </si>
+  <si>
+    <t>17,25</t>
+  </si>
+  <si>
+    <t>9,19,20,26,27,28</t>
+  </si>
+  <si>
+    <t>10,11,18,19,20,21,26,27</t>
+  </si>
+  <si>
+    <t>10,11,26,27,28</t>
+  </si>
+  <si>
+    <t>7,15,23</t>
+  </si>
+  <si>
+    <t>2,3,5,6,10,21,26,27</t>
+  </si>
+  <si>
+    <t>11,12,13,14,26,27</t>
+  </si>
+  <si>
+    <t>1,11</t>
+  </si>
+  <si>
+    <t>2,3,4,5,6,8,10,11,17,23,25,26,27</t>
+  </si>
+  <si>
+    <t>9,10,11,14,15,16,17,18,19,20,21,23,25,26,27,28</t>
+  </si>
+  <si>
+    <t>7,23</t>
+  </si>
+  <si>
+    <t>26,27,28</t>
+  </si>
+  <si>
+    <t>8,10,11,12,13,25,26,27</t>
+  </si>
+  <si>
+    <t>Not evening</t>
+  </si>
+  <si>
+    <t>Not task</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -870,21 +1000,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
-    <col min="3" max="3" width="26.25" customWidth="1"/>
-    <col min="4" max="4" width="52.125" customWidth="1"/>
+    <col min="2" max="2" width="15.09765625" customWidth="1"/>
+    <col min="3" max="3" width="26.19921875" customWidth="1"/>
+    <col min="4" max="4" width="52.09765625" customWidth="1"/>
+    <col min="7" max="7" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -903,8 +1035,14 @@
       <c r="F1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -923,8 +1061,11 @@
       <c r="F2">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -943,8 +1084,11 @@
       <c r="F3">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -963,8 +1107,14 @@
       <c r="F4">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>171</v>
+      </c>
+      <c r="H4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -983,8 +1133,14 @@
       <c r="F5">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>173</v>
+      </c>
+      <c r="H5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1003,8 +1159,14 @@
       <c r="F6">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>172</v>
+      </c>
+      <c r="H6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1023,8 +1185,14 @@
       <c r="F7">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>174</v>
+      </c>
+      <c r="H7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1043,8 +1211,14 @@
       <c r="F8">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>170</v>
+      </c>
+      <c r="H8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1063,8 +1237,14 @@
       <c r="F9">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>165</v>
+      </c>
+      <c r="H9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1083,8 +1263,14 @@
       <c r="F10">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>168</v>
+      </c>
+      <c r="H10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1103,8 +1289,14 @@
       <c r="F11">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>162</v>
+      </c>
+      <c r="H11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1123,8 +1315,14 @@
       <c r="F12">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>23</v>
+      </c>
+      <c r="H12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1143,8 +1341,14 @@
       <c r="F13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>176</v>
+      </c>
+      <c r="H13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1163,8 +1367,14 @@
       <c r="F14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>23</v>
+      </c>
+      <c r="H14" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1183,8 +1393,11 @@
       <c r="F15">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1203,8 +1416,14 @@
       <c r="F16">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>160</v>
+      </c>
+      <c r="H16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1223,8 +1442,11 @@
       <c r="F17">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1243,8 +1465,14 @@
       <c r="F18">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>8</v>
+      </c>
+      <c r="H18" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1263,8 +1491,14 @@
       <c r="F19">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>165</v>
+      </c>
+      <c r="H19" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1283,8 +1517,14 @@
       <c r="F20">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>180</v>
+      </c>
+      <c r="H20" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1304,7 +1544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1323,8 +1563,14 @@
       <c r="F22">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <v>10</v>
+      </c>
+      <c r="H22" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1343,8 +1589,14 @@
       <c r="F23">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>158</v>
+      </c>
+      <c r="H23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1363,8 +1615,11 @@
       <c r="F24">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1383,8 +1638,14 @@
       <c r="F25">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" t="s">
+        <v>186</v>
+      </c>
+      <c r="H25" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1403,8 +1664,11 @@
       <c r="F26">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1423,8 +1687,11 @@
       <c r="F27">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
@@ -1443,8 +1710,14 @@
       <c r="F28">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>10</v>
+      </c>
+      <c r="H28" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1463,8 +1736,14 @@
       <c r="F29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>7</v>
+      </c>
+      <c r="H29" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1483,8 +1762,14 @@
       <c r="F30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>190</v>
+      </c>
+      <c r="H30" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>107</v>
       </c>
@@ -1503,8 +1788,14 @@
       <c r="F31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>7</v>
+      </c>
+      <c r="H31" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>108</v>
       </c>
@@ -1523,8 +1814,14 @@
       <c r="F32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>196</v>
+      </c>
+      <c r="H32" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>109</v>
       </c>
@@ -1543,8 +1840,11 @@
       <c r="F33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>110</v>
       </c>
@@ -1563,8 +1863,14 @@
       <c r="F34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>7</v>
+      </c>
+      <c r="H34" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>111</v>
       </c>
@@ -1583,8 +1889,11 @@
       <c r="F35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H35" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>112</v>
       </c>
@@ -1604,7 +1913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>113</v>
       </c>
@@ -1624,7 +1933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>114</v>
       </c>
@@ -1643,8 +1952,14 @@
       <c r="F38">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>25</v>
+      </c>
+      <c r="H38" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>115</v>
       </c>
@@ -1664,7 +1979,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>117</v>
       </c>
@@ -1683,8 +1998,11 @@
       <c r="F40">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H40" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>118</v>
       </c>
@@ -1703,8 +2021,11 @@
       <c r="F41">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>119</v>
       </c>
@@ -1723,8 +2044,11 @@
       <c r="F42">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H42" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>120</v>
       </c>
@@ -1743,8 +2067,11 @@
       <c r="F43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H43" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
     </row>
   </sheetData>
@@ -1754,21 +2081,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="21.375" customWidth="1"/>
+    <col min="2" max="3" width="21.3984375" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="28.375" customWidth="1"/>
+    <col min="5" max="5" width="28.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1788,7 +2115,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1808,7 +2135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1828,7 +2155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1845,7 +2172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1862,7 +2189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -1879,7 +2206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -1896,7 +2223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1913,7 +2240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -1930,7 +2257,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1950,7 +2277,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1967,7 +2294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1984,7 +2311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -2004,7 +2331,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -2021,7 +2348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2041,7 +2368,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -2061,7 +2388,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -2081,7 +2408,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -2101,7 +2428,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -2121,7 +2448,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added probability for tasks and preferences
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Desktop\לימודים\Shibutzi\Automated-shifts-assignment\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Desktop\לימודים\Shibutzi\Automated-shifts-assignment\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="202">
   <si>
     <t>id</t>
   </si>
@@ -499,6 +490,147 @@
   </si>
   <si>
     <t>Compatible</t>
+  </si>
+  <si>
+    <t>1,26,27</t>
+  </si>
+  <si>
+    <t>9,17,26,27</t>
+  </si>
+  <si>
+    <t>5,6,19,20</t>
+  </si>
+  <si>
+    <t>10,18,23</t>
+  </si>
+  <si>
+    <t>9,12,13,26,27</t>
+  </si>
+  <si>
+    <t>14,25,31</t>
+  </si>
+  <si>
+    <t>1,3,12,13,24</t>
+  </si>
+  <si>
+    <t>2,11,17,23</t>
+  </si>
+  <si>
+    <t>12,13,26,27</t>
+  </si>
+  <si>
+    <t>5,6,12,13</t>
+  </si>
+  <si>
+    <t>2,9</t>
+  </si>
+  <si>
+    <t>8,12,13,26,27</t>
+  </si>
+  <si>
+    <t>5,6,26,27</t>
+  </si>
+  <si>
+    <t>4,9,15,22,29</t>
+  </si>
+  <si>
+    <t>26,27</t>
+  </si>
+  <si>
+    <t>2,9,15,23</t>
+  </si>
+  <si>
+    <t>2,9,18,23,30</t>
+  </si>
+  <si>
+    <t>9,25</t>
+  </si>
+  <si>
+    <t>4,9,16</t>
+  </si>
+  <si>
+    <t>9,18,23,30</t>
+  </si>
+  <si>
+    <t>11,12,13</t>
+  </si>
+  <si>
+    <t>11,14,23</t>
+  </si>
+  <si>
+    <t>19,20,26,27</t>
+  </si>
+  <si>
+    <t>19,20,26,27,30</t>
+  </si>
+  <si>
+    <t>7,17,26,27</t>
+  </si>
+  <si>
+    <t>3,23,29</t>
+  </si>
+  <si>
+    <t>2,9,16,23</t>
+  </si>
+  <si>
+    <t>1,3,4,5,6,9,16,23,26,27</t>
+  </si>
+  <si>
+    <t>3,14,17</t>
+  </si>
+  <si>
+    <t>3,5,6,17,25,26,27</t>
+  </si>
+  <si>
+    <t>3,10,21,23,26,27,28</t>
+  </si>
+  <si>
+    <t>17,25</t>
+  </si>
+  <si>
+    <t>9,19,20,26,27,28</t>
+  </si>
+  <si>
+    <t>10,11,18,19,20,21,26,27</t>
+  </si>
+  <si>
+    <t>10,11,26,27,28</t>
+  </si>
+  <si>
+    <t>7,15,23</t>
+  </si>
+  <si>
+    <t>2,3,5,6,10,21,26,27</t>
+  </si>
+  <si>
+    <t>11,12,13,14,26,27</t>
+  </si>
+  <si>
+    <t>1,11</t>
+  </si>
+  <si>
+    <t>2,3,4,5,6,8,10,11,17,23,25,26,27</t>
+  </si>
+  <si>
+    <t>9,10,11,14,15,16,17,18,19,20,21,23,25,26,27,28</t>
+  </si>
+  <si>
+    <t>7,23</t>
+  </si>
+  <si>
+    <t>26,27,28</t>
+  </si>
+  <si>
+    <t>8,10,11,12,13,25,26,27</t>
+  </si>
+  <si>
+    <t>Not evening</t>
+  </si>
+  <si>
+    <t>Not task</t>
+  </si>
+  <si>
+    <t>probability</t>
   </si>
 </sst>
 </file>
@@ -871,10 +1003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -882,9 +1014,11 @@
     <col min="2" max="2" width="15.125" customWidth="1"/>
     <col min="3" max="3" width="26.25" customWidth="1"/>
     <col min="4" max="4" width="52.125" customWidth="1"/>
+    <col min="7" max="7" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -903,8 +1037,14 @@
       <c r="F1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -923,8 +1063,11 @@
       <c r="F2">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -943,8 +1086,11 @@
       <c r="F3">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -963,8 +1109,14 @@
       <c r="F4">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>171</v>
+      </c>
+      <c r="H4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -983,8 +1135,14 @@
       <c r="F5">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>173</v>
+      </c>
+      <c r="H5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1003,8 +1161,14 @@
       <c r="F6">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>172</v>
+      </c>
+      <c r="H6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1023,8 +1187,14 @@
       <c r="F7">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>174</v>
+      </c>
+      <c r="H7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1043,8 +1213,14 @@
       <c r="F8">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>170</v>
+      </c>
+      <c r="H8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1063,8 +1239,14 @@
       <c r="F9">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>165</v>
+      </c>
+      <c r="H9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1083,8 +1265,14 @@
       <c r="F10">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>168</v>
+      </c>
+      <c r="H10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1103,8 +1291,14 @@
       <c r="F11">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>162</v>
+      </c>
+      <c r="H11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1123,8 +1317,14 @@
       <c r="F12">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>23</v>
+      </c>
+      <c r="H12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1143,8 +1343,14 @@
       <c r="F13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>176</v>
+      </c>
+      <c r="H13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1163,8 +1369,14 @@
       <c r="F14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>23</v>
+      </c>
+      <c r="H14" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1183,8 +1395,11 @@
       <c r="F15">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1203,8 +1418,14 @@
       <c r="F16">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>160</v>
+      </c>
+      <c r="H16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1223,8 +1444,11 @@
       <c r="F17">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1243,8 +1467,14 @@
       <c r="F18">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>8</v>
+      </c>
+      <c r="H18" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1263,8 +1493,14 @@
       <c r="F19">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>165</v>
+      </c>
+      <c r="H19" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1283,8 +1519,14 @@
       <c r="F20">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>180</v>
+      </c>
+      <c r="H20" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1304,7 +1546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1323,8 +1565,14 @@
       <c r="F22">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <v>10</v>
+      </c>
+      <c r="H22" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1343,8 +1591,14 @@
       <c r="F23">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>158</v>
+      </c>
+      <c r="H23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1363,8 +1617,11 @@
       <c r="F24">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1383,8 +1640,14 @@
       <c r="F25">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" t="s">
+        <v>186</v>
+      </c>
+      <c r="H25" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1403,8 +1666,11 @@
       <c r="F26">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1423,8 +1689,11 @@
       <c r="F27">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
@@ -1443,8 +1712,14 @@
       <c r="F28">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>10</v>
+      </c>
+      <c r="H28" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1463,8 +1738,14 @@
       <c r="F29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>7</v>
+      </c>
+      <c r="H29" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1483,8 +1764,14 @@
       <c r="F30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>190</v>
+      </c>
+      <c r="H30" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>107</v>
       </c>
@@ -1503,8 +1790,14 @@
       <c r="F31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>7</v>
+      </c>
+      <c r="H31" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>108</v>
       </c>
@@ -1523,8 +1816,14 @@
       <c r="F32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>196</v>
+      </c>
+      <c r="H32" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>109</v>
       </c>
@@ -1543,8 +1842,11 @@
       <c r="F33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>110</v>
       </c>
@@ -1563,8 +1865,14 @@
       <c r="F34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>7</v>
+      </c>
+      <c r="H34" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>111</v>
       </c>
@@ -1583,8 +1891,11 @@
       <c r="F35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H35" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>112</v>
       </c>
@@ -1604,7 +1915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>113</v>
       </c>
@@ -1624,7 +1935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>114</v>
       </c>
@@ -1643,8 +1954,14 @@
       <c r="F38">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>25</v>
+      </c>
+      <c r="H38" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>115</v>
       </c>
@@ -1664,7 +1981,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>117</v>
       </c>
@@ -1683,8 +2000,11 @@
       <c r="F40">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H40" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>118</v>
       </c>
@@ -1703,8 +2023,11 @@
       <c r="F41">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>119</v>
       </c>
@@ -1723,8 +2046,11 @@
       <c r="F42">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H42" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>120</v>
       </c>
@@ -1743,8 +2069,11 @@
       <c r="F43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H43" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
     </row>
   </sheetData>
@@ -1755,10 +2084,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1048576"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1768,7 +2097,7 @@
     <col min="5" max="5" width="28.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1787,8 +2116,11 @@
       <c r="F1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1807,8 +2139,11 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1827,8 +2162,11 @@
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1844,8 +2182,11 @@
       <c r="F4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1861,8 +2202,11 @@
       <c r="F5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -1878,8 +2222,11 @@
       <c r="F6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -1895,8 +2242,11 @@
       <c r="F7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1912,8 +2262,11 @@
       <c r="F8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -1929,8 +2282,11 @@
       <c r="F9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1949,8 +2305,11 @@
       <c r="F10">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1966,8 +2325,11 @@
       <c r="F11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1983,8 +2345,11 @@
       <c r="F12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -2003,8 +2368,11 @@
       <c r="F13">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -2020,8 +2388,11 @@
       <c r="F14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2040,8 +2411,11 @@
       <c r="F15">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -2060,8 +2434,11 @@
       <c r="F16">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -2080,8 +2457,11 @@
       <c r="F17">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -2100,8 +2480,11 @@
       <c r="F18">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -2119,6 +2502,9 @@
       </c>
       <c r="F19">
         <v>0.25</v>
+      </c>
+      <c r="G19">
+        <v>0.4</v>
       </c>
     </row>
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixed data importer by probability
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="156">
   <si>
     <t>id</t>
   </si>
@@ -499,6 +499,9 @@
   </si>
   <si>
     <t>tasks available</t>
+  </si>
+  <si>
+    <t>probability</t>
   </si>
 </sst>
 </file>
@@ -873,7 +876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -1755,10 +1758,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1048576"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1768,7 +1771,7 @@
     <col min="5" max="5" width="28.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1787,8 +1790,11 @@
       <c r="F1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1807,8 +1813,11 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1827,8 +1836,11 @@
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1844,8 +1856,11 @@
       <c r="F4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1861,8 +1876,11 @@
       <c r="F5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1878,8 +1896,11 @@
       <c r="F6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1895,8 +1916,11 @@
       <c r="F7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1912,8 +1936,11 @@
       <c r="F8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1929,8 +1956,11 @@
       <c r="F9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1949,8 +1979,11 @@
       <c r="F10">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1966,8 +1999,11 @@
       <c r="F11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -1983,8 +2019,11 @@
       <c r="F12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -2003,8 +2042,11 @@
       <c r="F13">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2020,8 +2062,11 @@
       <c r="F14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -2040,8 +2085,11 @@
       <c r="F15">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -2060,8 +2108,11 @@
       <c r="F16">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -2080,8 +2131,11 @@
       <c r="F17">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -2100,8 +2154,11 @@
       <c r="F18">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -2118,6 +2175,9 @@
         <v>71</v>
       </c>
       <c r="F19">
+        <v>0.25</v>
+      </c>
+      <c r="G19">
         <v>0.25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cleaned Dataframe from functions input
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Desktop\לימודים\Shibutzi\Automated-shifts-assignment\DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitza\Desktop\automated shifts assignment\Automated-shifts-assignment\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAD5EE9-F210-4E3B-A210-63C8DA0427F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
@@ -20,21 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="157">
   <si>
     <t>id</t>
   </si>
@@ -502,23 +494,26 @@
   </si>
   <si>
     <t>probability</t>
+  </si>
+  <si>
+    <t>min_per_month</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -873,21 +868,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
-    <col min="3" max="3" width="26.25" customWidth="1"/>
-    <col min="4" max="4" width="52.125" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" customWidth="1"/>
+    <col min="4" max="4" width="52.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -907,7 +902,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -927,7 +922,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -947,7 +942,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -967,7 +962,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -987,7 +982,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1007,7 +1002,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1027,7 +1022,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1047,7 +1042,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1067,7 +1062,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1087,7 +1082,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1107,7 +1102,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1127,7 +1122,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1147,7 +1142,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1167,7 +1162,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1187,7 +1182,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1207,7 +1202,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1227,7 +1222,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1247,7 +1242,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1267,7 +1262,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1287,7 +1282,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1307,7 +1302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1327,7 +1322,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1347,7 +1342,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1367,7 +1362,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1387,7 +1382,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1407,7 +1402,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1427,7 +1422,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>29</v>
       </c>
@@ -1447,7 +1442,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1467,7 +1462,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1487,7 +1482,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>106</v>
       </c>
@@ -1507,7 +1502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>107</v>
       </c>
@@ -1527,7 +1522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>108</v>
       </c>
@@ -1547,7 +1542,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>109</v>
       </c>
@@ -1567,7 +1562,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>110</v>
       </c>
@@ -1587,7 +1582,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>111</v>
       </c>
@@ -1607,7 +1602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>112</v>
       </c>
@@ -1627,7 +1622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>113</v>
       </c>
@@ -1647,7 +1642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -1667,7 +1662,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>116</v>
       </c>
@@ -1687,7 +1682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>117</v>
       </c>
@@ -1707,7 +1702,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>118</v>
       </c>
@@ -1727,7 +1722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>119</v>
       </c>
@@ -1747,7 +1742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
     </row>
   </sheetData>
@@ -1757,21 +1752,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="21.375" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="28.375" customWidth="1"/>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1793,8 +1793,11 @@
       <c r="G1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1816,8 +1819,11 @@
       <c r="G2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1839,8 +1845,11 @@
       <c r="G3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1859,8 +1868,11 @@
       <c r="G4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1879,8 +1891,11 @@
       <c r="G5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1899,8 +1914,11 @@
       <c r="G6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1919,8 +1937,11 @@
       <c r="G7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1939,8 +1960,11 @@
       <c r="G8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1959,8 +1983,11 @@
       <c r="G9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1982,8 +2009,11 @@
       <c r="G10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -2002,8 +2032,11 @@
       <c r="G11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -2022,8 +2055,11 @@
       <c r="G12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -2045,8 +2081,11 @@
       <c r="G13">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2065,8 +2104,11 @@
       <c r="G14">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -2088,8 +2130,11 @@
       <c r="G15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -2111,8 +2156,11 @@
       <c r="G16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -2134,8 +2182,11 @@
       <c r="G17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -2157,8 +2208,11 @@
       <c r="G18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -2180,8 +2234,11 @@
       <c r="G19">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1048576" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1048576" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added minimum per task type
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitza\Desktop\automated shifts assignment\Automated-shifts-assignment\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAD5EE9-F210-4E3B-A210-63C8DA0427F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAFA645-A588-4E1C-B4BF-056CCE0F763D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="182">
   <si>
     <t>id</t>
   </si>
@@ -497,6 +497,81 @@
   </si>
   <si>
     <t>min_per_month</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>bakut</t>
+  </si>
+  <si>
+    <t>equipment</t>
+  </si>
+  <si>
+    <t>ftt</t>
+  </si>
+  <si>
+    <t>qualified tasks</t>
+  </si>
+  <si>
+    <t>equip oper</t>
+  </si>
+  <si>
+    <t>bakut oper</t>
+  </si>
+  <si>
+    <t>CLANING THE TAHAK</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CLANING THE TAHAK, bakut, equipment, ftt, marzuk, equip oper, bakut oper  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, CLANING THE TAHAK, bakut, sar poduction, ftt, marzuk, bakut oper  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bakut, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bakut, equipment, wv equipment, bakut oper, equip oper  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, bakut, equipment, sar poduction, wv equipment, equip oper, bakut oper  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, bakut, equipment, sar poduction, equip oper, bakut oper  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sar poduction  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, equip oper, sar poduction, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, bakut, sar poduction  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, bakut, sar poduction, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bakut, wv equipment, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, bakut, equipment, sar poduction, wv equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, sar poduction  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> equip oper, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, sar poduction, equip oper, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bakut  </t>
   </si>
 </sst>
 </file>
@@ -869,20 +944,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="3" width="26.21875" customWidth="1"/>
-    <col min="4" max="4" width="52.109375" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="79.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -901,8 +981,11 @@
       <c r="F1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -921,8 +1004,11 @@
       <c r="F2">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -941,8 +1027,11 @@
       <c r="F3">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -961,8 +1050,11 @@
       <c r="F4">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -981,8 +1073,11 @@
       <c r="F5">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1001,8 +1096,11 @@
       <c r="F6">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1021,8 +1119,11 @@
       <c r="F7">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1041,8 +1142,11 @@
       <c r="F8">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1061,8 +1165,11 @@
       <c r="F9">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1081,8 +1188,11 @@
       <c r="F10">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1101,8 +1211,11 @@
       <c r="F11">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1121,8 +1234,11 @@
       <c r="F12">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1141,8 +1257,11 @@
       <c r="F13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1161,8 +1280,11 @@
       <c r="F14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1181,8 +1303,11 @@
       <c r="F15">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1201,8 +1326,11 @@
       <c r="F16">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1221,8 +1349,11 @@
       <c r="F17">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1241,8 +1372,11 @@
       <c r="F18">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1261,8 +1395,11 @@
       <c r="F19">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1281,8 +1418,11 @@
       <c r="F20">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1301,8 +1441,11 @@
       <c r="F21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1321,8 +1464,11 @@
       <c r="F22">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1341,8 +1487,11 @@
       <c r="F23">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1361,8 +1510,11 @@
       <c r="F24">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1381,8 +1533,11 @@
       <c r="F25">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1401,8 +1556,11 @@
       <c r="F26">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1421,8 +1579,11 @@
       <c r="F27">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>29</v>
       </c>
@@ -1441,8 +1602,11 @@
       <c r="F28">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1461,8 +1625,11 @@
       <c r="F29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1481,8 +1648,11 @@
       <c r="F30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>106</v>
       </c>
@@ -1501,8 +1671,11 @@
       <c r="F31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>107</v>
       </c>
@@ -1521,8 +1694,11 @@
       <c r="F32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>108</v>
       </c>
@@ -1541,8 +1717,11 @@
       <c r="F33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>109</v>
       </c>
@@ -1561,8 +1740,11 @@
       <c r="F34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>110</v>
       </c>
@@ -1581,8 +1763,11 @@
       <c r="F35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>111</v>
       </c>
@@ -1601,8 +1786,11 @@
       <c r="F36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>112</v>
       </c>
@@ -1621,8 +1809,11 @@
       <c r="F37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>113</v>
       </c>
@@ -1641,8 +1832,11 @@
       <c r="F38">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -1661,8 +1855,11 @@
       <c r="F39">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>116</v>
       </c>
@@ -1681,8 +1878,11 @@
       <c r="F40">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>117</v>
       </c>
@@ -1701,8 +1901,11 @@
       <c r="F41">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G41" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>118</v>
       </c>
@@ -1721,8 +1924,11 @@
       <c r="F42">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G42" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>119</v>
       </c>
@@ -1741,22 +1947,26 @@
       <c r="F43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G43" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1769,9 +1979,10 @@
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1796,8 +2007,11 @@
       <c r="H1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1822,8 +2036,11 @@
       <c r="H2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1848,8 +2065,11 @@
       <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1871,8 +2091,11 @@
       <c r="H4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1894,8 +2117,11 @@
       <c r="H5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1917,8 +2143,11 @@
       <c r="H6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1940,8 +2169,11 @@
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1963,8 +2195,11 @@
       <c r="H8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1986,8 +2221,11 @@
       <c r="H9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -2012,8 +2250,11 @@
       <c r="H10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -2035,8 +2276,11 @@
       <c r="H11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -2058,8 +2302,11 @@
       <c r="H12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -2084,8 +2331,11 @@
       <c r="H13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2107,8 +2357,11 @@
       <c r="H14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -2133,8 +2386,11 @@
       <c r="H15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -2159,8 +2415,11 @@
       <c r="H16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -2185,8 +2444,11 @@
       <c r="H17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -2211,8 +2473,11 @@
       <c r="H18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -2236,6 +2501,9 @@
       </c>
       <c r="H19">
         <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Min tasks per month (#10)
* cleaned Dataframe from functions input

* added minimum per task type

* update DB

* merged with master
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Desktop\לימודים\Shibutzi\Automated-shifts-assignment\DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitza\Desktop\automated shifts assignment\Automated-shifts-assignment\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAB8A5E-FC6B-4732-9F1A-B948A59D7D64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
@@ -20,21 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="182">
   <si>
     <t>id</t>
   </si>
@@ -505,23 +497,98 @@
   </si>
   <si>
     <t>min_per_month</t>
+  </si>
+  <si>
+    <t>qualified tasks</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CLANING THE TAHAK, bakut, equipment, ftt, marzuk, equip oper, bakut oper  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, CLANING THE TAHAK, bakut, sar poduction, ftt, marzuk, bakut oper  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bakut, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bakut, equipment, wv equipment, bakut oper, equip oper  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, bakut, equipment, sar poduction, wv equipment, equip oper, bakut oper  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, bakut, equipment, sar poduction, equip oper, bakut oper  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sar poduction  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, equip oper, sar poduction, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, bakut, sar poduction  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, bakut, sar poduction, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bakut, wv equipment, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, bakut, equipment, sar poduction, wv equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, sar poduction  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> equip oper, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, sar poduction, equip oper, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bakut  </t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>bakut</t>
+  </si>
+  <si>
+    <t>equipment</t>
+  </si>
+  <si>
+    <t>ftt</t>
+  </si>
+  <si>
+    <t>equip oper</t>
+  </si>
+  <si>
+    <t>bakut oper</t>
+  </si>
+  <si>
+    <t>CLANING THE TAHAK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -876,21 +943,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
-    <col min="3" max="3" width="26.25" customWidth="1"/>
-    <col min="4" max="4" width="52.125" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="74" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -909,8 +980,11 @@
       <c r="F1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -929,8 +1003,11 @@
       <c r="F2">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -949,8 +1026,11 @@
       <c r="F3">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -969,8 +1049,11 @@
       <c r="F4">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -989,8 +1072,11 @@
       <c r="F5">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1009,8 +1095,11 @@
       <c r="F6">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1029,8 +1118,11 @@
       <c r="F7">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1049,8 +1141,11 @@
       <c r="F8">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1069,8 +1164,11 @@
       <c r="F9">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1089,8 +1187,11 @@
       <c r="F10">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1109,8 +1210,11 @@
       <c r="F11">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1129,8 +1233,11 @@
       <c r="F12">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1149,8 +1256,11 @@
       <c r="F13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1169,8 +1279,11 @@
       <c r="F14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1189,8 +1302,11 @@
       <c r="F15">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1209,8 +1325,11 @@
       <c r="F16">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1229,8 +1348,11 @@
       <c r="F17">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1249,8 +1371,11 @@
       <c r="F18">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1269,8 +1394,11 @@
       <c r="F19">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1289,8 +1417,11 @@
       <c r="F20">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1309,8 +1440,11 @@
       <c r="F21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1329,8 +1463,11 @@
       <c r="F22">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1349,8 +1486,11 @@
       <c r="F23">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1369,8 +1509,11 @@
       <c r="F24">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1389,8 +1532,11 @@
       <c r="F25">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1409,8 +1555,11 @@
       <c r="F26">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1429,8 +1578,11 @@
       <c r="F27">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>29</v>
       </c>
@@ -1449,8 +1601,11 @@
       <c r="F28">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1469,8 +1624,11 @@
       <c r="F29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1489,8 +1647,11 @@
       <c r="F30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>106</v>
       </c>
@@ -1509,8 +1670,11 @@
       <c r="F31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>107</v>
       </c>
@@ -1529,8 +1693,11 @@
       <c r="F32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>108</v>
       </c>
@@ -1549,8 +1716,11 @@
       <c r="F33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>109</v>
       </c>
@@ -1569,8 +1739,11 @@
       <c r="F34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>110</v>
       </c>
@@ -1589,8 +1762,11 @@
       <c r="F35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>111</v>
       </c>
@@ -1609,8 +1785,11 @@
       <c r="F36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>112</v>
       </c>
@@ -1629,8 +1808,11 @@
       <c r="F37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>113</v>
       </c>
@@ -1649,8 +1831,11 @@
       <c r="F38">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -1669,8 +1854,11 @@
       <c r="F39">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>115</v>
       </c>
@@ -1689,8 +1877,11 @@
       <c r="F40">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>116</v>
       </c>
@@ -1709,8 +1900,11 @@
       <c r="F41">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>117</v>
       </c>
@@ -1729,8 +1923,11 @@
       <c r="F42">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>118</v>
       </c>
@@ -1749,8 +1946,11 @@
       <c r="F43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
     </row>
   </sheetData>
@@ -1760,25 +1960,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1803,8 +2005,11 @@
       <c r="H1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1829,8 +2034,11 @@
       <c r="H2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1855,8 +2063,11 @@
       <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1878,8 +2089,11 @@
       <c r="H4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1901,8 +2115,11 @@
       <c r="H5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1924,8 +2141,11 @@
       <c r="H6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1947,8 +2167,11 @@
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1970,8 +2193,11 @@
       <c r="H8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1993,8 +2219,11 @@
       <c r="H9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -2019,8 +2248,11 @@
       <c r="H10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -2042,8 +2274,11 @@
       <c r="H11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -2065,8 +2300,11 @@
       <c r="H12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -2091,8 +2329,11 @@
       <c r="H13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2114,8 +2355,11 @@
       <c r="H14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -2140,8 +2384,11 @@
       <c r="H15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -2166,8 +2413,11 @@
       <c r="H16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -2192,8 +2442,11 @@
       <c r="H17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -2218,8 +2471,11 @@
       <c r="H18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -2244,8 +2500,11 @@
       <c r="H19">
         <v>0</v>
       </c>
-    </row>
-    <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="1048576" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1048576" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added colors for the tasks
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Desktop\לימודים\Shibutzi\Automated-shifts-assignment\DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noabe\Desktop\omri\auto-shifts\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830D63B6-50E0-4CDB-8B73-766F3D3EE2D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
@@ -20,21 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="221">
   <si>
     <t>id</t>
   </si>
@@ -495,22 +487,214 @@
     <t>Compatible</t>
   </si>
   <si>
+    <t>1,26,27</t>
+  </si>
+  <si>
+    <t>9,17,26,27</t>
+  </si>
+  <si>
+    <t>5,6,19,20</t>
+  </si>
+  <si>
+    <t>10,18,23</t>
+  </si>
+  <si>
+    <t>9,12,13,26,27</t>
+  </si>
+  <si>
+    <t>14,25,31</t>
+  </si>
+  <si>
+    <t>1,3,12,13,24</t>
+  </si>
+  <si>
+    <t>2,11,17,23</t>
+  </si>
+  <si>
+    <t>12,13,26,27</t>
+  </si>
+  <si>
+    <t>5,6,12,13</t>
+  </si>
+  <si>
+    <t>2,9</t>
+  </si>
+  <si>
+    <t>8,12,13,26,27</t>
+  </si>
+  <si>
+    <t>5,6,26,27</t>
+  </si>
+  <si>
+    <t>4,9,15,22,29</t>
+  </si>
+  <si>
+    <t>26,27</t>
+  </si>
+  <si>
+    <t>2,9,15,23</t>
+  </si>
+  <si>
+    <t>2,9,18,23,30</t>
+  </si>
+  <si>
+    <t>9,25</t>
+  </si>
+  <si>
+    <t>4,9,16</t>
+  </si>
+  <si>
+    <t>9,18,23,30</t>
+  </si>
+  <si>
+    <t>11,12,13</t>
+  </si>
+  <si>
+    <t>11,14,23</t>
+  </si>
+  <si>
+    <t>19,20,26,27</t>
+  </si>
+  <si>
+    <t>19,20,26,27,30</t>
+  </si>
+  <si>
+    <t>7,17,26,27</t>
+  </si>
+  <si>
+    <t>3,23,29</t>
+  </si>
+  <si>
+    <t>2,9,16,23</t>
+  </si>
+  <si>
+    <t>1,3,4,5,6,9,16,23,26,27</t>
+  </si>
+  <si>
+    <t>3,14,17</t>
+  </si>
+  <si>
+    <t>3,5,6,17,25,26,27</t>
+  </si>
+  <si>
+    <t>3,10,21,23,26,27,28</t>
+  </si>
+  <si>
+    <t>17,25</t>
+  </si>
+  <si>
+    <t>9,19,20,26,27,28</t>
+  </si>
+  <si>
+    <t>10,11,18,19,20,21,26,27</t>
+  </si>
+  <si>
+    <t>10,11,26,27,28</t>
+  </si>
+  <si>
+    <t>7,15,23</t>
+  </si>
+  <si>
+    <t>2,3,5,6,10,21,26,27</t>
+  </si>
+  <si>
+    <t>11,12,13,14,26,27</t>
+  </si>
+  <si>
+    <t>1,11</t>
+  </si>
+  <si>
+    <t>2,3,4,5,6,8,10,11,17,23,25,26,27</t>
+  </si>
+  <si>
+    <t>9,10,11,14,15,16,17,18,19,20,21,23,25,26,27,28</t>
+  </si>
+  <si>
+    <t>7,23</t>
+  </si>
+  <si>
+    <t>26,27,28</t>
+  </si>
+  <si>
+    <t>8,10,11,12,13,25,26,27</t>
+  </si>
+  <si>
+    <t>Not evening</t>
+  </si>
+  <si>
+    <t>Not task</t>
+  </si>
+  <si>
+    <t>probability</t>
+  </si>
+  <si>
+    <t>YARDIT</t>
+  </si>
+  <si>
+    <t>min_per_month</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>#F28D9F</t>
+  </si>
+  <si>
+    <t>#F24452</t>
+  </si>
+  <si>
+    <t>#F2CB05</t>
+  </si>
+  <si>
+    <t>#17BF60</t>
+  </si>
+  <si>
+    <t>#B8D9C4</t>
+  </si>
+  <si>
+    <t>#F2E205</t>
+  </si>
+  <si>
+    <t>#F24171</t>
+  </si>
+  <si>
+    <t>#EAF205</t>
+  </si>
+  <si>
+    <t>#0BD9D9</t>
+  </si>
+  <si>
+    <t>#762CBF</t>
+  </si>
+  <si>
+    <t>#7216F2</t>
+  </si>
+  <si>
+    <t>#F2EEAC</t>
+  </si>
+  <si>
+    <t>#EDC4F2</t>
+  </si>
+  <si>
+    <t>#29A7D9</t>
+  </si>
+  <si>
+    <t>#F249A6</t>
+  </si>
+  <si>
+    <t>#50F205</t>
+  </si>
+  <si>
+    <t>#D9B29C</t>
+  </si>
+  <si>
     <t>tasks available</t>
-  </si>
-  <si>
-    <t>probability</t>
-  </si>
-  <si>
-    <t>YARDIT</t>
-  </si>
-  <si>
-    <t>min_per_month</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -876,21 +1060,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
-    <col min="3" max="3" width="26.25" customWidth="1"/>
-    <col min="4" max="4" width="52.125" customWidth="1"/>
+    <col min="2" max="2" width="15.09765625" customWidth="1"/>
+    <col min="3" max="3" width="26.19921875" customWidth="1"/>
+    <col min="4" max="4" width="52.09765625" customWidth="1"/>
+    <col min="7" max="7" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -901,7 +1087,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>153</v>
+        <v>220</v>
       </c>
       <c r="E1" t="s">
         <v>147</v>
@@ -909,8 +1095,14 @@
       <c r="F1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -929,8 +1121,11 @@
       <c r="F2">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -949,8 +1144,11 @@
       <c r="F3">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -969,8 +1167,14 @@
       <c r="F4">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>169</v>
+      </c>
+      <c r="H4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -989,8 +1193,14 @@
       <c r="F5">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>171</v>
+      </c>
+      <c r="H5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1009,8 +1219,14 @@
       <c r="F6">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1029,8 +1245,14 @@
       <c r="F7">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>172</v>
+      </c>
+      <c r="H7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1049,8 +1271,14 @@
       <c r="F8">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>168</v>
+      </c>
+      <c r="H8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1069,8 +1297,14 @@
       <c r="F9">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>163</v>
+      </c>
+      <c r="H9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1089,8 +1323,14 @@
       <c r="F10">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>166</v>
+      </c>
+      <c r="H10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1109,8 +1349,14 @@
       <c r="F11">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>160</v>
+      </c>
+      <c r="H11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1129,8 +1375,14 @@
       <c r="F12">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>23</v>
+      </c>
+      <c r="H12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1149,8 +1401,14 @@
       <c r="F13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>174</v>
+      </c>
+      <c r="H13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1169,8 +1427,14 @@
       <c r="F14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>23</v>
+      </c>
+      <c r="H14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1189,8 +1453,11 @@
       <c r="F15">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1209,8 +1476,14 @@
       <c r="F16">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>158</v>
+      </c>
+      <c r="H16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1229,8 +1502,11 @@
       <c r="F17">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1249,8 +1525,14 @@
       <c r="F18">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>8</v>
+      </c>
+      <c r="H18" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1269,8 +1551,14 @@
       <c r="F19">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>163</v>
+      </c>
+      <c r="H19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1289,13 +1577,19 @@
       <c r="F20">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>178</v>
+      </c>
+      <c r="H20" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>155</v>
+        <v>200</v>
       </c>
       <c r="C21">
         <v>4</v>
@@ -1310,7 +1604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1329,8 +1623,14 @@
       <c r="F22">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <v>10</v>
+      </c>
+      <c r="H22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1349,8 +1649,14 @@
       <c r="F23">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>156</v>
+      </c>
+      <c r="H23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1369,8 +1675,11 @@
       <c r="F24">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1389,8 +1698,14 @@
       <c r="F25">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" t="s">
+        <v>184</v>
+      </c>
+      <c r="H25" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1409,8 +1724,11 @@
       <c r="F26">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1429,8 +1747,11 @@
       <c r="F27">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>29</v>
       </c>
@@ -1449,8 +1770,14 @@
       <c r="F28">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>10</v>
+      </c>
+      <c r="H28" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1469,8 +1796,14 @@
       <c r="F29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>7</v>
+      </c>
+      <c r="H29" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1489,8 +1822,14 @@
       <c r="F30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>188</v>
+      </c>
+      <c r="H30" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>106</v>
       </c>
@@ -1509,8 +1848,14 @@
       <c r="F31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>7</v>
+      </c>
+      <c r="H31" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>107</v>
       </c>
@@ -1529,8 +1874,14 @@
       <c r="F32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>194</v>
+      </c>
+      <c r="H32" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>108</v>
       </c>
@@ -1549,8 +1900,11 @@
       <c r="F33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>109</v>
       </c>
@@ -1569,8 +1923,14 @@
       <c r="F34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>7</v>
+      </c>
+      <c r="H34" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>110</v>
       </c>
@@ -1589,8 +1949,11 @@
       <c r="F35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H35" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>111</v>
       </c>
@@ -1610,7 +1973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>112</v>
       </c>
@@ -1630,7 +1993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>113</v>
       </c>
@@ -1649,8 +2012,14 @@
       <c r="F38">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>25</v>
+      </c>
+      <c r="H38" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -1670,7 +2039,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>115</v>
       </c>
@@ -1689,8 +2058,11 @@
       <c r="F40">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H40" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>116</v>
       </c>
@@ -1709,8 +2081,11 @@
       <c r="F41">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>117</v>
       </c>
@@ -1729,8 +2104,11 @@
       <c r="F42">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H42" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>118</v>
       </c>
@@ -1749,8 +2127,11 @@
       <c r="F43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H43" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
     </row>
   </sheetData>
@@ -1760,25 +2141,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21.3984375" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="28.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1798,13 +2175,16 @@
         <v>149</v>
       </c>
       <c r="G1" t="s">
-        <v>154</v>
+        <v>199</v>
       </c>
       <c r="H1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+      <c r="I1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1829,8 +2209,11 @@
       <c r="H2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1855,8 +2238,11 @@
       <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1878,8 +2264,11 @@
       <c r="H4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1901,8 +2290,11 @@
       <c r="H5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1924,8 +2316,11 @@
       <c r="H6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1947,8 +2342,11 @@
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1970,8 +2368,11 @@
       <c r="H8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1993,8 +2394,11 @@
       <c r="H9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -2019,8 +2423,11 @@
       <c r="H10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -2042,8 +2449,11 @@
       <c r="H11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -2065,8 +2475,11 @@
       <c r="H12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -2091,8 +2504,11 @@
       <c r="H13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2109,13 +2525,16 @@
         <v>1</v>
       </c>
       <c r="G14">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -2140,8 +2559,11 @@
       <c r="H15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -2166,8 +2588,11 @@
       <c r="H16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -2192,8 +2617,11 @@
       <c r="H17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I17" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -2218,8 +2646,11 @@
       <c r="H18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -2239,13 +2670,16 @@
         <v>0.25</v>
       </c>
       <c r="G19">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
-    </row>
-    <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed all holidays problems - fully working
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="276">
   <si>
     <t>id</t>
   </si>
@@ -33,9 +33,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>pazam: 1-youngest etc</t>
-  </si>
-  <si>
     <t>O1</t>
   </si>
   <si>
@@ -267,9 +264,6 @@
     <t>ADI YOGEV</t>
   </si>
   <si>
-    <t>ROTEM COHEN</t>
-  </si>
-  <si>
     <t>YONTAN LEV</t>
   </si>
   <si>
@@ -675,30 +669,12 @@
     <t>ftt</t>
   </si>
   <si>
-    <t>WV equip</t>
-  </si>
-  <si>
-    <t>EO prod</t>
-  </si>
-  <si>
-    <t>SAR prod</t>
-  </si>
-  <si>
     <t>equip_oper</t>
   </si>
   <si>
     <t>bakut_oper</t>
   </si>
   <si>
-    <t>eo_oper</t>
-  </si>
-  <si>
-    <t>sar_oper</t>
-  </si>
-  <si>
-    <t>tahak</t>
-  </si>
-  <si>
     <t>1,2,3,4,5</t>
   </si>
   <si>
@@ -790,6 +766,93 @@
   </si>
   <si>
     <t>T1, T2, T3, T4 ,T5, T6, T7, T8, T9, T14, T15, T19, T20, T21</t>
+  </si>
+  <si>
+    <t>qualified tasks</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CLANING THE TAHAK, bakut, equipment, ftt, marzuk, equip oper, bakut oper  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, CLANING THE TAHAK, bakut, sar poduction, ftt, marzuk, bakut oper  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bakut, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bakut, equipment, wv equipment, bakut oper, equip oper  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, bakut, equipment, sar poduction, wv equipment, equip oper, bakut oper  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, bakut, equipment, sar poduction, equip oper, bakut oper  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sar poduction  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, equip oper, sar poduction, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, bakut, sar poduction  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, bakut, sar poduction, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bakut, wv equipment, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, bakut, equipment, sar poduction, wv equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, sar poduction  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> equip oper, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, sar poduction, equip oper, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bakut  </t>
+  </si>
+  <si>
+    <t>pazam</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CLANING THE TAHAK, bakut, equipment, ftt, marzuk, equip oper, bakut oper , </t>
+  </si>
+  <si>
+    <t>RC</t>
+  </si>
+  <si>
+    <t>CLANING THE TAHAK</t>
+  </si>
+  <si>
+    <t>#808080</t>
+  </si>
+  <si>
+    <t>#ffed4d</t>
+  </si>
+  <si>
+    <t>#f5eca2</t>
+  </si>
+  <si>
+    <t>#b6fa9b</t>
+  </si>
+  <si>
+    <t>#4cd615</t>
+  </si>
+  <si>
+    <t>#ffb536</t>
+  </si>
+  <si>
+    <t>#ff6236</t>
   </si>
 </sst>
 </file>
@@ -852,7 +915,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -860,6 +923,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1174,22 +1239,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
-    <col min="3" max="3" width="26.25" customWidth="1"/>
+    <col min="1" max="1" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="74.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="73.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1197,36 +1266,39 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G1" t="s">
-        <v>187</v>
-      </c>
-      <c r="H1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E2">
         <v>8</v>
@@ -1235,21 +1307,24 @@
         <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E3">
         <v>8</v>
@@ -1258,21 +1333,24 @@
         <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E4">
         <v>8</v>
@@ -1281,24 +1359,27 @@
         <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="E5">
         <v>8</v>
@@ -1307,24 +1388,27 @@
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>267</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="E6">
         <v>8</v>
@@ -1333,24 +1417,28 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="E7">
         <v>8</v>
@@ -1359,24 +1447,27 @@
         <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E8">
         <v>8</v>
@@ -1385,24 +1476,27 @@
         <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E9">
         <v>8</v>
@@ -1411,24 +1505,27 @@
         <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H9" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -1437,24 +1534,27 @@
         <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H10" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E11">
         <v>6</v>
@@ -1463,24 +1563,27 @@
         <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E12">
         <v>6</v>
@@ -1492,21 +1595,24 @@
         <v>23</v>
       </c>
       <c r="H12" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="E13">
         <v>6</v>
@@ -1515,24 +1621,27 @@
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="E14">
         <v>6</v>
@@ -1544,21 +1653,24 @@
         <v>23</v>
       </c>
       <c r="H14" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E15">
         <v>4</v>
@@ -1567,21 +1679,24 @@
         <v>8</v>
       </c>
       <c r="H15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C16">
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="E16">
         <v>4.5</v>
@@ -1590,24 +1705,27 @@
         <v>8</v>
       </c>
       <c r="G16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H16" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -1616,21 +1734,24 @@
         <v>8</v>
       </c>
       <c r="H17" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C18">
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="E18">
         <v>4</v>
@@ -1642,21 +1763,24 @@
         <v>8</v>
       </c>
       <c r="H18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="E19">
         <v>4</v>
@@ -1665,24 +1789,27 @@
         <v>8</v>
       </c>
       <c r="G19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H19" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C20">
         <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="E20">
         <v>4</v>
@@ -1691,24 +1818,27 @@
         <v>8</v>
       </c>
       <c r="G20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H20" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C21">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21">
         <v>2</v>
@@ -1716,19 +1846,22 @@
       <c r="F21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="7" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -1740,21 +1873,24 @@
         <v>10</v>
       </c>
       <c r="H22" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C23">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="E23">
         <v>4</v>
@@ -1763,24 +1899,27 @@
         <v>8</v>
       </c>
       <c r="G23" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H23" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C24">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="E24">
         <v>4</v>
@@ -1789,21 +1928,24 @@
         <v>8</v>
       </c>
       <c r="H24" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C25">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="E25">
         <v>4</v>
@@ -1812,24 +1954,27 @@
         <v>8</v>
       </c>
       <c r="G25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H25" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C26">
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="E26">
         <v>4</v>
@@ -1838,21 +1983,24 @@
         <v>8</v>
       </c>
       <c r="H26" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C27">
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="E27">
         <v>4</v>
@@ -1861,21 +2009,24 @@
         <v>8</v>
       </c>
       <c r="H27" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C28">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="E28">
         <v>4</v>
@@ -1887,21 +2038,24 @@
         <v>10</v>
       </c>
       <c r="H28" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C29">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E29">
         <v>3</v>
@@ -1913,21 +2067,24 @@
         <v>7</v>
       </c>
       <c r="H29" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C30">
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E30">
         <v>2</v>
@@ -1936,24 +2093,27 @@
         <v>5</v>
       </c>
       <c r="G30" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H30" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C31">
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="E31">
         <v>4</v>
@@ -1965,21 +2125,24 @@
         <v>7</v>
       </c>
       <c r="H31" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B32" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C32">
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E32">
         <v>2</v>
@@ -1988,24 +2151,27 @@
         <v>5</v>
       </c>
       <c r="G32" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H32" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C33">
         <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E33">
         <v>2.5</v>
@@ -2014,21 +2180,24 @@
         <v>4</v>
       </c>
       <c r="H33" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B34" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C34">
         <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E34">
         <v>2.5</v>
@@ -2040,21 +2209,24 @@
         <v>7</v>
       </c>
       <c r="H34" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C35">
         <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E35">
         <v>2.5</v>
@@ -2063,21 +2235,24 @@
         <v>4</v>
       </c>
       <c r="H35" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C36">
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E36">
         <v>3</v>
@@ -2085,19 +2260,22 @@
       <c r="F36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I36" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C37">
         <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E37">
         <v>2</v>
@@ -2105,19 +2283,22 @@
       <c r="F37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37" s="7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B38" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C38">
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E38">
         <v>2</v>
@@ -2129,21 +2310,24 @@
         <v>25</v>
       </c>
       <c r="H38" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B39" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C39">
         <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -2151,19 +2335,22 @@
       <c r="F39">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I39" s="7" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B40" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C40">
         <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E40">
         <v>3</v>
@@ -2172,21 +2359,24 @@
         <v>3</v>
       </c>
       <c r="H40" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B41" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C41">
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -2197,19 +2387,22 @@
       <c r="G41">
         <v>18</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I41" s="7" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B42" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C42">
         <v>9</v>
       </c>
       <c r="D42" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E42">
         <v>2</v>
@@ -2218,21 +2411,24 @@
         <v>2</v>
       </c>
       <c r="H42" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B43" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C43">
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -2241,11 +2437,15 @@
         <v>2</v>
       </c>
       <c r="H43" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
+      <c r="I44" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2255,10 +2455,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1048576"/>
+  <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2271,10 +2471,10 @@
     <col min="6" max="6" width="4.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.75" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.625" customWidth="1"/>
-    <col min="11" max="11" width="15.875" customWidth="1"/>
+    <col min="11" max="12" width="19.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2282,39 +2482,39 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" t="s">
         <v>140</v>
       </c>
-      <c r="D1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E1" t="s">
-        <v>142</v>
-      </c>
       <c r="F1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G1" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1" t="s">
         <v>189</v>
       </c>
-      <c r="H1" t="s">
-        <v>191</v>
-      </c>
       <c r="I1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="3">
         <v>0.33333333333333331</v>
@@ -2323,7 +2523,7 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -2335,21 +2535,22 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J2" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="K2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="L2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="3">
         <v>0.33333333333333331</v>
@@ -2358,7 +2559,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -2370,21 +2571,22 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J3" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="K3" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="L3" s="8"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="3">
         <v>0.83333333333333337</v>
@@ -2402,21 +2604,22 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J4" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="K4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="L4" s="8"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="3">
         <v>0.83333333333333337</v>
@@ -2434,21 +2637,22 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J5" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="K5" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="L5" s="8"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="3">
         <v>0.33333333333333331</v>
@@ -2466,18 +2670,19 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="L6" s="8"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3">
         <v>0.83333333333333337</v>
@@ -2495,18 +2700,19 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K7" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="L7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="3">
         <v>0.33333333333333331</v>
@@ -2524,21 +2730,22 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J8" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="K8" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+      <c r="L8" s="8"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="3">
         <v>0.83333333333333337</v>
@@ -2556,21 +2763,22 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J9" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="K9" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+      <c r="L9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="3">
         <v>0.33333333333333331</v>
@@ -2579,7 +2787,7 @@
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F10">
         <v>0.5</v>
@@ -2591,21 +2799,22 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J10" t="s">
-        <v>224</v>
-      </c>
-      <c r="K10" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K10" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="3">
         <v>0.33333333333333331</v>
@@ -2623,21 +2832,22 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J11" t="s">
-        <v>224</v>
-      </c>
-      <c r="K11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="L11" s="8"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="3">
         <v>0.33333333333333331</v>
@@ -2655,21 +2865,22 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J12" t="s">
-        <v>224</v>
-      </c>
-      <c r="K12" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" s="3">
         <v>0.33333333333333331</v>
@@ -2678,7 +2889,7 @@
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F13">
         <v>0.25</v>
@@ -2690,21 +2901,22 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J13">
         <v>3</v>
       </c>
       <c r="K13" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="3">
         <v>0.33333333333333331</v>
@@ -2722,21 +2934,22 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="J14">
         <v>2</v>
       </c>
       <c r="K14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" t="s">
-        <v>61</v>
       </c>
       <c r="C15" s="3">
         <v>0.33333333333333331</v>
@@ -2745,7 +2958,7 @@
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F15">
         <v>0.25</v>
@@ -2757,21 +2970,22 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J15" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="K15" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+      <c r="L15" s="8"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" s="3">
         <v>0.33333333333333331</v>
@@ -2780,7 +2994,7 @@
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F16">
         <v>0.25</v>
@@ -2792,21 +3006,22 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J16" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="K16" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" s="3">
         <v>0.33333333333333331</v>
@@ -2815,7 +3030,7 @@
         <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F17">
         <v>0.25</v>
@@ -2827,21 +3042,22 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J17" t="s">
-        <v>224</v>
-      </c>
-      <c r="K17" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" s="3">
         <v>0.33333333333333331</v>
@@ -2850,7 +3066,7 @@
         <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F18">
         <v>0.25</v>
@@ -2862,21 +3078,22 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J18">
         <v>1</v>
       </c>
-      <c r="K18" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K18" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="5">
         <v>0.33333333333333331</v>
@@ -2885,7 +3102,7 @@
         <v>9</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F19" s="4">
         <v>0.25</v>
@@ -2897,21 +3114,22 @@
         <v>0</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="L19" s="8"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="B20" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="C20" s="3">
         <v>0.33333333333333331</v>
@@ -2920,27 +3138,30 @@
         <v>60</v>
       </c>
       <c r="F20" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G20" s="6">
         <v>1</v>
       </c>
       <c r="H20" s="6">
         <v>1</v>
+      </c>
+      <c r="I20" t="s">
+        <v>269</v>
       </c>
       <c r="J20">
         <v>6</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="B21" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C21" s="3">
         <v>0.33333333333333331</v>
@@ -2949,27 +3170,30 @@
         <v>60</v>
       </c>
       <c r="F21" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G21" s="6">
         <v>1</v>
       </c>
       <c r="H21" s="6">
         <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>270</v>
       </c>
       <c r="J21">
         <v>6</v>
       </c>
-      <c r="K21" s="6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K21" s="8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B22" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="C22" s="3">
         <v>0.33333333333333331</v>
@@ -2978,27 +3202,30 @@
         <v>60</v>
       </c>
       <c r="F22" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G22" s="6">
         <v>1</v>
       </c>
       <c r="H22" s="6">
         <v>1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>271</v>
       </c>
       <c r="J22">
         <v>6</v>
       </c>
-      <c r="K22" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K22" s="7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B23" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="C23" s="3">
         <v>0.83333333333333337</v>
@@ -3007,27 +3234,30 @@
         <v>60</v>
       </c>
       <c r="F23" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G23" s="6">
         <v>1</v>
       </c>
       <c r="H23" s="6">
         <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>272</v>
       </c>
       <c r="J23">
         <v>6</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B24" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="C24" s="3">
         <v>0.83333333333333337</v>
@@ -3036,27 +3266,30 @@
         <v>60</v>
       </c>
       <c r="F24" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G24" s="6">
         <v>1</v>
       </c>
       <c r="H24" s="6">
         <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>273</v>
       </c>
       <c r="J24">
         <v>6</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="B25" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="C25" s="3">
         <v>0.83333333333333337</v>
@@ -3065,27 +3298,30 @@
         <v>60</v>
       </c>
       <c r="F25" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G25" s="6">
         <v>1</v>
       </c>
       <c r="H25" s="6">
         <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>274</v>
       </c>
       <c r="J25">
         <v>6</v>
       </c>
-      <c r="K25" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K25" s="7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B26" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C26" s="3">
         <v>0.33333333333333331</v>
@@ -3094,20 +3330,35 @@
         <v>60</v>
       </c>
       <c r="F26" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G26" s="6">
         <v>1</v>
       </c>
       <c r="H26" s="6">
         <v>1</v>
+      </c>
+      <c r="I26" t="s">
+        <v>275</v>
       </c>
       <c r="J26">
         <v>6</v>
       </c>
-      <c r="K26" t="s">
-        <v>217</v>
-      </c>
+      <c r="K26" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E33" s="7"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E34" s="7"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E35" s="7"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E36" s="7"/>
     </row>
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C1048576" s="3"/>

</xml_diff>

<commit_message>
Added malams to the butzi excel
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="278">
   <si>
     <t>id</t>
   </si>
@@ -853,13 +853,19 @@
   </si>
   <si>
     <t>#ff6236</t>
+  </si>
+  <si>
+    <t>MAX_Sofashim</t>
+  </si>
+  <si>
+    <t>is_sofash</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -869,6 +875,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -894,7 +908,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -911,20 +925,78 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1241,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1250,12 +1322,13 @@
     <col min="1" max="1" width="4.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="74.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="40.25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="73.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="74.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -1269,7 +1342,7 @@
         <v>265</v>
       </c>
       <c r="D1" t="s">
-        <v>208</v>
+        <v>276</v>
       </c>
       <c r="E1" t="s">
         <v>135</v>
@@ -1283,8 +1356,11 @@
       <c r="H1" t="s">
         <v>186</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="5" t="s">
         <v>247</v>
+      </c>
+      <c r="J1" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1297,8 +1373,8 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>236</v>
+      <c r="D2">
+        <v>2</v>
       </c>
       <c r="E2">
         <v>8</v>
@@ -1309,8 +1385,11 @@
       <c r="H2" t="s">
         <v>155</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="5" t="s">
         <v>266</v>
+      </c>
+      <c r="J2" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1323,8 +1402,8 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
-        <v>236</v>
+      <c r="D3">
+        <v>2</v>
       </c>
       <c r="E3">
         <v>8</v>
@@ -1335,8 +1414,11 @@
       <c r="H3" t="s">
         <v>152</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="5" t="s">
         <v>248</v>
+      </c>
+      <c r="J3" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1349,8 +1431,8 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
-        <v>236</v>
+      <c r="D4">
+        <v>2</v>
       </c>
       <c r="E4">
         <v>8</v>
@@ -1364,8 +1446,11 @@
       <c r="H4" t="s">
         <v>143</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="5" t="s">
         <v>248</v>
+      </c>
+      <c r="J4" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1378,8 +1463,8 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
-        <v>237</v>
+      <c r="D5">
+        <v>2</v>
       </c>
       <c r="E5">
         <v>8</v>
@@ -1393,8 +1478,11 @@
       <c r="H5" t="s">
         <v>153</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="5" t="s">
         <v>249</v>
+      </c>
+      <c r="J5" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1407,8 +1495,8 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
-        <v>233</v>
+      <c r="D6">
+        <v>2</v>
       </c>
       <c r="E6">
         <v>8</v>
@@ -1422,10 +1510,13 @@
       <c r="H6" t="s">
         <v>155</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="L6" s="7"/>
+      <c r="J6" t="s">
+        <v>233</v>
+      </c>
+      <c r="L6" s="5"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1437,8 +1528,8 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
-        <v>234</v>
+      <c r="D7">
+        <v>2</v>
       </c>
       <c r="E7">
         <v>8</v>
@@ -1452,8 +1543,11 @@
       <c r="H7" t="s">
         <v>143</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="5" t="s">
         <v>249</v>
+      </c>
+      <c r="J7" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -1466,8 +1560,8 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
-        <v>236</v>
+      <c r="D8">
+        <v>2</v>
       </c>
       <c r="E8">
         <v>8</v>
@@ -1481,8 +1575,11 @@
       <c r="H8" t="s">
         <v>155</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="5" t="s">
         <v>248</v>
+      </c>
+      <c r="J8" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -1495,8 +1592,8 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
-        <v>236</v>
+      <c r="D9">
+        <v>2</v>
       </c>
       <c r="E9">
         <v>8</v>
@@ -1510,8 +1607,11 @@
       <c r="H9" t="s">
         <v>150</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="5" t="s">
         <v>248</v>
+      </c>
+      <c r="J9" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1524,8 +1624,8 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
-        <v>236</v>
+      <c r="D10">
+        <v>2</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -1539,8 +1639,11 @@
       <c r="H10" t="s">
         <v>153</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="5" t="s">
         <v>248</v>
+      </c>
+      <c r="J10" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -1553,8 +1656,8 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11" t="s">
-        <v>236</v>
+      <c r="D11">
+        <v>2</v>
       </c>
       <c r="E11">
         <v>6</v>
@@ -1568,8 +1671,11 @@
       <c r="H11" t="s">
         <v>147</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="5" t="s">
         <v>248</v>
+      </c>
+      <c r="J11" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1582,8 +1688,8 @@
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="D12" t="s">
-        <v>236</v>
+      <c r="D12">
+        <v>2</v>
       </c>
       <c r="E12">
         <v>6</v>
@@ -1597,8 +1703,11 @@
       <c r="H12" t="s">
         <v>149</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="5" t="s">
         <v>248</v>
+      </c>
+      <c r="J12" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1611,8 +1720,8 @@
       <c r="C13">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
-        <v>233</v>
+      <c r="D13">
+        <v>2</v>
       </c>
       <c r="E13">
         <v>6</v>
@@ -1626,8 +1735,11 @@
       <c r="H13" t="s">
         <v>153</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="I13" s="5" t="s">
         <v>249</v>
+      </c>
+      <c r="J13" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1640,8 +1752,8 @@
       <c r="C14">
         <v>2</v>
       </c>
-      <c r="D14" t="s">
-        <v>238</v>
+      <c r="D14">
+        <v>2</v>
       </c>
       <c r="E14">
         <v>6</v>
@@ -1655,8 +1767,11 @@
       <c r="H14" t="s">
         <v>183</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="5" t="s">
         <v>250</v>
+      </c>
+      <c r="J14" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1669,8 +1784,8 @@
       <c r="C15">
         <v>3</v>
       </c>
-      <c r="D15" t="s">
-        <v>239</v>
+      <c r="D15">
+        <v>1</v>
       </c>
       <c r="E15">
         <v>4</v>
@@ -1681,8 +1796,11 @@
       <c r="H15" t="s">
         <v>161</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="5" t="s">
         <v>251</v>
+      </c>
+      <c r="J15" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1695,8 +1813,8 @@
       <c r="C16">
         <v>3</v>
       </c>
-      <c r="D16" t="s">
-        <v>232</v>
+      <c r="D16">
+        <v>1</v>
       </c>
       <c r="E16">
         <v>4.5</v>
@@ -1710,11 +1828,14 @@
       <c r="H16" t="s">
         <v>145</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="I16" s="5" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1724,8 +1845,8 @@
       <c r="C17">
         <v>3</v>
       </c>
-      <c r="D17" t="s">
-        <v>231</v>
+      <c r="D17">
+        <v>1</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -1736,11 +1857,14 @@
       <c r="H17" t="s">
         <v>180</v>
       </c>
-      <c r="I17" s="7" t="s">
+      <c r="I17" s="5" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1750,8 +1874,8 @@
       <c r="C18">
         <v>3</v>
       </c>
-      <c r="D18" t="s">
-        <v>231</v>
+      <c r="D18">
+        <v>1</v>
       </c>
       <c r="E18">
         <v>4</v>
@@ -1765,11 +1889,14 @@
       <c r="H18" t="s">
         <v>181</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="I18" s="5" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1779,8 +1906,8 @@
       <c r="C19">
         <v>3</v>
       </c>
-      <c r="D19" t="s">
-        <v>240</v>
+      <c r="D19">
+        <v>1</v>
       </c>
       <c r="E19">
         <v>4</v>
@@ -1794,11 +1921,14 @@
       <c r="H19" t="s">
         <v>178</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="I19" s="5" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1808,8 +1938,8 @@
       <c r="C20">
         <v>3</v>
       </c>
-      <c r="D20" t="s">
-        <v>241</v>
+      <c r="D20">
+        <v>1</v>
       </c>
       <c r="E20">
         <v>4</v>
@@ -1823,11 +1953,14 @@
       <c r="H20" t="s">
         <v>165</v>
       </c>
-      <c r="I20" s="7" t="s">
+      <c r="I20" s="5" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -1837,8 +1970,8 @@
       <c r="C21">
         <v>4</v>
       </c>
-      <c r="D21" t="s">
-        <v>41</v>
+      <c r="D21">
+        <v>0</v>
       </c>
       <c r="E21">
         <v>2</v>
@@ -1846,11 +1979,14 @@
       <c r="F21">
         <v>2</v>
       </c>
-      <c r="I21" s="7" t="s">
+      <c r="I21" s="5" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1860,8 +1996,8 @@
       <c r="C22">
         <v>4</v>
       </c>
-      <c r="D22" t="s">
-        <v>243</v>
+      <c r="D22">
+        <v>1</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -1875,11 +2011,14 @@
       <c r="H22" t="s">
         <v>142</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="I22" s="5" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1889,8 +2028,8 @@
       <c r="C23">
         <v>4</v>
       </c>
-      <c r="D23" t="s">
-        <v>244</v>
+      <c r="D23">
+        <v>1</v>
       </c>
       <c r="E23">
         <v>4</v>
@@ -1904,11 +2043,14 @@
       <c r="H23" t="s">
         <v>143</v>
       </c>
-      <c r="I23" s="7" t="s">
+      <c r="I23" s="5" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1918,8 +2060,8 @@
       <c r="C24">
         <v>4</v>
       </c>
-      <c r="D24" t="s">
-        <v>245</v>
+      <c r="D24">
+        <v>1</v>
       </c>
       <c r="E24">
         <v>4</v>
@@ -1930,11 +2072,14 @@
       <c r="H24" t="s">
         <v>177</v>
       </c>
-      <c r="I24" s="7" t="s">
+      <c r="I24" s="5" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1944,8 +2089,8 @@
       <c r="C25">
         <v>4</v>
       </c>
-      <c r="D25" t="s">
-        <v>245</v>
+      <c r="D25">
+        <v>1</v>
       </c>
       <c r="E25">
         <v>4</v>
@@ -1959,11 +2104,14 @@
       <c r="H25" t="s">
         <v>171</v>
       </c>
-      <c r="I25" s="7" t="s">
+      <c r="I25" s="5" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1973,8 +2121,8 @@
       <c r="C26">
         <v>4</v>
       </c>
-      <c r="D26" t="s">
-        <v>242</v>
+      <c r="D26">
+        <v>1</v>
       </c>
       <c r="E26">
         <v>4</v>
@@ -1985,11 +2133,14 @@
       <c r="H26" t="s">
         <v>184</v>
       </c>
-      <c r="I26" s="7" t="s">
+      <c r="I26" s="5" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1999,8 +2150,8 @@
       <c r="C27">
         <v>4</v>
       </c>
-      <c r="D27" t="s">
-        <v>245</v>
+      <c r="D27">
+        <v>1</v>
       </c>
       <c r="E27">
         <v>4</v>
@@ -2011,11 +2162,14 @@
       <c r="H27" t="s">
         <v>164</v>
       </c>
-      <c r="I27" s="7" t="s">
+      <c r="I27" s="5" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
@@ -2025,8 +2179,8 @@
       <c r="C28">
         <v>4</v>
       </c>
-      <c r="D28" t="s">
-        <v>246</v>
+      <c r="D28">
+        <v>1</v>
       </c>
       <c r="E28">
         <v>4</v>
@@ -2040,11 +2194,14 @@
       <c r="H28" t="s">
         <v>163</v>
       </c>
-      <c r="I28" s="7" t="s">
+      <c r="I28" s="5" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2054,8 +2211,8 @@
       <c r="C29">
         <v>5</v>
       </c>
-      <c r="D29" t="s">
-        <v>126</v>
+      <c r="D29">
+        <v>0</v>
       </c>
       <c r="E29">
         <v>3</v>
@@ -2069,11 +2226,14 @@
       <c r="H29" t="s">
         <v>170</v>
       </c>
-      <c r="I29" s="7" t="s">
+      <c r="I29" s="5" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2083,8 +2243,8 @@
       <c r="C30">
         <v>5</v>
       </c>
-      <c r="D30" t="s">
-        <v>124</v>
+      <c r="D30">
+        <v>0</v>
       </c>
       <c r="E30">
         <v>2</v>
@@ -2098,11 +2258,14 @@
       <c r="H30" t="s">
         <v>175</v>
       </c>
-      <c r="I30" s="7" t="s">
+      <c r="I30" s="5" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>104</v>
       </c>
@@ -2112,8 +2275,8 @@
       <c r="C31">
         <v>5</v>
       </c>
-      <c r="D31" t="s">
-        <v>235</v>
+      <c r="D31">
+        <v>0</v>
       </c>
       <c r="E31">
         <v>4</v>
@@ -2127,11 +2290,14 @@
       <c r="H31" t="s">
         <v>174</v>
       </c>
-      <c r="I31" s="7" t="s">
+      <c r="I31" s="5" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J31" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>105</v>
       </c>
@@ -2141,8 +2307,8 @@
       <c r="C32">
         <v>5</v>
       </c>
-      <c r="D32" t="s">
-        <v>127</v>
+      <c r="D32">
+        <v>0</v>
       </c>
       <c r="E32">
         <v>2</v>
@@ -2156,11 +2322,14 @@
       <c r="H32" t="s">
         <v>175</v>
       </c>
-      <c r="I32" s="7" t="s">
+      <c r="I32" s="5" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>106</v>
       </c>
@@ -2170,8 +2339,8 @@
       <c r="C33">
         <v>6</v>
       </c>
-      <c r="D33" t="s">
-        <v>125</v>
+      <c r="D33">
+        <v>0</v>
       </c>
       <c r="E33">
         <v>2.5</v>
@@ -2182,11 +2351,14 @@
       <c r="H33" t="s">
         <v>141</v>
       </c>
-      <c r="I33" s="7" t="s">
+      <c r="I33" s="5" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>107</v>
       </c>
@@ -2196,8 +2368,8 @@
       <c r="C34">
         <v>6</v>
       </c>
-      <c r="D34" t="s">
-        <v>128</v>
+      <c r="D34">
+        <v>0</v>
       </c>
       <c r="E34">
         <v>2.5</v>
@@ -2211,11 +2383,14 @@
       <c r="H34" t="s">
         <v>169</v>
       </c>
-      <c r="I34" s="7" t="s">
+      <c r="I34" s="5" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J34" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>108</v>
       </c>
@@ -2225,8 +2400,8 @@
       <c r="C35">
         <v>6</v>
       </c>
-      <c r="D35" t="s">
-        <v>128</v>
+      <c r="D35">
+        <v>0</v>
       </c>
       <c r="E35">
         <v>2.5</v>
@@ -2237,11 +2412,14 @@
       <c r="H35" t="s">
         <v>168</v>
       </c>
-      <c r="I35" s="7" t="s">
+      <c r="I35" s="5" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J35" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>109</v>
       </c>
@@ -2251,8 +2429,8 @@
       <c r="C36">
         <v>6</v>
       </c>
-      <c r="D36" t="s">
-        <v>129</v>
+      <c r="D36">
+        <v>0</v>
       </c>
       <c r="E36">
         <v>3</v>
@@ -2260,11 +2438,14 @@
       <c r="F36">
         <v>4</v>
       </c>
-      <c r="I36" s="7" t="s">
+      <c r="I36" s="5" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J36" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>110</v>
       </c>
@@ -2274,8 +2455,8 @@
       <c r="C37">
         <v>6</v>
       </c>
-      <c r="D37" t="s">
-        <v>130</v>
+      <c r="D37">
+        <v>0</v>
       </c>
       <c r="E37">
         <v>2</v>
@@ -2283,11 +2464,14 @@
       <c r="F37">
         <v>2</v>
       </c>
-      <c r="I37" s="7" t="s">
+      <c r="I37" s="5" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J37" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>111</v>
       </c>
@@ -2297,8 +2481,8 @@
       <c r="C38">
         <v>7</v>
       </c>
-      <c r="D38" t="s">
-        <v>131</v>
+      <c r="D38">
+        <v>0</v>
       </c>
       <c r="E38">
         <v>2</v>
@@ -2312,11 +2496,14 @@
       <c r="H38" t="s">
         <v>173</v>
       </c>
-      <c r="I38" s="7" t="s">
+      <c r="I38" s="5" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J38" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>112</v>
       </c>
@@ -2326,8 +2513,8 @@
       <c r="C39">
         <v>8</v>
       </c>
-      <c r="D39" t="s">
-        <v>132</v>
+      <c r="D39">
+        <v>0</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -2335,11 +2522,14 @@
       <c r="F39">
         <v>3</v>
       </c>
-      <c r="I39" s="7" t="s">
+      <c r="I39" s="5" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>113</v>
       </c>
@@ -2349,8 +2539,8 @@
       <c r="C40">
         <v>8</v>
       </c>
-      <c r="D40" t="s">
-        <v>133</v>
+      <c r="D40">
+        <v>0</v>
       </c>
       <c r="E40">
         <v>3</v>
@@ -2361,11 +2551,14 @@
       <c r="H40" t="s">
         <v>183</v>
       </c>
-      <c r="I40" s="7" t="s">
+      <c r="I40" s="5" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J40" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>114</v>
       </c>
@@ -2375,8 +2568,8 @@
       <c r="C41">
         <v>8</v>
       </c>
-      <c r="D41" t="s">
-        <v>132</v>
+      <c r="D41">
+        <v>0</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -2387,11 +2580,14 @@
       <c r="G41">
         <v>18</v>
       </c>
-      <c r="I41" s="7" t="s">
+      <c r="I41" s="5" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J41" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>115</v>
       </c>
@@ -2401,8 +2597,8 @@
       <c r="C42">
         <v>9</v>
       </c>
-      <c r="D42" t="s">
-        <v>130</v>
+      <c r="D42">
+        <v>0</v>
       </c>
       <c r="E42">
         <v>2</v>
@@ -2413,11 +2609,14 @@
       <c r="H42" t="s">
         <v>179</v>
       </c>
-      <c r="I42" s="7" t="s">
+      <c r="I42" s="5" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J42" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>116</v>
       </c>
@@ -2427,8 +2626,8 @@
       <c r="C43">
         <v>9</v>
       </c>
-      <c r="D43" t="s">
-        <v>134</v>
+      <c r="D43">
+        <v>0</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -2439,17 +2638,21 @@
       <c r="H43" t="s">
         <v>167</v>
       </c>
-      <c r="I43" s="7" t="s">
+      <c r="I43" s="5" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J43" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
-      <c r="I44" s="7"/>
+      <c r="I44" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2457,8 +2660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2474,43 +2677,46 @@
     <col min="11" max="12" width="19.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:12" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="7" t="s">
         <v>210</v>
       </c>
+      <c r="L1" s="9" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="10" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
@@ -2543,10 +2749,12 @@
       <c r="K2" t="s">
         <v>211</v>
       </c>
-      <c r="L2" s="8"/>
+      <c r="L2" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B3" t="s">
@@ -2579,10 +2787,12 @@
       <c r="K3" t="s">
         <v>211</v>
       </c>
-      <c r="L3" s="8"/>
+      <c r="L3" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="11" t="s">
         <v>33</v>
       </c>
       <c r="B4" t="s">
@@ -2612,10 +2822,12 @@
       <c r="K4" t="s">
         <v>211</v>
       </c>
-      <c r="L4" s="8"/>
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="11" t="s">
         <v>34</v>
       </c>
       <c r="B5" t="s">
@@ -2645,10 +2857,12 @@
       <c r="K5" t="s">
         <v>211</v>
       </c>
-      <c r="L5" s="8"/>
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B6" t="s">
@@ -2675,10 +2889,12 @@
       <c r="K6" t="s">
         <v>211</v>
       </c>
-      <c r="L6" s="8"/>
+      <c r="L6" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B7" t="s">
@@ -2705,10 +2921,12 @@
       <c r="K7" t="s">
         <v>211</v>
       </c>
-      <c r="L7" s="8"/>
+      <c r="L7" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B8" t="s">
@@ -2738,10 +2956,12 @@
       <c r="K8" t="s">
         <v>212</v>
       </c>
-      <c r="L8" s="8"/>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="11" t="s">
         <v>38</v>
       </c>
       <c r="B9" t="s">
@@ -2771,10 +2991,12 @@
       <c r="K9" t="s">
         <v>212</v>
       </c>
-      <c r="L9" s="8"/>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B10" t="s">
@@ -2804,13 +3026,15 @@
       <c r="J10" t="s">
         <v>216</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="L10" s="8"/>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B11" t="s">
@@ -2837,13 +3061,15 @@
       <c r="J11" t="s">
         <v>216</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="L11" s="8"/>
+      <c r="L11" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B12" t="s">
@@ -2870,13 +3096,15 @@
       <c r="J12" t="s">
         <v>216</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="L12" s="8"/>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B13" t="s">
@@ -2909,10 +3137,12 @@
       <c r="K13" t="s">
         <v>213</v>
       </c>
-      <c r="L13" s="8"/>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="11" t="s">
         <v>43</v>
       </c>
       <c r="B14" t="s">
@@ -2942,10 +3172,12 @@
       <c r="K14" t="s">
         <v>59</v>
       </c>
-      <c r="L14" s="8"/>
+      <c r="L14" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B15" t="s">
@@ -2978,10 +3210,12 @@
       <c r="K15" t="s">
         <v>214</v>
       </c>
-      <c r="L15" s="8"/>
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B16" t="s">
@@ -3014,10 +3248,12 @@
       <c r="K16" t="s">
         <v>215</v>
       </c>
-      <c r="L16" s="8"/>
+      <c r="L16" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="11" t="s">
         <v>46</v>
       </c>
       <c r="B17" t="s">
@@ -3047,13 +3283,15 @@
       <c r="J17" t="s">
         <v>216</v>
       </c>
-      <c r="K17" s="8" t="s">
+      <c r="K17" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="L17" s="8"/>
+      <c r="L17" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="11" t="s">
         <v>47</v>
       </c>
       <c r="B18" t="s">
@@ -3083,49 +3321,53 @@
       <c r="J18">
         <v>1</v>
       </c>
-      <c r="K18" s="8" t="s">
+      <c r="K18" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="L18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="15">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="13">
         <v>9</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="13">
         <v>0.25</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="13">
         <v>0.4</v>
       </c>
-      <c r="H19" s="4">
-        <v>0</v>
-      </c>
-      <c r="I19" s="4" t="s">
+      <c r="H19" s="13">
+        <v>0</v>
+      </c>
+      <c r="I19" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="K19" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="L19" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
         <v>217</v>
       </c>
       <c r="B20" t="s">
@@ -3134,16 +3376,16 @@
       <c r="C20" s="3">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="4">
         <v>60</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="4">
         <v>2</v>
       </c>
-      <c r="G20" s="6">
-        <v>1</v>
-      </c>
-      <c r="H20" s="6">
+      <c r="G20" s="4">
+        <v>1</v>
+      </c>
+      <c r="H20" s="4">
         <v>1</v>
       </c>
       <c r="I20" t="s">
@@ -3152,12 +3394,15 @@
       <c r="J20">
         <v>6</v>
       </c>
-      <c r="K20" s="6" t="s">
+      <c r="K20" s="4" t="s">
         <v>211</v>
       </c>
+      <c r="L20" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="11" t="s">
         <v>220</v>
       </c>
       <c r="B21" t="s">
@@ -3166,16 +3411,16 @@
       <c r="C21" s="3">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="4">
         <v>60</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="4">
         <v>2</v>
       </c>
-      <c r="G21" s="6">
-        <v>1</v>
-      </c>
-      <c r="H21" s="6">
+      <c r="G21" s="4">
+        <v>1</v>
+      </c>
+      <c r="H21" s="4">
         <v>1</v>
       </c>
       <c r="I21" t="s">
@@ -3184,12 +3429,15 @@
       <c r="J21">
         <v>6</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="K21" s="6" t="s">
         <v>211</v>
       </c>
+      <c r="L21" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="11" t="s">
         <v>221</v>
       </c>
       <c r="B22" t="s">
@@ -3198,16 +3446,16 @@
       <c r="C22" s="3">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="4">
         <v>60</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="4">
         <v>2</v>
       </c>
-      <c r="G22" s="6">
-        <v>1</v>
-      </c>
-      <c r="H22" s="6">
+      <c r="G22" s="4">
+        <v>1</v>
+      </c>
+      <c r="H22" s="4">
         <v>1</v>
       </c>
       <c r="I22" t="s">
@@ -3216,12 +3464,15 @@
       <c r="J22">
         <v>6</v>
       </c>
-      <c r="K22" s="7" t="s">
+      <c r="K22" s="5" t="s">
         <v>212</v>
       </c>
+      <c r="L22" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="11" t="s">
         <v>222</v>
       </c>
       <c r="B23" t="s">
@@ -3230,16 +3481,16 @@
       <c r="C23" s="3">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="4">
         <v>60</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="4">
         <v>4</v>
       </c>
-      <c r="G23" s="6">
-        <v>1</v>
-      </c>
-      <c r="H23" s="6">
+      <c r="G23" s="4">
+        <v>1</v>
+      </c>
+      <c r="H23" s="4">
         <v>1</v>
       </c>
       <c r="I23" t="s">
@@ -3248,12 +3499,15 @@
       <c r="J23">
         <v>6</v>
       </c>
-      <c r="K23" s="6" t="s">
+      <c r="K23" s="4" t="s">
         <v>211</v>
       </c>
+      <c r="L23" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="11" t="s">
         <v>226</v>
       </c>
       <c r="B24" t="s">
@@ -3262,16 +3516,16 @@
       <c r="C24" s="3">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="4">
         <v>60</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="4">
         <v>4</v>
       </c>
-      <c r="G24" s="6">
-        <v>1</v>
-      </c>
-      <c r="H24" s="6">
+      <c r="G24" s="4">
+        <v>1</v>
+      </c>
+      <c r="H24" s="4">
         <v>1</v>
       </c>
       <c r="I24" t="s">
@@ -3280,12 +3534,15 @@
       <c r="J24">
         <v>6</v>
       </c>
-      <c r="K24" s="6" t="s">
+      <c r="K24" s="4" t="s">
         <v>211</v>
       </c>
+      <c r="L24" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="11" t="s">
         <v>227</v>
       </c>
       <c r="B25" t="s">
@@ -3294,16 +3551,16 @@
       <c r="C25" s="3">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="4">
         <v>60</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="4">
         <v>4</v>
       </c>
-      <c r="G25" s="6">
-        <v>1</v>
-      </c>
-      <c r="H25" s="6">
+      <c r="G25" s="4">
+        <v>1</v>
+      </c>
+      <c r="H25" s="4">
         <v>1</v>
       </c>
       <c r="I25" t="s">
@@ -3312,12 +3569,15 @@
       <c r="J25">
         <v>6</v>
       </c>
-      <c r="K25" s="7" t="s">
+      <c r="K25" s="5" t="s">
         <v>212</v>
       </c>
+      <c r="L25" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="A26" s="11" t="s">
         <v>229</v>
       </c>
       <c r="B26" t="s">
@@ -3326,16 +3586,16 @@
       <c r="C26" s="3">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="4">
         <v>60</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="4">
         <v>2</v>
       </c>
-      <c r="G26" s="6">
-        <v>1</v>
-      </c>
-      <c r="H26" s="6">
+      <c r="G26" s="4">
+        <v>1</v>
+      </c>
+      <c r="H26" s="4">
         <v>1</v>
       </c>
       <c r="I26" t="s">
@@ -3344,21 +3604,24 @@
       <c r="J26">
         <v>6</v>
       </c>
-      <c r="K26" s="8" t="s">
+      <c r="K26" s="6" t="s">
         <v>62</v>
       </c>
+      <c r="L26" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E33" s="7"/>
+      <c r="E33" s="5"/>
     </row>
     <row r="34" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E34" s="7"/>
+      <c r="E34" s="5"/>
     </row>
     <row r="35" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E35" s="7"/>
+      <c r="E35" s="5"/>
     </row>
     <row r="36" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E36" s="7"/>
+      <c r="E36" s="5"/>
     </row>
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C1048576" s="3"/>

</xml_diff>

<commit_message>
Add weekend capacity limit
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Desktop\לימודים\Shibutzi\Automated-shifts-assignment\DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omri3\Documents\Projects\Automated-shifts-assignment\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4947A3-4A26-4EAD-8A8C-669DD18973D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
     <sheet name="Tasks" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Operators!$A$1:$L$44</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -864,18 +868,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -883,7 +887,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1310,28 +1314,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="73.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="74.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.3671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.62890625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.3671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.89453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.47265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.89453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.26171875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="73.3671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="74.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1363,7 +1367,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1374,7 +1378,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="E2">
         <v>8</v>
@@ -1392,7 +1396,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1402,8 +1406,8 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3">
-        <v>2</v>
+      <c r="D3" s="6">
+        <v>200</v>
       </c>
       <c r="E3">
         <v>8</v>
@@ -1421,7 +1425,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1431,8 +1435,8 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4">
-        <v>2</v>
+      <c r="D4" s="6">
+        <v>200</v>
       </c>
       <c r="E4">
         <v>8</v>
@@ -1453,7 +1457,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1463,8 +1467,8 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5">
-        <v>2</v>
+      <c r="D5" s="6">
+        <v>200</v>
       </c>
       <c r="E5">
         <v>8</v>
@@ -1485,7 +1489,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1495,8 +1499,8 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6">
-        <v>2</v>
+      <c r="D6" s="6">
+        <v>200</v>
       </c>
       <c r="E6">
         <v>8</v>
@@ -1518,7 +1522,7 @@
       </c>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1528,8 +1532,8 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7">
-        <v>2</v>
+      <c r="D7" s="6">
+        <v>200</v>
       </c>
       <c r="E7">
         <v>8</v>
@@ -1550,7 +1554,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1560,8 +1564,8 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8">
-        <v>2</v>
+      <c r="D8" s="6">
+        <v>200</v>
       </c>
       <c r="E8">
         <v>8</v>
@@ -1582,7 +1586,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1592,8 +1596,8 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9">
-        <v>2</v>
+      <c r="D9" s="6">
+        <v>200</v>
       </c>
       <c r="E9">
         <v>8</v>
@@ -1614,7 +1618,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1624,8 +1628,8 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10">
-        <v>2</v>
+      <c r="D10" s="6">
+        <v>200</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -1646,7 +1650,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1656,8 +1660,8 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11">
-        <v>2</v>
+      <c r="D11" s="6">
+        <v>200</v>
       </c>
       <c r="E11">
         <v>6</v>
@@ -1678,7 +1682,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1688,8 +1692,8 @@
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="D12">
-        <v>2</v>
+      <c r="D12" s="6">
+        <v>200</v>
       </c>
       <c r="E12">
         <v>6</v>
@@ -1710,7 +1714,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1720,8 +1724,8 @@
       <c r="C13">
         <v>2</v>
       </c>
-      <c r="D13">
-        <v>2</v>
+      <c r="D13" s="6">
+        <v>200</v>
       </c>
       <c r="E13">
         <v>6</v>
@@ -1742,7 +1746,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1752,8 +1756,8 @@
       <c r="C14">
         <v>2</v>
       </c>
-      <c r="D14">
-        <v>2</v>
+      <c r="D14" s="6">
+        <v>200</v>
       </c>
       <c r="E14">
         <v>6</v>
@@ -1774,7 +1778,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1785,7 +1789,7 @@
         <v>3</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E15">
         <v>4</v>
@@ -1803,7 +1807,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1813,8 +1817,8 @@
       <c r="C16">
         <v>3</v>
       </c>
-      <c r="D16">
-        <v>1</v>
+      <c r="D16" s="6">
+        <v>100</v>
       </c>
       <c r="E16">
         <v>4.5</v>
@@ -1835,7 +1839,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1845,8 +1849,8 @@
       <c r="C17">
         <v>3</v>
       </c>
-      <c r="D17">
-        <v>1</v>
+      <c r="D17" s="6">
+        <v>100</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -1864,7 +1868,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1874,8 +1878,8 @@
       <c r="C18">
         <v>3</v>
       </c>
-      <c r="D18">
-        <v>1</v>
+      <c r="D18" s="6">
+        <v>100</v>
       </c>
       <c r="E18">
         <v>4</v>
@@ -1896,7 +1900,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1906,8 +1910,8 @@
       <c r="C19">
         <v>3</v>
       </c>
-      <c r="D19">
-        <v>1</v>
+      <c r="D19" s="6">
+        <v>100</v>
       </c>
       <c r="E19">
         <v>4</v>
@@ -1928,7 +1932,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1938,8 +1942,8 @@
       <c r="C20">
         <v>3</v>
       </c>
-      <c r="D20">
-        <v>1</v>
+      <c r="D20" s="6">
+        <v>100</v>
       </c>
       <c r="E20">
         <v>4</v>
@@ -1960,7 +1964,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -1970,7 +1974,7 @@
       <c r="C21">
         <v>4</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="6">
         <v>0</v>
       </c>
       <c r="E21">
@@ -1986,7 +1990,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1996,8 +2000,8 @@
       <c r="C22">
         <v>4</v>
       </c>
-      <c r="D22">
-        <v>1</v>
+      <c r="D22" s="6">
+        <v>100</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -2018,7 +2022,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2028,8 +2032,8 @@
       <c r="C23">
         <v>4</v>
       </c>
-      <c r="D23">
-        <v>1</v>
+      <c r="D23" s="6">
+        <v>100</v>
       </c>
       <c r="E23">
         <v>4</v>
@@ -2050,7 +2054,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2060,8 +2064,8 @@
       <c r="C24">
         <v>4</v>
       </c>
-      <c r="D24">
-        <v>1</v>
+      <c r="D24" s="6">
+        <v>100</v>
       </c>
       <c r="E24">
         <v>4</v>
@@ -2079,7 +2083,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2089,8 +2093,8 @@
       <c r="C25">
         <v>4</v>
       </c>
-      <c r="D25">
-        <v>1</v>
+      <c r="D25" s="6">
+        <v>100</v>
       </c>
       <c r="E25">
         <v>4</v>
@@ -2111,7 +2115,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2121,8 +2125,8 @@
       <c r="C26">
         <v>4</v>
       </c>
-      <c r="D26">
-        <v>1</v>
+      <c r="D26" s="6">
+        <v>100</v>
       </c>
       <c r="E26">
         <v>4</v>
@@ -2140,7 +2144,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2150,8 +2154,8 @@
       <c r="C27">
         <v>4</v>
       </c>
-      <c r="D27">
-        <v>1</v>
+      <c r="D27" s="6">
+        <v>100</v>
       </c>
       <c r="E27">
         <v>4</v>
@@ -2169,7 +2173,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
@@ -2179,8 +2183,8 @@
       <c r="C28">
         <v>4</v>
       </c>
-      <c r="D28">
-        <v>1</v>
+      <c r="D28" s="6">
+        <v>100</v>
       </c>
       <c r="E28">
         <v>4</v>
@@ -2201,7 +2205,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2211,8 +2215,8 @@
       <c r="C29">
         <v>5</v>
       </c>
-      <c r="D29">
-        <v>0</v>
+      <c r="D29" s="6">
+        <v>100</v>
       </c>
       <c r="E29">
         <v>3</v>
@@ -2233,7 +2237,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2243,8 +2247,8 @@
       <c r="C30">
         <v>5</v>
       </c>
-      <c r="D30">
-        <v>0</v>
+      <c r="D30" s="6">
+        <v>100</v>
       </c>
       <c r="E30">
         <v>2</v>
@@ -2265,7 +2269,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>104</v>
       </c>
@@ -2275,8 +2279,8 @@
       <c r="C31">
         <v>5</v>
       </c>
-      <c r="D31">
-        <v>0</v>
+      <c r="D31" s="6">
+        <v>100</v>
       </c>
       <c r="E31">
         <v>4</v>
@@ -2297,7 +2301,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>105</v>
       </c>
@@ -2307,8 +2311,8 @@
       <c r="C32">
         <v>5</v>
       </c>
-      <c r="D32">
-        <v>0</v>
+      <c r="D32" s="6">
+        <v>100</v>
       </c>
       <c r="E32">
         <v>2</v>
@@ -2329,7 +2333,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>106</v>
       </c>
@@ -2339,8 +2343,8 @@
       <c r="C33">
         <v>6</v>
       </c>
-      <c r="D33">
-        <v>0</v>
+      <c r="D33" s="6">
+        <v>100</v>
       </c>
       <c r="E33">
         <v>2.5</v>
@@ -2358,7 +2362,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>107</v>
       </c>
@@ -2368,8 +2372,8 @@
       <c r="C34">
         <v>6</v>
       </c>
-      <c r="D34">
-        <v>0</v>
+      <c r="D34" s="6">
+        <v>100</v>
       </c>
       <c r="E34">
         <v>2.5</v>
@@ -2390,7 +2394,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>108</v>
       </c>
@@ -2400,8 +2404,8 @@
       <c r="C35">
         <v>6</v>
       </c>
-      <c r="D35">
-        <v>0</v>
+      <c r="D35" s="6">
+        <v>100</v>
       </c>
       <c r="E35">
         <v>2.5</v>
@@ -2419,7 +2423,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>109</v>
       </c>
@@ -2429,8 +2433,8 @@
       <c r="C36">
         <v>6</v>
       </c>
-      <c r="D36">
-        <v>0</v>
+      <c r="D36" s="6">
+        <v>100</v>
       </c>
       <c r="E36">
         <v>3</v>
@@ -2445,7 +2449,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
         <v>110</v>
       </c>
@@ -2455,8 +2459,8 @@
       <c r="C37">
         <v>6</v>
       </c>
-      <c r="D37">
-        <v>0</v>
+      <c r="D37" s="6">
+        <v>100</v>
       </c>
       <c r="E37">
         <v>2</v>
@@ -2471,7 +2475,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>111</v>
       </c>
@@ -2481,8 +2485,8 @@
       <c r="C38">
         <v>7</v>
       </c>
-      <c r="D38">
-        <v>0</v>
+      <c r="D38" s="6">
+        <v>100</v>
       </c>
       <c r="E38">
         <v>2</v>
@@ -2503,7 +2507,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>112</v>
       </c>
@@ -2513,8 +2517,8 @@
       <c r="C39">
         <v>8</v>
       </c>
-      <c r="D39">
-        <v>0</v>
+      <c r="D39" s="6">
+        <v>100</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -2529,7 +2533,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>113</v>
       </c>
@@ -2539,8 +2543,8 @@
       <c r="C40">
         <v>8</v>
       </c>
-      <c r="D40">
-        <v>0</v>
+      <c r="D40" s="6">
+        <v>100</v>
       </c>
       <c r="E40">
         <v>3</v>
@@ -2558,7 +2562,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>114</v>
       </c>
@@ -2568,8 +2572,8 @@
       <c r="C41">
         <v>8</v>
       </c>
-      <c r="D41">
-        <v>0</v>
+      <c r="D41" s="6">
+        <v>100</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -2587,7 +2591,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>115</v>
       </c>
@@ -2597,8 +2601,8 @@
       <c r="C42">
         <v>9</v>
       </c>
-      <c r="D42">
-        <v>0</v>
+      <c r="D42" s="6">
+        <v>100</v>
       </c>
       <c r="E42">
         <v>2</v>
@@ -2616,7 +2620,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>116</v>
       </c>
@@ -2626,8 +2630,8 @@
       <c r="C43">
         <v>9</v>
       </c>
-      <c r="D43">
-        <v>0</v>
+      <c r="D43" s="6">
+        <v>100</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -2645,11 +2649,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2"/>
       <c r="I44" s="5"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L44" xr:uid="{EFBEFAD7-39D5-4626-81BE-F838DB4CBFA9}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2657,27 +2662,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.625" customWidth="1"/>
-    <col min="11" max="12" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.89453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.3671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.89453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.89453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.62890625" customWidth="1"/>
+    <col min="11" max="12" width="19.3671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2715,7 +2720,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="10" t="s">
         <v>31</v>
       </c>
@@ -2753,7 +2758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="11" t="s">
         <v>32</v>
       </c>
@@ -2791,7 +2796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="11" t="s">
         <v>33</v>
       </c>
@@ -2826,7 +2831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="11" t="s">
         <v>34</v>
       </c>
@@ -2861,7 +2866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="11" t="s">
         <v>35</v>
       </c>
@@ -2893,7 +2898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="11" t="s">
         <v>36</v>
       </c>
@@ -2925,7 +2930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="11" t="s">
         <v>37</v>
       </c>
@@ -2960,7 +2965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="11" t="s">
         <v>38</v>
       </c>
@@ -2995,7 +3000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="11" t="s">
         <v>39</v>
       </c>
@@ -3033,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="11" t="s">
         <v>40</v>
       </c>
@@ -3068,7 +3073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="11" t="s">
         <v>41</v>
       </c>
@@ -3103,7 +3108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="11" t="s">
         <v>42</v>
       </c>
@@ -3141,7 +3146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="11" t="s">
         <v>43</v>
       </c>
@@ -3176,7 +3181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="11" t="s">
         <v>44</v>
       </c>
@@ -3214,7 +3219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="11" t="s">
         <v>45</v>
       </c>
@@ -3252,7 +3257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="11" t="s">
         <v>46</v>
       </c>
@@ -3290,7 +3295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="11" t="s">
         <v>47</v>
       </c>
@@ -3328,7 +3333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A19" s="12" t="s">
         <v>48</v>
       </c>
@@ -3366,7 +3371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="11" t="s">
         <v>217</v>
       </c>
@@ -3380,7 +3385,7 @@
         <v>60</v>
       </c>
       <c r="F20" s="4">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="G20" s="4">
         <v>1</v>
@@ -3401,7 +3406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="11" t="s">
         <v>220</v>
       </c>
@@ -3415,7 +3420,7 @@
         <v>60</v>
       </c>
       <c r="F21" s="4">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="G21" s="4">
         <v>1</v>
@@ -3436,7 +3441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="11" t="s">
         <v>221</v>
       </c>
@@ -3450,7 +3455,7 @@
         <v>60</v>
       </c>
       <c r="F22" s="4">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="G22" s="4">
         <v>1</v>
@@ -3471,7 +3476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="11" t="s">
         <v>222</v>
       </c>
@@ -3485,7 +3490,7 @@
         <v>60</v>
       </c>
       <c r="F23" s="4">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="G23" s="4">
         <v>1</v>
@@ -3506,7 +3511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="11" t="s">
         <v>226</v>
       </c>
@@ -3520,7 +3525,7 @@
         <v>60</v>
       </c>
       <c r="F24" s="4">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="G24" s="4">
         <v>1</v>
@@ -3541,7 +3546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="11" t="s">
         <v>227</v>
       </c>
@@ -3555,7 +3560,7 @@
         <v>60</v>
       </c>
       <c r="F25" s="4">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="G25" s="4">
         <v>1</v>
@@ -3576,7 +3581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="11" t="s">
         <v>229</v>
       </c>
@@ -3590,7 +3595,7 @@
         <v>60</v>
       </c>
       <c r="F26" s="4">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="G26" s="4">
         <v>1</v>
@@ -3611,19 +3616,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E36" s="5"/>
     </row>
-    <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="1048576" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C1048576" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix 'Roni Sova' bug (giving weekends to veterans)
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omri3\Documents\Projects\Automated-shifts-assignment\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4947A3-4A26-4EAD-8A8C-669DD18973D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B067AABC-9993-41A9-B125-6CA014522700}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="269">
   <si>
     <t>id</t>
   </si>
@@ -454,415 +454,388 @@
     <t>Compatible</t>
   </si>
   <si>
+    <t>10,18,23</t>
+  </si>
+  <si>
+    <t>14,25,31</t>
+  </si>
+  <si>
+    <t>2,11,17,23</t>
+  </si>
+  <si>
+    <t>2,9</t>
+  </si>
+  <si>
+    <t>4,9,15,22,29</t>
+  </si>
+  <si>
+    <t>2,9,15,23</t>
+  </si>
+  <si>
+    <t>2,9,18,23,30</t>
+  </si>
+  <si>
+    <t>9,25</t>
+  </si>
+  <si>
+    <t>4,9,16</t>
+  </si>
+  <si>
+    <t>9,18,23,30</t>
+  </si>
+  <si>
+    <t>11,14,23</t>
+  </si>
+  <si>
+    <t>3,23,29</t>
+  </si>
+  <si>
+    <t>17,25</t>
+  </si>
+  <si>
+    <t>7,15,23</t>
+  </si>
+  <si>
+    <t>7,23</t>
+  </si>
+  <si>
+    <t>Not evening</t>
+  </si>
+  <si>
+    <t>Not task</t>
+  </si>
+  <si>
+    <t>probability</t>
+  </si>
+  <si>
+    <t>YARDIT</t>
+  </si>
+  <si>
+    <t>min_per_month</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>#F28D9F</t>
+  </si>
+  <si>
+    <t>#F24452</t>
+  </si>
+  <si>
+    <t>#F2CB05</t>
+  </si>
+  <si>
+    <t>#17BF60</t>
+  </si>
+  <si>
+    <t>#B8D9C4</t>
+  </si>
+  <si>
+    <t>#F2E205</t>
+  </si>
+  <si>
+    <t>#F24171</t>
+  </si>
+  <si>
+    <t>#EAF205</t>
+  </si>
+  <si>
+    <t>#0BD9D9</t>
+  </si>
+  <si>
+    <t>#762CBF</t>
+  </si>
+  <si>
+    <t>#7216F2</t>
+  </si>
+  <si>
+    <t>#F2EEAC</t>
+  </si>
+  <si>
+    <t>#EDC4F2</t>
+  </si>
+  <si>
+    <t>#29A7D9</t>
+  </si>
+  <si>
+    <t>#F249A6</t>
+  </si>
+  <si>
+    <t>#50F205</t>
+  </si>
+  <si>
+    <t>#D9B29C</t>
+  </si>
+  <si>
+    <t>tasks available</t>
+  </si>
+  <si>
+    <t>days_in_week</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>bakut</t>
+  </si>
+  <si>
+    <t>equipment</t>
+  </si>
+  <si>
+    <t>ftt</t>
+  </si>
+  <si>
+    <t>equip_oper</t>
+  </si>
+  <si>
+    <t>bakut_oper</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5</t>
+  </si>
+  <si>
+    <t>T19</t>
+  </si>
+  <si>
+    <t>Sofash bakut day 1</t>
+  </si>
+  <si>
+    <t>Sofash bakut day 2</t>
+  </si>
+  <si>
+    <t>T20</t>
+  </si>
+  <si>
+    <t>T21</t>
+  </si>
+  <si>
+    <t>T22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sofash Equip day </t>
+  </si>
+  <si>
+    <t>Sofash bakut night 1</t>
+  </si>
+  <si>
+    <t>Sofash bakut night 2</t>
+  </si>
+  <si>
+    <t>T23</t>
+  </si>
+  <si>
+    <t>T24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sofash Equip night </t>
+  </si>
+  <si>
+    <t>T25</t>
+  </si>
+  <si>
+    <t>Sofash production</t>
+  </si>
+  <si>
+    <t>T1, T2, T5, T7, T10, T11, T14, T15 ,T16, T17, T19, T20, T21, T22, T23, T24, T25</t>
+  </si>
+  <si>
+    <t>T1, T2, T5, T7, , T9, T10, T11, T14, T15 ,T16, T17, T19, T20, T21, T22, T23, T24, T25</t>
+  </si>
+  <si>
+    <t>T1, T2, T3, T4 ,T5, T6, T10, T11, T12, T13, T15, T16, T17, T18 , T19, T20, T22, T23, T25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T1, T2, T3, T4 ,T5, T6, T10, T11, T12, T13, T15, T16, T17, T18 ,T19, T20, T22, T23, T25 </t>
+  </si>
+  <si>
+    <t>T1, T2, T3, T4 ,T5, T6, T7, T8, T9, T10, T11</t>
+  </si>
+  <si>
+    <t>T1, T2, T3, T4 ,T5, T6, T7, T8 , T12, T13, T14, T15, T18, T19, T20, T21, T22, T23, T24</t>
+  </si>
+  <si>
+    <t>T1, T2, T3, T4 ,T5, T6, T10, T11, T12, T13, T15, T16, T17, T18 , T19, T20, T22, T23</t>
+  </si>
+  <si>
+    <t>T1, T2, T3, T4 ,T5, T6, T7, T8, T19, T20, T21, T22, T23, T24</t>
+  </si>
+  <si>
+    <t>T1, T2, T5, T7, , T9, T14, T15, T19, T20, T21, T22, T23, T24</t>
+  </si>
+  <si>
+    <t>T7, T8 , T19, T21, T24</t>
+  </si>
+  <si>
+    <t>T1, T2, T3, T4 ,T5, T6, T7, T8, T9, T14, T15, T19, T20, T21, T22, T23, T24</t>
+  </si>
+  <si>
+    <t>T7, T8 , T21, T24</t>
+  </si>
+  <si>
+    <t>T1, T2, T5, T7, , T9, T14, T15, T19, T20, T21</t>
+  </si>
+  <si>
+    <t>T7, T10, T11, T14, T16, T17, T21, T25</t>
+  </si>
+  <si>
+    <t>T1, T2, T3, T4 ,T5, T6, T10, T11, T19, T20, T25</t>
+  </si>
+  <si>
+    <t>T1, T2, T3, T4 ,T5, T6, T7, T8, T9, T14, T15, T19, T20, T21</t>
+  </si>
+  <si>
+    <t>qualified tasks</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CLANING THE TAHAK, bakut, equipment, ftt, marzuk, equip oper, bakut oper  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, CLANING THE TAHAK, bakut, sar poduction, ftt, marzuk, bakut oper  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bakut, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bakut, equipment, wv equipment, bakut oper, equip oper  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, bakut, equipment, sar poduction, wv equipment, equip oper, bakut oper  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, bakut, equipment, sar poduction, equip oper, bakut oper  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sar poduction  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, equip oper, sar poduction, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, bakut, sar poduction  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, bakut, sar poduction, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bakut, wv equipment, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, bakut, equipment, sar poduction, wv equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, sar poduction  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> equip oper, equipment  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bakut  </t>
+  </si>
+  <si>
+    <t>pazam</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CLANING THE TAHAK, bakut, equipment, ftt, marzuk, equip oper, bakut oper , </t>
+  </si>
+  <si>
+    <t>RC</t>
+  </si>
+  <si>
+    <t>CLANING THE TAHAK</t>
+  </si>
+  <si>
+    <t>#808080</t>
+  </si>
+  <si>
+    <t>#ffed4d</t>
+  </si>
+  <si>
+    <t>#f5eca2</t>
+  </si>
+  <si>
+    <t>#b6fa9b</t>
+  </si>
+  <si>
+    <t>#4cd615</t>
+  </si>
+  <si>
+    <t>#ffb536</t>
+  </si>
+  <si>
+    <t>#ff6236</t>
+  </si>
+  <si>
+    <t>MAX_Sofashim</t>
+  </si>
+  <si>
+    <t>is_sofash</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eo production, sar poduction, equip oper, equipment</t>
+  </si>
+  <si>
+    <t>26,27</t>
+  </si>
+  <si>
+    <t>19,20</t>
+  </si>
+  <si>
+    <t>5,6</t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>26,27,28</t>
+  </si>
+  <si>
+    <t>11,12,13</t>
+  </si>
+  <si>
+    <t>9,12,13</t>
+  </si>
+  <si>
+    <t>2,3,4,5</t>
+  </si>
+  <si>
+    <t>7,17,26,27</t>
+  </si>
+  <si>
+    <t>9,17,26,27</t>
+  </si>
+  <si>
+    <t>5,6,19,20</t>
+  </si>
+  <si>
+    <t>2,3,5,6,10</t>
+  </si>
+  <si>
+    <t>19,20,26,27</t>
+  </si>
+  <si>
+    <t>3,5,6,17</t>
+  </si>
+  <si>
+    <t>10,11</t>
+  </si>
+  <si>
     <t>1,26,27</t>
   </si>
   <si>
-    <t>9,17,26,27</t>
-  </si>
-  <si>
-    <t>5,6,19,20</t>
-  </si>
-  <si>
-    <t>10,18,23</t>
-  </si>
-  <si>
-    <t>9,12,13,26,27</t>
-  </si>
-  <si>
-    <t>14,25,31</t>
-  </si>
-  <si>
-    <t>1,3,12,13,24</t>
-  </si>
-  <si>
-    <t>2,11,17,23</t>
-  </si>
-  <si>
-    <t>12,13,26,27</t>
-  </si>
-  <si>
-    <t>5,6,12,13</t>
-  </si>
-  <si>
-    <t>2,9</t>
-  </si>
-  <si>
-    <t>8,12,13,26,27</t>
-  </si>
-  <si>
-    <t>5,6,26,27</t>
-  </si>
-  <si>
-    <t>4,9,15,22,29</t>
-  </si>
-  <si>
-    <t>26,27</t>
-  </si>
-  <si>
-    <t>2,9,15,23</t>
-  </si>
-  <si>
-    <t>2,9,18,23,30</t>
-  </si>
-  <si>
-    <t>9,25</t>
-  </si>
-  <si>
-    <t>4,9,16</t>
-  </si>
-  <si>
-    <t>9,18,23,30</t>
-  </si>
-  <si>
-    <t>11,12,13</t>
-  </si>
-  <si>
-    <t>11,14,23</t>
-  </si>
-  <si>
-    <t>19,20,26,27</t>
-  </si>
-  <si>
-    <t>19,20,26,27,30</t>
-  </si>
-  <si>
-    <t>7,17,26,27</t>
-  </si>
-  <si>
-    <t>3,23,29</t>
+    <t>3,14,17</t>
+  </si>
+  <si>
+    <t>1,3,4,5,6,9</t>
+  </si>
+  <si>
+    <t>1,11</t>
   </si>
   <si>
     <t>2,9,16,23</t>
-  </si>
-  <si>
-    <t>1,3,4,5,6,9,16,23,26,27</t>
-  </si>
-  <si>
-    <t>3,14,17</t>
-  </si>
-  <si>
-    <t>3,5,6,17,25,26,27</t>
-  </si>
-  <si>
-    <t>3,10,21,23,26,27,28</t>
-  </si>
-  <si>
-    <t>17,25</t>
-  </si>
-  <si>
-    <t>9,19,20,26,27,28</t>
-  </si>
-  <si>
-    <t>10,11,18,19,20,21,26,27</t>
-  </si>
-  <si>
-    <t>10,11,26,27,28</t>
-  </si>
-  <si>
-    <t>7,15,23</t>
-  </si>
-  <si>
-    <t>2,3,5,6,10,21,26,27</t>
-  </si>
-  <si>
-    <t>11,12,13,14,26,27</t>
-  </si>
-  <si>
-    <t>1,11</t>
-  </si>
-  <si>
-    <t>2,3,4,5,6,8,10,11,17,23,25,26,27</t>
-  </si>
-  <si>
-    <t>9,10,11,14,15,16,17,18,19,20,21,23,25,26,27,28</t>
-  </si>
-  <si>
-    <t>7,23</t>
-  </si>
-  <si>
-    <t>26,27,28</t>
-  </si>
-  <si>
-    <t>8,10,11,12,13,25,26,27</t>
-  </si>
-  <si>
-    <t>Not evening</t>
-  </si>
-  <si>
-    <t>Not task</t>
-  </si>
-  <si>
-    <t>probability</t>
-  </si>
-  <si>
-    <t>YARDIT</t>
-  </si>
-  <si>
-    <t>min_per_month</t>
-  </si>
-  <si>
-    <t>color</t>
-  </si>
-  <si>
-    <t>#F28D9F</t>
-  </si>
-  <si>
-    <t>#F24452</t>
-  </si>
-  <si>
-    <t>#F2CB05</t>
-  </si>
-  <si>
-    <t>#17BF60</t>
-  </si>
-  <si>
-    <t>#B8D9C4</t>
-  </si>
-  <si>
-    <t>#F2E205</t>
-  </si>
-  <si>
-    <t>#F24171</t>
-  </si>
-  <si>
-    <t>#EAF205</t>
-  </si>
-  <si>
-    <t>#0BD9D9</t>
-  </si>
-  <si>
-    <t>#762CBF</t>
-  </si>
-  <si>
-    <t>#7216F2</t>
-  </si>
-  <si>
-    <t>#F2EEAC</t>
-  </si>
-  <si>
-    <t>#EDC4F2</t>
-  </si>
-  <si>
-    <t>#29A7D9</t>
-  </si>
-  <si>
-    <t>#F249A6</t>
-  </si>
-  <si>
-    <t>#50F205</t>
-  </si>
-  <si>
-    <t>#D9B29C</t>
-  </si>
-  <si>
-    <t>tasks available</t>
-  </si>
-  <si>
-    <t>days_in_week</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>bakut</t>
-  </si>
-  <si>
-    <t>equipment</t>
-  </si>
-  <si>
-    <t>ftt</t>
-  </si>
-  <si>
-    <t>equip_oper</t>
-  </si>
-  <si>
-    <t>bakut_oper</t>
-  </si>
-  <si>
-    <t>1,2,3,4,5</t>
-  </si>
-  <si>
-    <t>T19</t>
-  </si>
-  <si>
-    <t>Sofash bakut day 1</t>
-  </si>
-  <si>
-    <t>Sofash bakut day 2</t>
-  </si>
-  <si>
-    <t>T20</t>
-  </si>
-  <si>
-    <t>T21</t>
-  </si>
-  <si>
-    <t>T22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sofash Equip day </t>
-  </si>
-  <si>
-    <t>Sofash bakut night 1</t>
-  </si>
-  <si>
-    <t>Sofash bakut night 2</t>
-  </si>
-  <si>
-    <t>T23</t>
-  </si>
-  <si>
-    <t>T24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sofash Equip night </t>
-  </si>
-  <si>
-    <t>T25</t>
-  </si>
-  <si>
-    <t>Sofash production</t>
-  </si>
-  <si>
-    <t>T1, T2, T5, T7, T10, T11, T14, T15 ,T16, T17, T19, T20, T21, T22, T23, T24, T25</t>
-  </si>
-  <si>
-    <t>T1, T2, T5, T7, , T9, T10, T11, T14, T15 ,T16, T17, T19, T20, T21, T22, T23, T24, T25</t>
-  </si>
-  <si>
-    <t>T1, T2, T3, T4 ,T5, T6, T10, T11, T12, T13, T15, T16, T17, T18 , T19, T20, T22, T23, T25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T1, T2, T3, T4 ,T5, T6, T10, T11, T12, T13, T15, T16, T17, T18 ,T19, T20, T22, T23, T25 </t>
-  </si>
-  <si>
-    <t>T1, T2, T3, T4 ,T5, T6, T7, T8, T9, T10, T11</t>
-  </si>
-  <si>
-    <t>T1, T2, T3, T4 ,T5, T6, T7, T8 , T12, T13, T14, T15, T18, T19, T20, T21, T22, T23, T24</t>
-  </si>
-  <si>
-    <t>T1, T2, T3, T4 ,T5, T6, T10, T11, T12, T13, T15, T16, T17, T18 , T19, T20, T22, T23</t>
-  </si>
-  <si>
-    <t>T1, T2, T3, T4 ,T5, T6, T7, T8, T19, T20, T21, T22, T23, T24</t>
-  </si>
-  <si>
-    <t>T1, T2, T5, T7, , T9, T14, T15, T19, T20, T21, T22, T23, T24</t>
-  </si>
-  <si>
-    <t>T7, T8 , T19, T21, T24</t>
-  </si>
-  <si>
-    <t>T1, T2, T3, T4 ,T5, T6, T7, T8, T9, T14, T15, T19, T20, T21, T22, T23, T24</t>
-  </si>
-  <si>
-    <t>T7, T8 , T21, T24</t>
-  </si>
-  <si>
-    <t>T1, T2, T5, T7, , T9, T14, T15, T19, T20, T21</t>
-  </si>
-  <si>
-    <t>T7, T10, T11, T14, T16, T17, T21, T25</t>
-  </si>
-  <si>
-    <t>T1, T2, T3, T4 ,T5, T6, T10, T11, T19, T20, T25</t>
-  </si>
-  <si>
-    <t>T1, T2, T3, T4 ,T5, T6, T7, T8, T9, T14, T15, T19, T20, T21</t>
-  </si>
-  <si>
-    <t>qualified tasks</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CLANING THE TAHAK, bakut, equipment, ftt, marzuk, equip oper, bakut oper  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> eo production, CLANING THE TAHAK, bakut, sar poduction, ftt, marzuk, bakut oper  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> bakut, equipment  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> bakut, equipment, wv equipment, bakut oper, equip oper  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> eo production, bakut, equipment, sar poduction, wv equipment, equip oper, bakut oper  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> eo production, bakut, equipment, sar poduction, equip oper, bakut oper  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> equipment  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sar poduction  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> eo production, equip oper, sar poduction, equipment  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> eo production, bakut, sar poduction  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> eo production, bakut, sar poduction, equipment  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> bakut, wv equipment, equipment  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> eo production, bakut, equipment, sar poduction, wv equipment  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> eo production, sar poduction  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> equip oper, equipment  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> eo production, sar poduction, equip oper, equipment  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> bakut  </t>
-  </si>
-  <si>
-    <t>pazam</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CLANING THE TAHAK, bakut, equipment, ftt, marzuk, equip oper, bakut oper , </t>
-  </si>
-  <si>
-    <t>RC</t>
-  </si>
-  <si>
-    <t>CLANING THE TAHAK</t>
-  </si>
-  <si>
-    <t>#808080</t>
-  </si>
-  <si>
-    <t>#ffed4d</t>
-  </si>
-  <si>
-    <t>#f5eca2</t>
-  </si>
-  <si>
-    <t>#b6fa9b</t>
-  </si>
-  <si>
-    <t>#4cd615</t>
-  </si>
-  <si>
-    <t>#ffb536</t>
-  </si>
-  <si>
-    <t>#ff6236</t>
-  </si>
-  <si>
-    <t>MAX_Sofashim</t>
-  </si>
-  <si>
-    <t>is_sofash</t>
   </si>
 </sst>
 </file>
@@ -1317,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1343,10 +1316,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>265</v>
+        <v>235</v>
       </c>
       <c r="D1" t="s">
-        <v>276</v>
+        <v>246</v>
       </c>
       <c r="E1" t="s">
         <v>135</v>
@@ -1355,16 +1328,16 @@
         <v>136</v>
       </c>
       <c r="G1" t="s">
-        <v>185</v>
+        <v>156</v>
       </c>
       <c r="H1" t="s">
-        <v>186</v>
+        <v>157</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>247</v>
+        <v>218</v>
       </c>
       <c r="J1" t="s">
-        <v>208</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1387,13 +1360,13 @@
         <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>155</v>
+        <v>249</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>266</v>
+        <v>236</v>
       </c>
       <c r="J2" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1415,14 +1388,14 @@
       <c r="F3">
         <v>14</v>
       </c>
-      <c r="H3" t="s">
-        <v>152</v>
+      <c r="H3">
+        <v>8</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="J3" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1445,16 +1418,16 @@
         <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>157</v>
-      </c>
-      <c r="H4" t="s">
-        <v>143</v>
+        <v>147</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="J4" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1477,16 +1450,13 @@
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>249</v>
+        <v>220</v>
       </c>
       <c r="J5" t="s">
-        <v>237</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1494,7 +1464,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>267</v>
+        <v>237</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1509,16 +1479,16 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="H6" t="s">
-        <v>155</v>
+        <v>249</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>249</v>
+        <v>220</v>
       </c>
       <c r="J6" t="s">
-        <v>233</v>
+        <v>204</v>
       </c>
       <c r="L6" s="5"/>
     </row>
@@ -1542,16 +1512,16 @@
         <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="H7" t="s">
-        <v>143</v>
+        <v>250</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>249</v>
+        <v>220</v>
       </c>
       <c r="J7" t="s">
-        <v>234</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1574,16 +1544,16 @@
         <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="H8" t="s">
-        <v>155</v>
+        <v>249</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="J8" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1606,16 +1576,16 @@
         <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>151</v>
-      </c>
-      <c r="H9" t="s">
-        <v>150</v>
+        <v>144</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="J9" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1638,16 +1608,16 @@
         <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="H10" t="s">
-        <v>153</v>
+        <v>251</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="J10" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1657,7 +1627,7 @@
       <c r="B11" t="s">
         <v>80</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>2</v>
       </c>
       <c r="D11" s="6">
@@ -1670,16 +1640,16 @@
         <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H11" t="s">
-        <v>147</v>
+        <v>252</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="J11" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1689,7 +1659,7 @@
       <c r="B12" t="s">
         <v>81</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <v>2</v>
       </c>
       <c r="D12" s="6">
@@ -1704,14 +1674,11 @@
       <c r="G12">
         <v>23</v>
       </c>
-      <c r="H12" t="s">
-        <v>149</v>
-      </c>
       <c r="I12" s="5" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="J12" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1721,7 +1688,7 @@
       <c r="B13" t="s">
         <v>85</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="6">
         <v>2</v>
       </c>
       <c r="D13" s="6">
@@ -1734,16 +1701,16 @@
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="H13" t="s">
-        <v>153</v>
+        <v>251</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>249</v>
+        <v>220</v>
       </c>
       <c r="J13" t="s">
-        <v>233</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1753,7 +1720,7 @@
       <c r="B14" t="s">
         <v>86</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="6">
         <v>2</v>
       </c>
       <c r="D14" s="6">
@@ -1769,13 +1736,13 @@
         <v>23</v>
       </c>
       <c r="H14" t="s">
-        <v>183</v>
+        <v>253</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>250</v>
+        <v>221</v>
       </c>
       <c r="J14" t="s">
-        <v>238</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1785,8 +1752,8 @@
       <c r="B15" t="s">
         <v>87</v>
       </c>
-      <c r="C15">
-        <v>3</v>
+      <c r="C15" s="6">
+        <v>2</v>
       </c>
       <c r="D15">
         <v>100</v>
@@ -1798,13 +1765,13 @@
         <v>8</v>
       </c>
       <c r="H15" t="s">
-        <v>161</v>
+        <v>254</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>251</v>
+        <v>222</v>
       </c>
       <c r="J15" t="s">
-        <v>239</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1814,8 +1781,8 @@
       <c r="B16" t="s">
         <v>74</v>
       </c>
-      <c r="C16">
-        <v>3</v>
+      <c r="C16" s="6">
+        <v>2</v>
       </c>
       <c r="D16" s="6">
         <v>100</v>
@@ -1827,16 +1794,16 @@
         <v>8</v>
       </c>
       <c r="G16" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H16" t="s">
-        <v>145</v>
+        <v>255</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>252</v>
+        <v>223</v>
       </c>
       <c r="J16" t="s">
-        <v>232</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1846,8 +1813,8 @@
       <c r="B17" t="s">
         <v>88</v>
       </c>
-      <c r="C17">
-        <v>3</v>
+      <c r="C17" s="6">
+        <v>2</v>
       </c>
       <c r="D17" s="6">
         <v>100</v>
@@ -1859,13 +1826,13 @@
         <v>8</v>
       </c>
       <c r="H17" t="s">
-        <v>180</v>
+        <v>256</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>253</v>
+        <v>224</v>
       </c>
       <c r="J17" t="s">
-        <v>231</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1875,8 +1842,8 @@
       <c r="B18" t="s">
         <v>75</v>
       </c>
-      <c r="C18">
-        <v>3</v>
+      <c r="C18" s="6">
+        <v>2</v>
       </c>
       <c r="D18" s="6">
         <v>100</v>
@@ -1890,14 +1857,14 @@
       <c r="G18">
         <v>8</v>
       </c>
-      <c r="H18" t="s">
-        <v>181</v>
+      <c r="H18">
+        <v>9</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>253</v>
+        <v>224</v>
       </c>
       <c r="J18" t="s">
-        <v>231</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1907,8 +1874,8 @@
       <c r="B19" t="s">
         <v>89</v>
       </c>
-      <c r="C19">
-        <v>3</v>
+      <c r="C19" s="6">
+        <v>2</v>
       </c>
       <c r="D19" s="6">
         <v>100</v>
@@ -1920,16 +1887,16 @@
         <v>8</v>
       </c>
       <c r="G19" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="H19" t="s">
-        <v>178</v>
+        <v>254</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>254</v>
+        <v>225</v>
       </c>
       <c r="J19" t="s">
-        <v>240</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1939,8 +1906,8 @@
       <c r="B20" t="s">
         <v>90</v>
       </c>
-      <c r="C20">
-        <v>3</v>
+      <c r="C20" s="6">
+        <v>2</v>
       </c>
       <c r="D20" s="6">
         <v>100</v>
@@ -1952,16 +1919,16 @@
         <v>8</v>
       </c>
       <c r="G20" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="H20" t="s">
-        <v>165</v>
+        <v>257</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>251</v>
+        <v>222</v>
       </c>
       <c r="J20" t="s">
-        <v>241</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1969,10 +1936,10 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>188</v>
-      </c>
-      <c r="C21">
-        <v>4</v>
+        <v>159</v>
+      </c>
+      <c r="C21" s="6">
+        <v>3</v>
       </c>
       <c r="D21" s="6">
         <v>0</v>
@@ -1984,7 +1951,7 @@
         <v>2</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="J21" t="s">
         <v>41</v>
@@ -1997,8 +1964,8 @@
       <c r="B22" t="s">
         <v>72</v>
       </c>
-      <c r="C22">
-        <v>4</v>
+      <c r="C22" s="6">
+        <v>3</v>
       </c>
       <c r="D22" s="6">
         <v>100</v>
@@ -2013,13 +1980,13 @@
         <v>10</v>
       </c>
       <c r="H22" t="s">
-        <v>142</v>
+        <v>258</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>251</v>
+        <v>222</v>
       </c>
       <c r="J22" t="s">
-        <v>243</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2029,8 +1996,8 @@
       <c r="B23" t="s">
         <v>73</v>
       </c>
-      <c r="C23">
-        <v>4</v>
+      <c r="C23" s="6">
+        <v>3</v>
       </c>
       <c r="D23" s="6">
         <v>100</v>
@@ -2042,16 +2009,16 @@
         <v>8</v>
       </c>
       <c r="G23" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H23" t="s">
-        <v>143</v>
+        <v>259</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="J23" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2061,8 +2028,8 @@
       <c r="B24" t="s">
         <v>91</v>
       </c>
-      <c r="C24">
-        <v>4</v>
+      <c r="C24" s="6">
+        <v>3</v>
       </c>
       <c r="D24" s="6">
         <v>100</v>
@@ -2074,13 +2041,13 @@
         <v>8</v>
       </c>
       <c r="H24" t="s">
-        <v>177</v>
+        <v>260</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>257</v>
+        <v>228</v>
       </c>
       <c r="J24" t="s">
-        <v>245</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2090,8 +2057,8 @@
       <c r="B25" t="s">
         <v>92</v>
       </c>
-      <c r="C25">
-        <v>4</v>
+      <c r="C25" s="6">
+        <v>3</v>
       </c>
       <c r="D25" s="6">
         <v>100</v>
@@ -2103,16 +2070,16 @@
         <v>8</v>
       </c>
       <c r="G25" t="s">
-        <v>172</v>
-      </c>
-      <c r="H25" t="s">
-        <v>171</v>
+        <v>153</v>
+      </c>
+      <c r="H25">
+        <v>23</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>257</v>
+        <v>228</v>
       </c>
       <c r="J25" t="s">
-        <v>245</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2122,8 +2089,8 @@
       <c r="B26" t="s">
         <v>93</v>
       </c>
-      <c r="C26">
-        <v>4</v>
+      <c r="C26" s="6">
+        <v>3</v>
       </c>
       <c r="D26" s="6">
         <v>100</v>
@@ -2134,14 +2101,14 @@
       <c r="F26">
         <v>8</v>
       </c>
-      <c r="H26" t="s">
-        <v>184</v>
+      <c r="H26">
+        <v>8</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>254</v>
+        <v>225</v>
       </c>
       <c r="J26" t="s">
-        <v>242</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2151,8 +2118,8 @@
       <c r="B27" t="s">
         <v>94</v>
       </c>
-      <c r="C27">
-        <v>4</v>
+      <c r="C27" s="6">
+        <v>3</v>
       </c>
       <c r="D27" s="6">
         <v>100</v>
@@ -2163,14 +2130,14 @@
       <c r="F27">
         <v>8</v>
       </c>
-      <c r="H27" t="s">
-        <v>164</v>
+      <c r="H27">
+        <v>30</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>257</v>
+        <v>228</v>
       </c>
       <c r="J27" t="s">
-        <v>245</v>
+        <v>216</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2180,8 +2147,8 @@
       <c r="B28" t="s">
         <v>95</v>
       </c>
-      <c r="C28">
-        <v>4</v>
+      <c r="C28" s="6">
+        <v>3</v>
       </c>
       <c r="D28" s="6">
         <v>100</v>
@@ -2196,13 +2163,13 @@
         <v>10</v>
       </c>
       <c r="H28" t="s">
-        <v>163</v>
+        <v>261</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>251</v>
+        <v>222</v>
       </c>
       <c r="J28" t="s">
-        <v>246</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2212,8 +2179,8 @@
       <c r="B29" t="s">
         <v>96</v>
       </c>
-      <c r="C29">
-        <v>5</v>
+      <c r="C29" s="6">
+        <v>4</v>
       </c>
       <c r="D29" s="6">
         <v>100</v>
@@ -2228,10 +2195,10 @@
         <v>7</v>
       </c>
       <c r="H29" t="s">
-        <v>170</v>
+        <v>262</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>258</v>
+        <v>229</v>
       </c>
       <c r="J29" t="s">
         <v>126</v>
@@ -2244,8 +2211,8 @@
       <c r="B30" t="s">
         <v>97</v>
       </c>
-      <c r="C30">
-        <v>5</v>
+      <c r="C30" s="6">
+        <v>4</v>
       </c>
       <c r="D30" s="6">
         <v>100</v>
@@ -2257,13 +2224,13 @@
         <v>5</v>
       </c>
       <c r="G30" t="s">
-        <v>176</v>
-      </c>
-      <c r="H30" t="s">
-        <v>175</v>
+        <v>154</v>
+      </c>
+      <c r="H30">
+        <v>28</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>259</v>
+        <v>230</v>
       </c>
       <c r="J30" t="s">
         <v>124</v>
@@ -2276,8 +2243,8 @@
       <c r="B31" t="s">
         <v>98</v>
       </c>
-      <c r="C31">
-        <v>5</v>
+      <c r="C31" s="6">
+        <v>4</v>
       </c>
       <c r="D31" s="6">
         <v>100</v>
@@ -2292,13 +2259,13 @@
         <v>7</v>
       </c>
       <c r="H31" t="s">
-        <v>174</v>
+        <v>263</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>260</v>
+        <v>231</v>
       </c>
       <c r="J31" t="s">
-        <v>235</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2308,8 +2275,8 @@
       <c r="B32" t="s">
         <v>99</v>
       </c>
-      <c r="C32">
-        <v>5</v>
+      <c r="C32" s="6">
+        <v>4</v>
       </c>
       <c r="D32" s="6">
         <v>100</v>
@@ -2321,13 +2288,13 @@
         <v>5</v>
       </c>
       <c r="G32" t="s">
-        <v>182</v>
-      </c>
-      <c r="H32" t="s">
-        <v>175</v>
+        <v>155</v>
+      </c>
+      <c r="H32">
+        <v>4</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>250</v>
+        <v>221</v>
       </c>
       <c r="J32" t="s">
         <v>127</v>
@@ -2340,8 +2307,8 @@
       <c r="B33" t="s">
         <v>71</v>
       </c>
-      <c r="C33">
-        <v>6</v>
+      <c r="C33" s="6">
+        <v>4</v>
       </c>
       <c r="D33" s="6">
         <v>100</v>
@@ -2353,10 +2320,10 @@
         <v>4</v>
       </c>
       <c r="H33" t="s">
-        <v>141</v>
+        <v>264</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>251</v>
+        <v>222</v>
       </c>
       <c r="J33" t="s">
         <v>125</v>
@@ -2369,8 +2336,8 @@
       <c r="B34" t="s">
         <v>100</v>
       </c>
-      <c r="C34">
-        <v>6</v>
+      <c r="C34" s="6">
+        <v>4</v>
       </c>
       <c r="D34" s="6">
         <v>100</v>
@@ -2385,10 +2352,10 @@
         <v>7</v>
       </c>
       <c r="H34" t="s">
-        <v>169</v>
+        <v>265</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>259</v>
+        <v>230</v>
       </c>
       <c r="J34" t="s">
         <v>128</v>
@@ -2401,8 +2368,8 @@
       <c r="B35" t="s">
         <v>101</v>
       </c>
-      <c r="C35">
-        <v>6</v>
+      <c r="C35" s="6">
+        <v>4</v>
       </c>
       <c r="D35" s="6">
         <v>100</v>
@@ -2414,10 +2381,10 @@
         <v>4</v>
       </c>
       <c r="H35" t="s">
-        <v>168</v>
+        <v>266</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>259</v>
+        <v>230</v>
       </c>
       <c r="J35" t="s">
         <v>128</v>
@@ -2430,8 +2397,8 @@
       <c r="B36" t="s">
         <v>102</v>
       </c>
-      <c r="C36">
-        <v>6</v>
+      <c r="C36" s="6">
+        <v>4</v>
       </c>
       <c r="D36" s="6">
         <v>100</v>
@@ -2443,7 +2410,7 @@
         <v>4</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>257</v>
+        <v>228</v>
       </c>
       <c r="J36" t="s">
         <v>129</v>
@@ -2456,8 +2423,8 @@
       <c r="B37" t="s">
         <v>103</v>
       </c>
-      <c r="C37">
-        <v>6</v>
+      <c r="C37" s="6">
+        <v>4</v>
       </c>
       <c r="D37" s="6">
         <v>100</v>
@@ -2469,7 +2436,7 @@
         <v>2</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>261</v>
+        <v>232</v>
       </c>
       <c r="J37" t="s">
         <v>130</v>
@@ -2482,8 +2449,8 @@
       <c r="B38" t="s">
         <v>117</v>
       </c>
-      <c r="C38">
-        <v>7</v>
+      <c r="C38" s="6">
+        <v>4</v>
       </c>
       <c r="D38" s="6">
         <v>100</v>
@@ -2497,11 +2464,11 @@
       <c r="G38">
         <v>25</v>
       </c>
-      <c r="H38" t="s">
-        <v>173</v>
+      <c r="H38">
+        <v>19</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>250</v>
+        <v>221</v>
       </c>
       <c r="J38" t="s">
         <v>131</v>
@@ -2514,8 +2481,8 @@
       <c r="B39" t="s">
         <v>118</v>
       </c>
-      <c r="C39">
-        <v>8</v>
+      <c r="C39" s="6">
+        <v>4</v>
       </c>
       <c r="D39" s="6">
         <v>100</v>
@@ -2527,7 +2494,7 @@
         <v>3</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>262</v>
+        <v>233</v>
       </c>
       <c r="J39" t="s">
         <v>132</v>
@@ -2540,8 +2507,8 @@
       <c r="B40" t="s">
         <v>119</v>
       </c>
-      <c r="C40">
-        <v>8</v>
+      <c r="C40" s="6">
+        <v>4</v>
       </c>
       <c r="D40" s="6">
         <v>100</v>
@@ -2553,10 +2520,10 @@
         <v>3</v>
       </c>
       <c r="H40" t="s">
-        <v>183</v>
+        <v>253</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="J40" t="s">
         <v>133</v>
@@ -2569,8 +2536,8 @@
       <c r="B41" t="s">
         <v>120</v>
       </c>
-      <c r="C41">
-        <v>8</v>
+      <c r="C41" s="6">
+        <v>4</v>
       </c>
       <c r="D41" s="6">
         <v>100</v>
@@ -2585,7 +2552,7 @@
         <v>18</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>262</v>
+        <v>233</v>
       </c>
       <c r="J41" t="s">
         <v>132</v>
@@ -2598,8 +2565,8 @@
       <c r="B42" t="s">
         <v>121</v>
       </c>
-      <c r="C42">
-        <v>9</v>
+      <c r="C42" s="6">
+        <v>4</v>
       </c>
       <c r="D42" s="6">
         <v>100</v>
@@ -2611,10 +2578,10 @@
         <v>2</v>
       </c>
       <c r="H42" t="s">
-        <v>179</v>
+        <v>267</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>261</v>
+        <v>232</v>
       </c>
       <c r="J42" t="s">
         <v>130</v>
@@ -2627,8 +2594,8 @@
       <c r="B43" t="s">
         <v>122</v>
       </c>
-      <c r="C43">
-        <v>9</v>
+      <c r="C43" s="6">
+        <v>4</v>
       </c>
       <c r="D43" s="6">
         <v>100</v>
@@ -2640,10 +2607,10 @@
         <v>2</v>
       </c>
       <c r="H43" t="s">
-        <v>167</v>
+        <v>268</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>264</v>
+        <v>234</v>
       </c>
       <c r="J43" t="s">
         <v>134</v>
@@ -2666,7 +2633,7 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="F8" sqref="F8:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2702,22 +2669,22 @@
         <v>137</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>187</v>
+        <v>158</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>189</v>
+        <v>160</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>190</v>
+        <v>161</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>209</v>
+        <v>180</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>210</v>
+        <v>181</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>277</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -2746,13 +2713,13 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>191</v>
+        <v>162</v>
       </c>
       <c r="J2" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="K2" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="L2" s="6">
         <v>0</v>
@@ -2784,13 +2751,13 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>192</v>
+        <v>163</v>
       </c>
       <c r="J3" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="K3" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="L3" s="6">
         <v>0</v>
@@ -2819,13 +2786,13 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>193</v>
+        <v>164</v>
       </c>
       <c r="J4" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="K4" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="L4" s="6">
         <v>0</v>
@@ -2854,13 +2821,13 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>194</v>
+        <v>165</v>
       </c>
       <c r="J5" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="K5" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="L5" s="4">
         <v>0</v>
@@ -2889,10 +2856,10 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>195</v>
+        <v>166</v>
       </c>
       <c r="K6" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="L6" s="4">
         <v>0</v>
@@ -2921,10 +2888,10 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>196</v>
+        <v>167</v>
       </c>
       <c r="K7" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="L7" s="4">
         <v>0</v>
@@ -2953,13 +2920,13 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>196</v>
+        <v>167</v>
       </c>
       <c r="J8" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="K8" t="s">
-        <v>212</v>
+        <v>183</v>
       </c>
       <c r="L8" s="4">
         <v>0</v>
@@ -2988,13 +2955,13 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>197</v>
+        <v>168</v>
       </c>
       <c r="J9" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="K9" t="s">
-        <v>212</v>
+        <v>183</v>
       </c>
       <c r="L9" s="4">
         <v>0</v>
@@ -3026,10 +2993,10 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>198</v>
+        <v>169</v>
       </c>
       <c r="J10" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>57</v>
@@ -3061,10 +3028,10 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>199</v>
+        <v>170</v>
       </c>
       <c r="J11" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="K11" s="6" t="s">
         <v>62</v>
@@ -3096,10 +3063,10 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>200</v>
+        <v>171</v>
       </c>
       <c r="J12" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>63</v>
@@ -3134,13 +3101,13 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>201</v>
+        <v>172</v>
       </c>
       <c r="J13">
         <v>3</v>
       </c>
       <c r="K13" t="s">
-        <v>213</v>
+        <v>184</v>
       </c>
       <c r="L13" s="4">
         <v>0</v>
@@ -3169,7 +3136,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>202</v>
+        <v>173</v>
       </c>
       <c r="J14">
         <v>2</v>
@@ -3207,13 +3174,13 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>203</v>
+        <v>174</v>
       </c>
       <c r="J15" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="K15" t="s">
-        <v>214</v>
+        <v>185</v>
       </c>
       <c r="L15" s="4">
         <v>0</v>
@@ -3245,13 +3212,13 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="J16" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="K16" t="s">
-        <v>215</v>
+        <v>186</v>
       </c>
       <c r="L16" s="4">
         <v>0</v>
@@ -3283,10 +3250,10 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>205</v>
+        <v>176</v>
       </c>
       <c r="J17" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="K17" s="6" t="s">
         <v>62</v>
@@ -3321,7 +3288,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>206</v>
+        <v>177</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -3359,13 +3326,13 @@
         <v>0</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>268</v>
+        <v>238</v>
       </c>
       <c r="L19" s="13">
         <v>0</v>
@@ -3373,10 +3340,10 @@
     </row>
     <row r="20" spans="1:12" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="11" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
       <c r="B20" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="C20" s="3">
         <v>0.33333333333333331</v>
@@ -3394,13 +3361,13 @@
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>269</v>
+        <v>239</v>
       </c>
       <c r="J20">
         <v>6</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="L20" s="4">
         <v>1</v>
@@ -3408,10 +3375,10 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="11" t="s">
-        <v>220</v>
+        <v>191</v>
       </c>
       <c r="B21" t="s">
-        <v>219</v>
+        <v>190</v>
       </c>
       <c r="C21" s="3">
         <v>0.33333333333333331</v>
@@ -3429,13 +3396,13 @@
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>270</v>
+        <v>240</v>
       </c>
       <c r="J21">
         <v>6</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="L21" s="4">
         <v>1</v>
@@ -3443,10 +3410,10 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="11" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
       <c r="B22" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="C22" s="3">
         <v>0.33333333333333331</v>
@@ -3464,13 +3431,13 @@
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>271</v>
+        <v>241</v>
       </c>
       <c r="J22">
         <v>6</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>212</v>
+        <v>183</v>
       </c>
       <c r="L22" s="4">
         <v>1</v>
@@ -3478,10 +3445,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="11" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="B23" t="s">
-        <v>224</v>
+        <v>195</v>
       </c>
       <c r="C23" s="3">
         <v>0.83333333333333337</v>
@@ -3499,13 +3466,13 @@
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>272</v>
+        <v>242</v>
       </c>
       <c r="J23">
         <v>6</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="L23" s="4">
         <v>1</v>
@@ -3513,10 +3480,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="11" t="s">
-        <v>226</v>
+        <v>197</v>
       </c>
       <c r="B24" t="s">
-        <v>225</v>
+        <v>196</v>
       </c>
       <c r="C24" s="3">
         <v>0.83333333333333337</v>
@@ -3534,13 +3501,13 @@
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>273</v>
+        <v>243</v>
       </c>
       <c r="J24">
         <v>6</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="L24" s="4">
         <v>1</v>
@@ -3548,10 +3515,10 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="11" t="s">
-        <v>227</v>
+        <v>198</v>
       </c>
       <c r="B25" t="s">
-        <v>228</v>
+        <v>199</v>
       </c>
       <c r="C25" s="3">
         <v>0.83333333333333337</v>
@@ -3569,13 +3536,13 @@
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>274</v>
+        <v>244</v>
       </c>
       <c r="J25">
         <v>6</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>212</v>
+        <v>183</v>
       </c>
       <c r="L25" s="4">
         <v>1</v>
@@ -3583,10 +3550,10 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="11" t="s">
-        <v>229</v>
+        <v>200</v>
       </c>
       <c r="B26" t="s">
-        <v>230</v>
+        <v>201</v>
       </c>
       <c r="C26" s="3">
         <v>0.33333333333333331</v>
@@ -3604,7 +3571,7 @@
         <v>1</v>
       </c>
       <c r="I26" t="s">
-        <v>275</v>
+        <v>245</v>
       </c>
       <c r="J26">
         <v>6</v>

</xml_diff>

<commit_message>
Added hamishi to weekend calculation
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omri3\Documents\Projects\Automated-shifts-assignment\DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Desktop\projects\Shibutzi\Automated-shifts-assignment\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B067AABC-9993-41A9-B125-6CA014522700}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="276">
   <si>
     <t>id</t>
   </si>
@@ -836,23 +835,44 @@
   </si>
   <si>
     <t>2,9,16,23</t>
+  </si>
+  <si>
+    <t>1,2,3,4</t>
+  </si>
+  <si>
+    <t>T26</t>
+  </si>
+  <si>
+    <t>Hamishi - bakut night 1</t>
+  </si>
+  <si>
+    <t>Hamishi - bakut night 2</t>
+  </si>
+  <si>
+    <t>Hamishi - equipment night</t>
+  </si>
+  <si>
+    <t>#2f4f2f</t>
+  </si>
+  <si>
+    <t>#6d8383</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -860,7 +880,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -957,7 +977,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -974,6 +994,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1287,28 +1308,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.3671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.62890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.3671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.89453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.47265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.89453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.26171875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="73.3671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="74.62890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="73.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="74.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1340,7 +1361,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1369,7 +1390,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1398,7 +1419,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1430,7 +1451,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1459,7 +1480,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1492,7 +1513,7 @@
       </c>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1524,7 +1545,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1556,7 +1577,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1588,7 +1609,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1620,7 +1641,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1631,7 +1652,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="6">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E11">
         <v>6</v>
@@ -1652,7 +1673,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1663,7 +1684,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="6">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E12">
         <v>6</v>
@@ -1681,7 +1702,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1692,7 +1713,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="6">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E13">
         <v>6</v>
@@ -1713,7 +1734,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1724,7 +1745,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="6">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E14">
         <v>6</v>
@@ -1745,7 +1766,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1753,10 +1774,10 @@
         <v>87</v>
       </c>
       <c r="C15" s="6">
-        <v>2</v>
-      </c>
-      <c r="D15">
-        <v>100</v>
+        <v>3</v>
+      </c>
+      <c r="D15" s="6">
+        <v>125</v>
       </c>
       <c r="E15">
         <v>4</v>
@@ -1774,7 +1795,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1782,10 +1803,10 @@
         <v>74</v>
       </c>
       <c r="C16" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16" s="6">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="E16">
         <v>4.5</v>
@@ -1806,7 +1827,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1814,10 +1835,10 @@
         <v>88</v>
       </c>
       <c r="C17" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17" s="6">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -1835,7 +1856,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1843,10 +1864,10 @@
         <v>75</v>
       </c>
       <c r="C18" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18" s="6">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="E18">
         <v>4</v>
@@ -1867,7 +1888,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1875,10 +1896,10 @@
         <v>89</v>
       </c>
       <c r="C19" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" s="6">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="E19">
         <v>4</v>
@@ -1899,7 +1920,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1907,10 +1928,10 @@
         <v>90</v>
       </c>
       <c r="C20" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D20" s="6">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="E20">
         <v>4</v>
@@ -1931,7 +1952,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -1939,7 +1960,7 @@
         <v>159</v>
       </c>
       <c r="C21" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D21" s="6">
         <v>0</v>
@@ -1957,7 +1978,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1965,10 +1986,10 @@
         <v>72</v>
       </c>
       <c r="C22" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D22" s="6">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -1989,7 +2010,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1997,10 +2018,10 @@
         <v>73</v>
       </c>
       <c r="C23" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D23" s="6">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="E23">
         <v>4</v>
@@ -2021,7 +2042,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2029,10 +2050,10 @@
         <v>91</v>
       </c>
       <c r="C24" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D24" s="6">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="E24">
         <v>4</v>
@@ -2050,7 +2071,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2058,10 +2079,10 @@
         <v>92</v>
       </c>
       <c r="C25" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D25" s="6">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="E25">
         <v>4</v>
@@ -2082,7 +2103,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2090,10 +2111,10 @@
         <v>93</v>
       </c>
       <c r="C26" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D26" s="6">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="E26">
         <v>4</v>
@@ -2111,7 +2132,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2119,10 +2140,10 @@
         <v>94</v>
       </c>
       <c r="C27" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D27" s="6">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="E27">
         <v>4</v>
@@ -2140,7 +2161,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
@@ -2148,10 +2169,10 @@
         <v>95</v>
       </c>
       <c r="C28" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D28" s="6">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="E28">
         <v>4</v>
@@ -2172,7 +2193,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2180,7 +2201,7 @@
         <v>96</v>
       </c>
       <c r="C29" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D29" s="6">
         <v>100</v>
@@ -2204,7 +2225,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2212,7 +2233,7 @@
         <v>97</v>
       </c>
       <c r="C30" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D30" s="6">
         <v>100</v>
@@ -2236,7 +2257,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>104</v>
       </c>
@@ -2244,7 +2265,7 @@
         <v>98</v>
       </c>
       <c r="C31" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D31" s="6">
         <v>100</v>
@@ -2268,7 +2289,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>105</v>
       </c>
@@ -2276,7 +2297,7 @@
         <v>99</v>
       </c>
       <c r="C32" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D32" s="6">
         <v>100</v>
@@ -2300,7 +2321,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>106</v>
       </c>
@@ -2308,7 +2329,7 @@
         <v>71</v>
       </c>
       <c r="C33" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D33" s="6">
         <v>100</v>
@@ -2329,7 +2350,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>107</v>
       </c>
@@ -2337,7 +2358,7 @@
         <v>100</v>
       </c>
       <c r="C34" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D34" s="6">
         <v>100</v>
@@ -2361,7 +2382,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>108</v>
       </c>
@@ -2369,7 +2390,7 @@
         <v>101</v>
       </c>
       <c r="C35" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D35" s="6">
         <v>100</v>
@@ -2390,7 +2411,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>109</v>
       </c>
@@ -2398,7 +2419,7 @@
         <v>102</v>
       </c>
       <c r="C36" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D36" s="6">
         <v>100</v>
@@ -2416,7 +2437,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>110</v>
       </c>
@@ -2424,7 +2445,7 @@
         <v>103</v>
       </c>
       <c r="C37" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D37" s="6">
         <v>100</v>
@@ -2442,7 +2463,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>111</v>
       </c>
@@ -2450,7 +2471,7 @@
         <v>117</v>
       </c>
       <c r="C38" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D38" s="6">
         <v>100</v>
@@ -2474,7 +2495,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>112</v>
       </c>
@@ -2482,7 +2503,7 @@
         <v>118</v>
       </c>
       <c r="C39" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D39" s="6">
         <v>100</v>
@@ -2500,7 +2521,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>113</v>
       </c>
@@ -2508,7 +2529,7 @@
         <v>119</v>
       </c>
       <c r="C40" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D40" s="6">
         <v>100</v>
@@ -2529,7 +2550,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>114</v>
       </c>
@@ -2537,7 +2558,7 @@
         <v>120</v>
       </c>
       <c r="C41" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D41" s="6">
         <v>100</v>
@@ -2558,7 +2579,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>115</v>
       </c>
@@ -2566,7 +2587,7 @@
         <v>121</v>
       </c>
       <c r="C42" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D42" s="6">
         <v>100</v>
@@ -2587,7 +2608,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>116</v>
       </c>
@@ -2595,7 +2616,7 @@
         <v>122</v>
       </c>
       <c r="C43" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D43" s="6">
         <v>100</v>
@@ -2616,12 +2637,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="I44" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L44" xr:uid="{EFBEFAD7-39D5-4626-81BE-F838DB4CBFA9}"/>
+  <autoFilter ref="A1:L44"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2629,27 +2650,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:F12"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27:F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.89453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.3671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.89453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.89453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.62890625" customWidth="1"/>
-    <col min="11" max="12" width="19.3671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.625" customWidth="1"/>
+    <col min="11" max="12" width="19.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2687,7 +2708,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>31</v>
       </c>
@@ -2725,7 +2746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>32</v>
       </c>
@@ -2763,7 +2784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>33</v>
       </c>
@@ -2789,7 +2810,7 @@
         <v>164</v>
       </c>
       <c r="J4" t="s">
-        <v>187</v>
+        <v>269</v>
       </c>
       <c r="K4" t="s">
         <v>182</v>
@@ -2798,7 +2819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>34</v>
       </c>
@@ -2824,7 +2845,7 @@
         <v>165</v>
       </c>
       <c r="J5" t="s">
-        <v>187</v>
+        <v>269</v>
       </c>
       <c r="K5" t="s">
         <v>182</v>
@@ -2833,7 +2854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>35</v>
       </c>
@@ -2865,7 +2886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>36</v>
       </c>
@@ -2897,7 +2918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>37</v>
       </c>
@@ -2932,7 +2953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>38</v>
       </c>
@@ -2958,7 +2979,7 @@
         <v>168</v>
       </c>
       <c r="J9" t="s">
-        <v>187</v>
+        <v>269</v>
       </c>
       <c r="K9" t="s">
         <v>183</v>
@@ -2967,7 +2988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>39</v>
       </c>
@@ -3005,7 +3026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>40</v>
       </c>
@@ -3040,7 +3061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>41</v>
       </c>
@@ -3075,7 +3096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>42</v>
       </c>
@@ -3113,7 +3134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>43</v>
       </c>
@@ -3148,7 +3169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>44</v>
       </c>
@@ -3186,7 +3207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>45</v>
       </c>
@@ -3224,7 +3245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>46</v>
       </c>
@@ -3262,7 +3283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>47</v>
       </c>
@@ -3300,7 +3321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>48</v>
       </c>
@@ -3338,7 +3359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>188</v>
       </c>
@@ -3373,7 +3394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>191</v>
       </c>
@@ -3408,7 +3429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>192</v>
       </c>
@@ -3443,7 +3464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>193</v>
       </c>
@@ -3478,7 +3499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>197</v>
       </c>
@@ -3513,7 +3534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>198</v>
       </c>
@@ -3548,7 +3569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>200</v>
       </c>
@@ -3583,19 +3604,139 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D27" s="4">
+        <v>24</v>
+      </c>
+      <c r="F27" s="4">
+        <v>25</v>
+      </c>
+      <c r="G27" s="4">
+        <v>1</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="J27">
+        <v>5</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="L27" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D28" s="4">
+        <v>24</v>
+      </c>
+      <c r="F28" s="4">
+        <v>25</v>
+      </c>
+      <c r="G28" s="4">
+        <v>1</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="J28">
+        <v>5</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="L28" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D29" s="4">
+        <v>24</v>
+      </c>
+      <c r="F29" s="4">
+        <v>25</v>
+      </c>
+      <c r="G29" s="4">
+        <v>1</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0</v>
+      </c>
+      <c r="I29" t="s">
+        <v>275</v>
+      </c>
+      <c r="J29">
+        <v>5</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="L29" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E36" s="5"/>
     </row>
-    <row r="1048576" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C1048576" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added max nights constraint
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555" activeTab="1"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="278">
   <si>
     <t>id</t>
   </si>
@@ -36,9 +36,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>O1</t>
-  </si>
-  <si>
     <t>O2</t>
   </si>
   <si>
@@ -856,6 +853,15 @@
   </si>
   <si>
     <t>#6d8383</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C+A2+I3:K3+I3:L3</t>
+  </si>
+  <si>
+    <t>MAX_nights</t>
   </si>
 </sst>
 </file>
@@ -1311,8 +1317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="J12" sqref="A1:J12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1323,10 +1329,11 @@
     <col min="4" max="4" width="15.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="73.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="74.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.375" customWidth="1"/>
+    <col min="8" max="8" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="73.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="74.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -1337,36 +1344,39 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1" t="s">
         <v>135</v>
       </c>
-      <c r="F1" t="s">
-        <v>136</v>
-      </c>
       <c r="G1" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I1" t="s">
         <v>156</v>
       </c>
-      <c r="H1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="J1" t="s">
-        <v>179</v>
+      <c r="J1" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="K1" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>275</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1380,22 +1390,25 @@
       <c r="F2">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
-        <v>249</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="J2" t="s">
-        <v>207</v>
+      <c r="G2" s="6">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>248</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="K2" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1409,22 +1422,25 @@
       <c r="F3">
         <v>14</v>
       </c>
-      <c r="H3">
+      <c r="G3" s="6">
+        <v>10</v>
+      </c>
+      <c r="I3">
         <v>8</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="J3" t="s">
-        <v>207</v>
+      <c r="J3" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="K3" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1438,25 +1454,28 @@
       <c r="F4">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
-        <v>147</v>
-      </c>
-      <c r="H4">
+      <c r="G4" s="6">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>146</v>
+      </c>
+      <c r="I4">
         <v>5</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="J4" t="s">
-        <v>207</v>
+      <c r="J4" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="K4" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1470,22 +1489,25 @@
       <c r="F5">
         <v>14</v>
       </c>
-      <c r="G5" t="s">
-        <v>149</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="J5" t="s">
-        <v>208</v>
+      <c r="G5" s="6">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>148</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="K5" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1499,26 +1521,29 @@
       <c r="F6">
         <v>14</v>
       </c>
-      <c r="G6" t="s">
-        <v>148</v>
+      <c r="G6" s="6">
+        <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>249</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="J6" t="s">
-        <v>204</v>
+        <v>147</v>
+      </c>
+      <c r="I6" t="s">
+        <v>248</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="K6" t="s">
+        <v>203</v>
       </c>
       <c r="L6" s="5"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1532,25 +1557,28 @@
       <c r="F7">
         <v>14</v>
       </c>
-      <c r="G7" t="s">
-        <v>150</v>
+      <c r="G7" s="6">
+        <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>250</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="J7" t="s">
-        <v>205</v>
+        <v>149</v>
+      </c>
+      <c r="I7" t="s">
+        <v>249</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="K7" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1564,25 +1592,28 @@
       <c r="F8">
         <v>14</v>
       </c>
-      <c r="G8" t="s">
-        <v>146</v>
+      <c r="G8" s="6">
+        <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>249</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="J8" t="s">
-        <v>207</v>
+        <v>145</v>
+      </c>
+      <c r="I8" t="s">
+        <v>248</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="K8" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1596,25 +1627,28 @@
       <c r="F9">
         <v>14</v>
       </c>
-      <c r="G9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H9">
+      <c r="G9" s="6">
+        <v>10</v>
+      </c>
+      <c r="H9" t="s">
+        <v>143</v>
+      </c>
+      <c r="I9">
         <v>5</v>
       </c>
-      <c r="I9" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="J9" t="s">
-        <v>207</v>
+      <c r="J9" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="K9" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1628,25 +1662,28 @@
       <c r="F10">
         <v>14</v>
       </c>
-      <c r="G10" t="s">
-        <v>145</v>
+      <c r="G10" s="6">
+        <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>251</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="J10" t="s">
-        <v>207</v>
+        <v>144</v>
+      </c>
+      <c r="I10" t="s">
+        <v>250</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="K10" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="6">
         <v>2</v>
@@ -1660,25 +1697,28 @@
       <c r="F11">
         <v>12</v>
       </c>
-      <c r="G11" t="s">
-        <v>143</v>
+      <c r="G11" s="6">
+        <v>8</v>
       </c>
       <c r="H11" t="s">
-        <v>252</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="J11" t="s">
-        <v>207</v>
+        <v>142</v>
+      </c>
+      <c r="I11" t="s">
+        <v>251</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="K11" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="6">
         <v>2</v>
@@ -1692,22 +1732,25 @@
       <c r="F12">
         <v>12</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="6">
+        <v>8</v>
+      </c>
+      <c r="H12">
         <v>23</v>
       </c>
-      <c r="I12" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="J12" t="s">
-        <v>207</v>
+      <c r="J12" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="K12" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="6">
         <v>2</v>
@@ -1721,25 +1764,28 @@
       <c r="F13">
         <v>12</v>
       </c>
-      <c r="G13" t="s">
-        <v>151</v>
+      <c r="G13" s="6">
+        <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>251</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="J13" t="s">
-        <v>204</v>
+        <v>150</v>
+      </c>
+      <c r="I13" t="s">
+        <v>250</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="K13" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C14" s="6">
         <v>2</v>
@@ -1753,25 +1799,28 @@
       <c r="F14">
         <v>12</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="6">
+        <v>8</v>
+      </c>
+      <c r="H14">
         <v>23</v>
       </c>
-      <c r="H14" t="s">
-        <v>253</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="J14" t="s">
-        <v>209</v>
+      <c r="I14" t="s">
+        <v>252</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="K14" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C15" s="6">
         <v>3</v>
@@ -1785,22 +1834,25 @@
       <c r="F15">
         <v>8</v>
       </c>
-      <c r="H15" t="s">
-        <v>254</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="J15" t="s">
-        <v>210</v>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>253</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="K15" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C16" s="6">
         <v>3</v>
@@ -1814,25 +1866,28 @@
       <c r="F16">
         <v>8</v>
       </c>
-      <c r="G16" t="s">
-        <v>142</v>
+      <c r="G16">
+        <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>255</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="J16" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+      <c r="I16" t="s">
+        <v>254</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="K16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C17" s="6">
         <v>3</v>
@@ -1846,22 +1901,25 @@
       <c r="F17">
         <v>8</v>
       </c>
-      <c r="H17" t="s">
-        <v>256</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="J17" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>255</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="K17" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" s="6">
         <v>3</v>
@@ -1875,25 +1933,28 @@
       <c r="F18">
         <v>8</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="6">
+        <v>0</v>
+      </c>
+      <c r="H18">
         <v>8</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>9</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="J18" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J18" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="K18" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C19" s="6">
         <v>3</v>
@@ -1907,25 +1968,28 @@
       <c r="F19">
         <v>8</v>
       </c>
-      <c r="G19" t="s">
-        <v>144</v>
+      <c r="G19" s="6">
+        <v>8</v>
       </c>
       <c r="H19" t="s">
-        <v>254</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="J19" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+      <c r="I19" t="s">
+        <v>253</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="K19" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C20" s="6">
         <v>3</v>
@@ -1939,25 +2003,28 @@
       <c r="F20">
         <v>8</v>
       </c>
-      <c r="G20" t="s">
-        <v>152</v>
+      <c r="G20" s="6">
+        <v>8</v>
       </c>
       <c r="H20" t="s">
-        <v>257</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="J20" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+      <c r="I20" t="s">
+        <v>256</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="K20" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C21" s="6">
         <v>4</v>
@@ -1971,19 +2038,22 @@
       <c r="F21">
         <v>2</v>
       </c>
-      <c r="I21" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="J21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G21" s="6">
+        <v>0</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="K21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C22" s="6">
         <v>4</v>
@@ -1998,24 +2068,27 @@
         <v>8</v>
       </c>
       <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
         <v>10</v>
       </c>
-      <c r="H22" t="s">
-        <v>258</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="J22" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I22" t="s">
+        <v>257</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="K22" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23" s="6">
         <v>4</v>
@@ -2029,25 +2102,28 @@
       <c r="F23">
         <v>8</v>
       </c>
-      <c r="G23" t="s">
-        <v>141</v>
+      <c r="G23">
+        <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>259</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="J23" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+      <c r="I23" t="s">
+        <v>258</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="K23" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24" s="6">
         <v>4</v>
@@ -2059,24 +2135,27 @@
         <v>4</v>
       </c>
       <c r="F24">
-        <v>8</v>
-      </c>
-      <c r="H24" t="s">
-        <v>260</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="J24" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="G24" s="6">
+        <v>4</v>
+      </c>
+      <c r="I24" t="s">
+        <v>259</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="K24" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C25" s="6">
         <v>4</v>
@@ -2088,27 +2167,30 @@
         <v>4</v>
       </c>
       <c r="F25">
-        <v>8</v>
-      </c>
-      <c r="G25" t="s">
-        <v>153</v>
-      </c>
-      <c r="H25">
+        <v>6</v>
+      </c>
+      <c r="G25" s="6">
+        <v>4</v>
+      </c>
+      <c r="H25" t="s">
+        <v>152</v>
+      </c>
+      <c r="I25">
         <v>23</v>
       </c>
-      <c r="I25" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="J25" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J25" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="K25" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C26" s="6">
         <v>4</v>
@@ -2120,24 +2202,27 @@
         <v>4</v>
       </c>
       <c r="F26">
+        <v>6</v>
+      </c>
+      <c r="G26" s="6">
+        <v>4</v>
+      </c>
+      <c r="I26">
         <v>8</v>
       </c>
-      <c r="H26">
-        <v>8</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="J26" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J26" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="K26" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C27" s="6">
         <v>4</v>
@@ -2149,24 +2234,27 @@
         <v>4</v>
       </c>
       <c r="F27">
-        <v>8</v>
-      </c>
-      <c r="H27">
+        <v>6</v>
+      </c>
+      <c r="G27" s="6">
+        <v>4</v>
+      </c>
+      <c r="I27">
         <v>30</v>
       </c>
-      <c r="I27" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="J27" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J27" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="K27" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C28" s="6">
         <v>4</v>
@@ -2178,27 +2266,30 @@
         <v>4</v>
       </c>
       <c r="F28">
-        <v>8</v>
-      </c>
-      <c r="G28">
+        <v>6</v>
+      </c>
+      <c r="G28" s="6">
+        <v>4</v>
+      </c>
+      <c r="H28">
         <v>10</v>
       </c>
-      <c r="H28" t="s">
-        <v>261</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="J28" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I28" t="s">
+        <v>260</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="K28" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C29" s="6">
         <v>5</v>
@@ -2212,25 +2303,28 @@
       <c r="F29">
         <v>5</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="6">
+        <v>2</v>
+      </c>
+      <c r="H29">
         <v>7</v>
       </c>
-      <c r="H29" t="s">
-        <v>262</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="J29" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I29" t="s">
+        <v>261</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="K29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C30" s="6">
         <v>5</v>
@@ -2244,25 +2338,28 @@
       <c r="F30">
         <v>5</v>
       </c>
-      <c r="G30" t="s">
-        <v>154</v>
-      </c>
-      <c r="H30">
+      <c r="G30" s="6">
+        <v>2</v>
+      </c>
+      <c r="H30" t="s">
+        <v>153</v>
+      </c>
+      <c r="I30">
         <v>28</v>
       </c>
-      <c r="I30" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="J30" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J30" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="K30" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C31" s="6">
         <v>5</v>
@@ -2276,25 +2373,28 @@
       <c r="F31">
         <v>5</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="6">
+        <v>2</v>
+      </c>
+      <c r="H31">
         <v>7</v>
       </c>
-      <c r="H31" t="s">
-        <v>263</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="J31" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I31" t="s">
+        <v>262</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="K31" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C32" s="6">
         <v>5</v>
@@ -2308,25 +2408,28 @@
       <c r="F32">
         <v>5</v>
       </c>
-      <c r="G32" t="s">
-        <v>155</v>
-      </c>
-      <c r="H32">
+      <c r="G32" s="6">
+        <v>0</v>
+      </c>
+      <c r="H32" t="s">
+        <v>154</v>
+      </c>
+      <c r="I32">
         <v>4</v>
       </c>
-      <c r="I32" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="J32" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J32" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="K32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C33" s="6">
         <v>6</v>
@@ -2340,22 +2443,25 @@
       <c r="F33">
         <v>4</v>
       </c>
-      <c r="H33" t="s">
-        <v>264</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="J33" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="I33" t="s">
+        <v>263</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="K33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C34" s="6">
         <v>6</v>
@@ -2370,24 +2476,27 @@
         <v>4</v>
       </c>
       <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
         <v>7</v>
       </c>
-      <c r="H34" t="s">
-        <v>265</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="J34" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I34" t="s">
+        <v>264</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="K34" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C35" s="6">
         <v>6</v>
@@ -2401,22 +2510,25 @@
       <c r="F35">
         <v>4</v>
       </c>
-      <c r="H35" t="s">
-        <v>266</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="J35" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="I35" t="s">
+        <v>265</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="K35" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C36" s="6">
         <v>6</v>
@@ -2430,19 +2542,22 @@
       <c r="F36">
         <v>4</v>
       </c>
-      <c r="I36" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="J36" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="K36" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C37" s="6">
         <v>6</v>
@@ -2456,19 +2571,22 @@
       <c r="F37">
         <v>2</v>
       </c>
-      <c r="I37" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="J37" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="K37" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C38" s="6">
         <v>6</v>
@@ -2483,24 +2601,27 @@
         <v>3</v>
       </c>
       <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
         <v>25</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <v>19</v>
       </c>
-      <c r="I38" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="J38" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J38" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="K38" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C39" s="6">
         <v>6</v>
@@ -2514,19 +2635,22 @@
       <c r="F39">
         <v>3</v>
       </c>
-      <c r="I39" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="J39" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="K39" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C40" s="6">
         <v>6</v>
@@ -2540,22 +2664,25 @@
       <c r="F40">
         <v>3</v>
       </c>
-      <c r="H40" t="s">
-        <v>253</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="J40" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="I40" t="s">
+        <v>252</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="K40" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B41" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C41" s="6">
         <v>6</v>
@@ -2570,21 +2697,24 @@
         <v>3</v>
       </c>
       <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
         <v>18</v>
       </c>
-      <c r="I41" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="J41" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J41" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="K41" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C42" s="6">
         <v>6</v>
@@ -2598,22 +2728,25 @@
       <c r="F42">
         <v>2</v>
       </c>
-      <c r="H42" t="s">
-        <v>267</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="J42" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="I42" t="s">
+        <v>266</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="K42" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C43" s="6">
         <v>6</v>
@@ -2627,19 +2760,22 @@
       <c r="F43">
         <v>2</v>
       </c>
-      <c r="H43" t="s">
-        <v>268</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="J43" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="I43" t="s">
+        <v>267</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="K43" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
-      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L44"/>
@@ -2653,8 +2789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K1:K29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="A4:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2678,42 +2814,42 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>140</v>
-      </c>
       <c r="F1" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="I1" s="7" t="s">
-        <v>161</v>
-      </c>
       <c r="J1" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="K1" s="7" t="s">
-        <v>181</v>
-      </c>
       <c r="L1" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="3">
         <v>0.33333333333333331</v>
@@ -2722,7 +2858,7 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -2734,13 +2870,13 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L2" s="6">
         <v>0</v>
@@ -2748,10 +2884,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="3">
         <v>0.33333333333333331</v>
@@ -2760,7 +2896,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -2772,13 +2908,13 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L3" s="6">
         <v>0</v>
@@ -2786,10 +2922,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="3">
         <v>0.83333333333333337</v>
@@ -2807,13 +2943,13 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L4" s="6">
         <v>0</v>
@@ -2821,10 +2957,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="3">
         <v>0.83333333333333337</v>
@@ -2842,13 +2978,13 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L5" s="4">
         <v>0</v>
@@ -2856,10 +2992,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="3">
         <v>0.33333333333333331</v>
@@ -2877,10 +3013,10 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L6" s="4">
         <v>0</v>
@@ -2888,10 +3024,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="3">
         <v>0.83333333333333337</v>
@@ -2909,10 +3045,10 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L7" s="4">
         <v>0</v>
@@ -2920,10 +3056,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="3">
         <v>0.33333333333333331</v>
@@ -2941,13 +3077,13 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L8" s="4">
         <v>0</v>
@@ -2955,10 +3091,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="3">
         <v>0.83333333333333337</v>
@@ -2976,13 +3112,13 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L9" s="4">
         <v>0</v>
@@ -2990,10 +3126,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="3">
         <v>0.33333333333333331</v>
@@ -3002,7 +3138,7 @@
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F10">
         <v>0.5</v>
@@ -3014,13 +3150,13 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L10" s="4">
         <v>0</v>
@@ -3028,10 +3164,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" s="3">
         <v>0.33333333333333331</v>
@@ -3049,13 +3185,13 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L11" s="4">
         <v>0</v>
@@ -3063,10 +3199,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="3">
         <v>0.33333333333333331</v>
@@ -3084,13 +3220,13 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L12" s="4">
         <v>0</v>
@@ -3098,10 +3234,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" s="3">
         <v>0.33333333333333331</v>
@@ -3110,7 +3246,7 @@
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F13">
         <v>0.25</v>
@@ -3122,13 +3258,13 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J13">
         <v>3</v>
       </c>
       <c r="K13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L13" s="4">
         <v>0</v>
@@ -3136,10 +3272,10 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" s="3">
         <v>0.33333333333333331</v>
@@ -3157,13 +3293,13 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J14">
         <v>2</v>
       </c>
       <c r="K14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L14" s="4">
         <v>0</v>
@@ -3171,10 +3307,10 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="3">
         <v>0.33333333333333331</v>
@@ -3183,7 +3319,7 @@
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F15">
         <v>0.25</v>
@@ -3195,13 +3331,13 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L15" s="4">
         <v>0</v>
@@ -3209,10 +3345,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="3">
         <v>0.33333333333333331</v>
@@ -3221,7 +3357,7 @@
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F16">
         <v>0.25</v>
@@ -3233,13 +3369,13 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L16" s="4">
         <v>0</v>
@@ -3247,10 +3383,10 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C17" s="3">
         <v>0.33333333333333331</v>
@@ -3259,7 +3395,7 @@
         <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F17">
         <v>0.25</v>
@@ -3271,13 +3407,13 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L17" s="4">
         <v>0</v>
@@ -3285,10 +3421,10 @@
     </row>
     <row r="18" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" s="3">
         <v>0.33333333333333331</v>
@@ -3297,7 +3433,7 @@
         <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F18">
         <v>0.25</v>
@@ -3309,13 +3445,13 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J18">
         <v>1</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L18" s="4">
         <v>0</v>
@@ -3323,10 +3459,10 @@
     </row>
     <row r="19" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" s="15">
         <v>0.33333333333333331</v>
@@ -3335,7 +3471,7 @@
         <v>9</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19" s="13">
         <v>0.25</v>
@@ -3347,13 +3483,13 @@
         <v>0</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L19" s="13">
         <v>0</v>
@@ -3361,10 +3497,10 @@
     </row>
     <row r="20" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="B20" t="s">
         <v>188</v>
-      </c>
-      <c r="B20" t="s">
-        <v>189</v>
       </c>
       <c r="C20" s="3">
         <v>0.33333333333333331</v>
@@ -3382,13 +3518,13 @@
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J20">
         <v>6</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L20" s="4">
         <v>1</v>
@@ -3396,10 +3532,10 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C21" s="3">
         <v>0.33333333333333331</v>
@@ -3417,13 +3553,13 @@
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J21">
         <v>6</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L21" s="4">
         <v>1</v>
@@ -3431,10 +3567,10 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C22" s="3">
         <v>0.33333333333333331</v>
@@ -3452,13 +3588,13 @@
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J22">
         <v>6</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L22" s="4">
         <v>1</v>
@@ -3466,10 +3602,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C23" s="3">
         <v>0.83333333333333337</v>
@@ -3487,13 +3623,13 @@
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J23">
         <v>6</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L23" s="4">
         <v>1</v>
@@ -3501,10 +3637,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C24" s="3">
         <v>0.83333333333333337</v>
@@ -3522,13 +3658,13 @@
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J24">
         <v>6</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L24" s="4">
         <v>1</v>
@@ -3536,10 +3672,10 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="B25" t="s">
         <v>198</v>
-      </c>
-      <c r="B25" t="s">
-        <v>199</v>
       </c>
       <c r="C25" s="3">
         <v>0.83333333333333337</v>
@@ -3557,13 +3693,13 @@
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J25">
         <v>6</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L25" s="4">
         <v>1</v>
@@ -3571,10 +3707,10 @@
     </row>
     <row r="26" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="B26" t="s">
         <v>200</v>
-      </c>
-      <c r="B26" t="s">
-        <v>201</v>
       </c>
       <c r="C26" s="3">
         <v>0.33333333333333331</v>
@@ -3592,13 +3728,13 @@
         <v>1</v>
       </c>
       <c r="I26" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J26">
         <v>6</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L26" s="4">
         <v>1</v>
@@ -3606,10 +3742,10 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>270</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>271</v>
       </c>
       <c r="C27" s="3">
         <v>0.83333333333333337</v>
@@ -3627,13 +3763,13 @@
         <v>0</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J27">
         <v>5</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L27" s="4">
         <v>1</v>
@@ -3641,10 +3777,10 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C28" s="3">
         <v>0.83333333333333337</v>
@@ -3662,13 +3798,13 @@
         <v>0</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J28">
         <v>5</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L28" s="4">
         <v>1</v>
@@ -3676,10 +3812,10 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C29" s="3">
         <v>0.83333333333333337</v>
@@ -3697,13 +3833,13 @@
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J29">
         <v>5</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L29" s="4">
         <v>1</v>

</xml_diff>

<commit_message>
added not evening stats
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Desktop\projects\Shibutzi\Automated-shifts-assignment\DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitza\Desktop\automated shifts assignment\Automated-shifts-assignment\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532E5357-7F95-477A-8A50-4ADB0D8055ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="277">
   <si>
     <t>id</t>
   </si>
@@ -856,23 +857,26 @@
   </si>
   <si>
     <t>#6d8383</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -880,7 +884,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1308,28 +1312,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="J12" sqref="A1:J12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="73.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="74.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="73.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="74.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1361,7 +1365,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1390,7 +1394,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1409,6 +1413,9 @@
       <c r="F3">
         <v>14</v>
       </c>
+      <c r="G3" t="s">
+        <v>276</v>
+      </c>
       <c r="H3">
         <v>8</v>
       </c>
@@ -1419,7 +1426,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1451,7 +1458,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1480,7 +1487,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1513,7 +1520,7 @@
       </c>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1545,7 +1552,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1577,7 +1584,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1609,7 +1616,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1641,7 +1648,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1673,7 +1680,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1702,7 +1709,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1734,7 +1741,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1766,7 +1773,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1795,7 +1802,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1827,7 +1834,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1856,7 +1863,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1888,7 +1895,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1920,7 +1927,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1952,7 +1959,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -1978,7 +1985,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2010,7 +2017,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2042,7 +2049,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2071,7 +2078,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2103,7 +2110,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2132,7 +2139,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2161,7 +2168,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
@@ -2193,7 +2200,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2225,7 +2232,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2257,7 +2264,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>104</v>
       </c>
@@ -2289,7 +2296,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>105</v>
       </c>
@@ -2321,7 +2328,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>106</v>
       </c>
@@ -2350,7 +2357,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>107</v>
       </c>
@@ -2382,7 +2389,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>108</v>
       </c>
@@ -2411,7 +2418,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>109</v>
       </c>
@@ -2437,7 +2444,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>110</v>
       </c>
@@ -2463,7 +2470,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>111</v>
       </c>
@@ -2495,7 +2502,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>112</v>
       </c>
@@ -2521,7 +2528,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>113</v>
       </c>
@@ -2550,7 +2557,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>114</v>
       </c>
@@ -2579,7 +2586,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>115</v>
       </c>
@@ -2608,7 +2615,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>116</v>
       </c>
@@ -2637,12 +2644,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="I44" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L44"/>
+  <autoFilter ref="A1:L44" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2650,27 +2657,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K29" sqref="K1:K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.625" customWidth="1"/>
-    <col min="11" max="12" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="11" max="12" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2708,7 +2715,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>31</v>
       </c>
@@ -2746,7 +2753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>32</v>
       </c>
@@ -2784,7 +2791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>33</v>
       </c>
@@ -2819,7 +2826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>34</v>
       </c>
@@ -2854,7 +2861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>35</v>
       </c>
@@ -2886,7 +2893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>36</v>
       </c>
@@ -2918,7 +2925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>37</v>
       </c>
@@ -2953,7 +2960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>38</v>
       </c>
@@ -2988,7 +2995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>39</v>
       </c>
@@ -3026,7 +3033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>40</v>
       </c>
@@ -3061,7 +3068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>41</v>
       </c>
@@ -3096,7 +3103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>42</v>
       </c>
@@ -3134,7 +3141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>43</v>
       </c>
@@ -3169,7 +3176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>44</v>
       </c>
@@ -3207,7 +3214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>45</v>
       </c>
@@ -3245,7 +3252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>46</v>
       </c>
@@ -3283,7 +3290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>47</v>
       </c>
@@ -3321,7 +3328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>48</v>
       </c>
@@ -3359,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>188</v>
       </c>
@@ -3394,7 +3401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>191</v>
       </c>
@@ -3429,7 +3436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>192</v>
       </c>
@@ -3464,7 +3471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>193</v>
       </c>
@@ -3499,7 +3506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>197</v>
       </c>
@@ -3534,7 +3541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>198</v>
       </c>
@@ -3569,7 +3576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>200</v>
       </c>
@@ -3604,7 +3611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
         <v>270</v>
       </c>
@@ -3639,7 +3646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
         <v>270</v>
       </c>
@@ -3674,7 +3681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
         <v>270</v>
       </c>
@@ -3709,34 +3716,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E36" s="5"/>
     </row>
-    <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="1048576" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1048576" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add cool stats (#24)
* added capacity stats

* added not evening stats

* fixed excel
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Desktop\projects\Shibutzi\Automated-shifts-assignment\DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitza\Desktop\automated shifts assignment\Automated-shifts-assignment\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFD33C2-C835-488D-AE34-8D93746FB0AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="277">
   <si>
     <t>id</t>
   </si>
@@ -735,9 +736,6 @@
     <t>pazam</t>
   </si>
   <si>
-    <t xml:space="preserve"> CLANING THE TAHAK, bakut, equipment, ftt, marzuk, equip oper, bakut oper , </t>
-  </si>
-  <si>
     <t>RC</t>
   </si>
   <si>
@@ -855,30 +853,30 @@
     <t>#6d8383</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> C+A2+I3:K3+I3:L3</t>
-  </si>
-  <si>
     <t>MAX_nights</t>
+  </si>
+  <si>
+    <t>O1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CLANING THE TAHAK, bakut, equipment, ftt, marzuk, equip oper, bakut oper</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -886,7 +884,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1314,29 +1312,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.375" customWidth="1"/>
-    <col min="8" max="8" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="73.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="74.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="73.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="74.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1347,7 +1345,7 @@
         <v>234</v>
       </c>
       <c r="D1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E1" t="s">
         <v>134</v>
@@ -1356,7 +1354,7 @@
         <v>135</v>
       </c>
       <c r="G1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H1" t="s">
         <v>155</v>
@@ -1371,7 +1369,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>275</v>
       </c>
@@ -1394,16 +1392,16 @@
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>235</v>
+        <v>276</v>
       </c>
       <c r="K2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1429,13 +1427,13 @@
         <v>8</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>276</v>
+        <v>218</v>
       </c>
       <c r="K3" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1470,7 +1468,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1502,12 +1500,12 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1528,7 +1526,7 @@
         <v>147</v>
       </c>
       <c r="I6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>219</v>
@@ -1538,7 +1536,7 @@
       </c>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1564,7 +1562,7 @@
         <v>149</v>
       </c>
       <c r="I7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>219</v>
@@ -1573,7 +1571,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1599,7 +1597,7 @@
         <v>145</v>
       </c>
       <c r="I8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>218</v>
@@ -1608,7 +1606,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1643,7 +1641,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1669,7 +1667,7 @@
         <v>144</v>
       </c>
       <c r="I10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>218</v>
@@ -1678,7 +1676,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1704,7 +1702,7 @@
         <v>142</v>
       </c>
       <c r="I11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>218</v>
@@ -1713,7 +1711,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1745,7 +1743,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1771,7 +1769,7 @@
         <v>150</v>
       </c>
       <c r="I13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>219</v>
@@ -1780,7 +1778,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1806,7 +1804,7 @@
         <v>23</v>
       </c>
       <c r="I14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>220</v>
@@ -1815,7 +1813,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1838,7 +1836,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>221</v>
@@ -1847,7 +1845,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1873,7 +1871,7 @@
         <v>141</v>
       </c>
       <c r="I16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>222</v>
@@ -1882,7 +1880,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1905,7 +1903,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>223</v>
@@ -1914,7 +1912,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1949,7 +1947,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1975,7 +1973,7 @@
         <v>143</v>
       </c>
       <c r="I19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>224</v>
@@ -1984,7 +1982,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2010,7 +2008,7 @@
         <v>151</v>
       </c>
       <c r="I20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>221</v>
@@ -2019,7 +2017,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -2048,7 +2046,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2074,7 +2072,7 @@
         <v>10</v>
       </c>
       <c r="I22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>221</v>
@@ -2083,7 +2081,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2109,7 +2107,7 @@
         <v>140</v>
       </c>
       <c r="I23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>226</v>
@@ -2118,7 +2116,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2141,7 +2139,7 @@
         <v>4</v>
       </c>
       <c r="I24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>227</v>
@@ -2150,7 +2148,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2185,7 +2183,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2217,7 +2215,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2249,7 +2247,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -2275,7 +2273,7 @@
         <v>10</v>
       </c>
       <c r="I28" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>221</v>
@@ -2284,7 +2282,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2310,7 +2308,7 @@
         <v>7</v>
       </c>
       <c r="I29" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>228</v>
@@ -2319,7 +2317,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2354,7 +2352,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>103</v>
       </c>
@@ -2380,7 +2378,7 @@
         <v>7</v>
       </c>
       <c r="I31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>230</v>
@@ -2389,7 +2387,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>104</v>
       </c>
@@ -2424,7 +2422,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>105</v>
       </c>
@@ -2447,7 +2445,7 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>221</v>
@@ -2456,7 +2454,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>106</v>
       </c>
@@ -2482,7 +2480,7 @@
         <v>7</v>
       </c>
       <c r="I34" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>229</v>
@@ -2491,7 +2489,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>107</v>
       </c>
@@ -2514,7 +2512,7 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J35" s="5" t="s">
         <v>229</v>
@@ -2523,7 +2521,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>108</v>
       </c>
@@ -2552,7 +2550,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>109</v>
       </c>
@@ -2581,7 +2579,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>110</v>
       </c>
@@ -2616,7 +2614,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>111</v>
       </c>
@@ -2645,7 +2643,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>112</v>
       </c>
@@ -2668,16 +2666,16 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K40" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>113</v>
       </c>
@@ -2709,7 +2707,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>114</v>
       </c>
@@ -2732,7 +2730,7 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J42" s="5" t="s">
         <v>231</v>
@@ -2741,7 +2739,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>115</v>
       </c>
@@ -2764,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J43" s="5" t="s">
         <v>233</v>
@@ -2773,12 +2771,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="J44" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L44"/>
+  <autoFilter ref="A1:L44" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2786,27 +2784,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="A4:G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.625" customWidth="1"/>
-    <col min="11" max="12" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="11" max="12" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2841,10 +2839,10 @@
         <v>180</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>30</v>
       </c>
@@ -2882,7 +2880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>31</v>
       </c>
@@ -2920,7 +2918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>32</v>
       </c>
@@ -2946,7 +2944,7 @@
         <v>163</v>
       </c>
       <c r="J4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K4" t="s">
         <v>181</v>
@@ -2955,7 +2953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>33</v>
       </c>
@@ -2981,7 +2979,7 @@
         <v>164</v>
       </c>
       <c r="J5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K5" t="s">
         <v>181</v>
@@ -2990,7 +2988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>34</v>
       </c>
@@ -3022,7 +3020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>35</v>
       </c>
@@ -3054,7 +3052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>36</v>
       </c>
@@ -3089,7 +3087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>37</v>
       </c>
@@ -3115,7 +3113,7 @@
         <v>167</v>
       </c>
       <c r="J9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K9" t="s">
         <v>182</v>
@@ -3124,7 +3122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>38</v>
       </c>
@@ -3162,7 +3160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>39</v>
       </c>
@@ -3197,7 +3195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>40</v>
       </c>
@@ -3232,7 +3230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>41</v>
       </c>
@@ -3270,7 +3268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>42</v>
       </c>
@@ -3305,7 +3303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>43</v>
       </c>
@@ -3343,7 +3341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>44</v>
       </c>
@@ -3381,7 +3379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>45</v>
       </c>
@@ -3419,7 +3417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>46</v>
       </c>
@@ -3457,7 +3455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>47</v>
       </c>
@@ -3489,13 +3487,13 @@
         <v>186</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L19" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>187</v>
       </c>
@@ -3518,7 +3516,7 @@
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J20">
         <v>6</v>
@@ -3530,7 +3528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>190</v>
       </c>
@@ -3553,7 +3551,7 @@
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J21">
         <v>6</v>
@@ -3565,7 +3563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>191</v>
       </c>
@@ -3588,7 +3586,7 @@
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J22">
         <v>6</v>
@@ -3600,7 +3598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>192</v>
       </c>
@@ -3623,7 +3621,7 @@
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J23">
         <v>6</v>
@@ -3635,7 +3633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>196</v>
       </c>
@@ -3658,7 +3656,7 @@
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J24">
         <v>6</v>
@@ -3670,7 +3668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>197</v>
       </c>
@@ -3693,7 +3691,7 @@
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J25">
         <v>6</v>
@@ -3705,7 +3703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>199</v>
       </c>
@@ -3728,7 +3726,7 @@
         <v>1</v>
       </c>
       <c r="I26" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J26">
         <v>6</v>
@@ -3740,12 +3738,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>269</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>270</v>
       </c>
       <c r="C27" s="3">
         <v>0.83333333333333337</v>
@@ -3763,7 +3761,7 @@
         <v>0</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J27">
         <v>5</v>
@@ -3775,12 +3773,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C28" s="3">
         <v>0.83333333333333337</v>
@@ -3798,7 +3796,7 @@
         <v>0</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J28">
         <v>5</v>
@@ -3810,12 +3808,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C29" s="3">
         <v>0.83333333333333337</v>
@@ -3833,7 +3831,7 @@
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J29">
         <v>5</v>
@@ -3845,34 +3843,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E36" s="5"/>
     </row>
-    <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="1048576" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1048576" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commented capacity calculation beacuse it stop the running
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
     <sheet name="Tasks" sheetId="4" r:id="rId2"/>
-    <sheet name="בקות" sheetId="5" r:id="rId3"/>
+    <sheet name="בקות" sheetId="5" state="hidden" r:id="rId3"/>
     <sheet name="Mishmarot" sheetId="6" r:id="rId4"/>
     <sheet name="סופשים" sheetId="2" state="hidden" r:id="rId5"/>
     <sheet name="הערות" sheetId="3" state="hidden" r:id="rId6"/>
@@ -1606,7 +1606,7 @@
   <dimension ref="A1:L1006"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4275,7 +4275,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6489,7 +6489,7 @@
   <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fixed night tasks length so it wont count as not evening of the next day
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitza\Desktop\automated shifts assignment\Automated-shifts-assignment\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1095196-FA54-4670-9C40-95F8A5A43769}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7911BA41-B8C2-4EB3-A325-495A06D1C9AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
@@ -1623,7 +1623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
@@ -4292,8 +4292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4470,7 +4470,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D4" s="1">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1">
         <v>2</v>
@@ -4511,7 +4511,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D5" s="1">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1">
         <v>2</v>
@@ -4590,7 +4590,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D7" s="1">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F7" s="1">
         <v>2</v>
@@ -4669,7 +4669,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D9" s="1">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F9" s="1">
         <v>2</v>
@@ -5195,7 +5195,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D21" s="3">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F21" s="3">
         <v>4</v>
@@ -5236,7 +5236,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D22" s="3">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F22" s="3">
         <v>4</v>
@@ -5277,7 +5277,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D23" s="3">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F23" s="3">
         <v>4</v>
@@ -5318,7 +5318,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D24" s="3">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="F24" s="3">
         <v>4</v>
@@ -5359,7 +5359,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D25" s="3">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="F25" s="3">
         <v>4</v>
@@ -5400,7 +5400,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D26" s="3">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="F26" s="3">
         <v>4</v>
@@ -5441,7 +5441,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D27" s="3">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F27" s="3">
         <v>4</v>
@@ -5482,7 +5482,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D28" s="3">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F28" s="3">
         <v>2</v>
@@ -5523,7 +5523,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D29" s="3">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F29" s="3">
         <v>2</v>
@@ -5564,7 +5564,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D30" s="3">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F30" s="3">
         <v>2</v>

</xml_diff>

<commit_message>
fixed typos add ub to variety slack variable
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitza\Desktop\automated shifts assignment\Automated-shifts-assignment\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B794DD-211A-43ED-BF75-6E86AE4118F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667F6994-2B45-457B-B970-51FD5C758E5C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="397">
   <si>
     <t>id</t>
   </si>
@@ -693,9 +693,6 @@
   </si>
   <si>
     <t>#0BD9D9</t>
-  </si>
-  <si>
-    <t>sar poduction</t>
   </si>
   <si>
     <t>#762CBF</t>
@@ -1699,7 +1696,7 @@
     </row>
     <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>11</v>
@@ -1720,13 +1717,13 @@
         <v>10</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>326</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>12</v>
@@ -1755,11 +1752,11 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I3" s="7"/>
       <c r="J3" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>14</v>
@@ -1788,11 +1785,11 @@
         <v>10</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>12</v>
@@ -1821,11 +1818,11 @@
         <v>10</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>12</v>
@@ -1854,11 +1851,11 @@
         <v>10</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>12</v>
@@ -1887,13 +1884,13 @@
         <v>10</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I7" s="7">
         <v>13</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>14</v>
@@ -1926,7 +1923,7 @@
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>14</v>
@@ -1955,11 +1952,11 @@
         <v>10</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>12</v>
@@ -1988,11 +1985,11 @@
         <v>10</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>12</v>
@@ -2021,11 +2018,11 @@
         <v>10</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>12</v>
@@ -2054,13 +2051,13 @@
         <v>10</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>27</v>
@@ -2089,13 +2086,13 @@
         <v>10</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I13" s="7">
         <v>2</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>14</v>
@@ -2125,11 +2122,11 @@
         <v>10</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>32</v>
@@ -2158,11 +2155,11 @@
         <v>10</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>12</v>
@@ -2191,11 +2188,11 @@
         <v>10</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>12</v>
@@ -2224,11 +2221,11 @@
         <v>10</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>12</v>
@@ -2257,13 +2254,13 @@
         <v>8</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>12</v>
@@ -2292,13 +2289,13 @@
         <v>8</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>12</v>
@@ -2327,13 +2324,13 @@
         <v>8</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>14</v>
@@ -2362,13 +2359,13 @@
         <v>8</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>47</v>
@@ -2397,13 +2394,13 @@
         <v>0</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>50</v>
@@ -2432,13 +2429,13 @@
         <v>0</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>53</v>
@@ -2468,10 +2465,10 @@
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>56</v>
@@ -2501,10 +2498,10 @@
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>56</v>
@@ -2533,10 +2530,10 @@
         <v>8</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>209</v>
@@ -2568,13 +2565,13 @@
         <v>8</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>64</v>
@@ -2605,7 +2602,7 @@
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
       <c r="J28" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>67</v>
@@ -2634,13 +2631,13 @@
         <v>0</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>70</v>
@@ -2669,13 +2666,13 @@
         <v>0</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>73</v>
@@ -2704,10 +2701,10 @@
         <v>4</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>217</v>
@@ -2742,7 +2739,7 @@
         <v>6</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>209</v>
@@ -2775,7 +2772,7 @@
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>190</v>
@@ -2810,10 +2807,10 @@
         <v>20</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>85</v>
@@ -2842,13 +2839,13 @@
         <v>2</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>88</v>
@@ -2877,13 +2874,13 @@
         <v>2</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>91</v>
@@ -2915,10 +2912,10 @@
         <v>20</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>94</v>
@@ -2947,13 +2944,13 @@
         <v>0</v>
       </c>
       <c r="H38" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="I38" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="I38" s="7" t="s">
-        <v>320</v>
-      </c>
       <c r="J38" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>97</v>
@@ -2985,10 +2982,10 @@
         <v>20</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>100</v>
@@ -3020,7 +3017,7 @@
         <v>3</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>190</v>
@@ -3052,7 +3049,7 @@
         <v>0</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>209</v>
@@ -3063,7 +3060,7 @@
     </row>
     <row r="42" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>110</v>
@@ -3087,10 +3084,10 @@
         <v>5</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>111</v>
@@ -3119,7 +3116,7 @@
         <v>0</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>217</v>
@@ -3130,7 +3127,7 @@
     </row>
     <row r="44" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>116</v>
@@ -3151,13 +3148,13 @@
         <v>0</v>
       </c>
       <c r="H44" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>111</v>
@@ -3165,7 +3162,7 @@
     </row>
     <row r="45" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>118</v>
@@ -4165,8 +4162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4222,7 +4219,7 @@
         <v>182</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>183</v>
@@ -4231,10 +4228,10 @@
         <v>184</v>
       </c>
       <c r="N1" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="O1" s="9" t="s">
         <v>288</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>289</v>
       </c>
       <c r="P1" s="11"/>
       <c r="Q1" s="11"/>
@@ -4282,7 +4279,7 @@
         <v>189</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>190</v>
@@ -4294,7 +4291,7 @@
         <v>1</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4339,7 +4336,7 @@
         <v>0</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4371,7 +4368,7 @@
         <v>197</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>190</v>
@@ -4383,7 +4380,7 @@
         <v>1</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4425,7 +4422,7 @@
         <v>0</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4463,7 +4460,7 @@
         <v>0</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4501,7 +4498,7 @@
         <v>0</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4533,7 +4530,7 @@
         <v>189</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>209</v>
@@ -4545,7 +4542,7 @@
         <v>1</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4577,7 +4574,7 @@
         <v>197</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>209</v>
@@ -4589,7 +4586,7 @@
         <v>1</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4624,7 +4621,7 @@
         <v>189</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>213</v>
@@ -4636,7 +4633,7 @@
         <v>1</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4668,7 +4665,7 @@
         <v>189</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>217</v>
@@ -4680,7 +4677,7 @@
         <v>1</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4688,7 +4685,7 @@
         <v>67</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C12" s="13">
         <v>0.33333333333333331</v>
@@ -4706,14 +4703,14 @@
         <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>189</v>
       </c>
       <c r="K12" s="1"/>
-      <c r="L12" s="3" t="s">
-        <v>219</v>
+      <c r="L12" s="1" t="s">
+        <v>298</v>
       </c>
       <c r="M12" s="3">
         <v>0</v>
@@ -4722,15 +4719,15 @@
         <v>0</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="C13" s="13">
         <v>0.33333333333333331</v>
@@ -4739,7 +4736,7 @@
         <v>9</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F13" s="1">
         <v>0.25</v>
@@ -4751,14 +4748,14 @@
         <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J13" s="1">
         <v>3</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M13" s="3">
         <v>0</v>
@@ -4767,15 +4764,15 @@
         <v>0</v>
       </c>
       <c r="O13" s="29" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C14" s="13">
         <v>0.33333333333333331</v>
@@ -4794,14 +4791,14 @@
         <v>0</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J14" s="1">
         <v>2</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M14" s="3">
         <v>0</v>
@@ -4810,15 +4807,15 @@
         <v>0</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="28" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C15" s="13">
         <v>0.33333333333333331</v>
@@ -4836,14 +4833,14 @@
         <v>0</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J15" s="1">
         <v>2</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M15" s="3">
         <v>0</v>
@@ -4852,15 +4849,15 @@
         <v>0</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C16" s="13">
         <v>0.33333333333333331</v>
@@ -4869,7 +4866,7 @@
         <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F16" s="1">
         <v>0.25</v>
@@ -4881,14 +4878,14 @@
         <v>0</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>189</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="M16" s="3">
         <v>0</v>
@@ -4897,15 +4894,15 @@
         <v>0</v>
       </c>
       <c r="O16" s="29" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C17" s="13">
         <v>0.33333333333333331</v>
@@ -4914,7 +4911,7 @@
         <v>9</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F17" s="1">
         <v>0.25</v>
@@ -4926,14 +4923,14 @@
         <v>0</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>189</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="M17" s="3">
         <v>0</v>
@@ -4942,15 +4939,15 @@
         <v>0</v>
       </c>
       <c r="O17" s="29" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C18" s="13">
         <v>0.33333333333333331</v>
@@ -4959,7 +4956,7 @@
         <v>9</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F18" s="1">
         <v>0.25</v>
@@ -4971,7 +4968,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>189</v>
@@ -4987,15 +4984,15 @@
         <v>0</v>
       </c>
       <c r="O18" s="29" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="28" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C19" s="13">
         <v>0.33333333333333331</v>
@@ -5004,7 +5001,7 @@
         <v>9</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F19" s="1">
         <v>0.25</v>
@@ -5016,14 +5013,14 @@
         <v>0</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J19" s="1">
         <v>1</v>
       </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="M19" s="3">
         <v>0</v>
@@ -5032,16 +5029,16 @@
         <v>0</v>
       </c>
       <c r="O19" s="29" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="P19" s="7"/>
     </row>
     <row r="20" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C20" s="15">
         <v>0.33333333333333331</v>
@@ -5050,7 +5047,7 @@
         <v>9</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F20" s="16">
         <v>0.25</v>
@@ -5062,14 +5059,14 @@
         <v>0</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J20" s="16" t="s">
         <v>189</v>
       </c>
       <c r="K20" s="16"/>
       <c r="L20" s="32" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M20" s="16">
         <v>0</v>
@@ -5078,15 +5075,15 @@
         <v>0</v>
       </c>
       <c r="O20" s="29" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="28" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C21" s="13">
         <v>0.33333333333333331</v>
@@ -5104,7 +5101,7 @@
         <v>1</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J21" s="1">
         <v>6</v>
@@ -5120,15 +5117,15 @@
         <v>1</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="28" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C22" s="13">
         <v>0.33333333333333331</v>
@@ -5146,7 +5143,7 @@
         <v>1</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J22" s="1">
         <v>6</v>
@@ -5162,15 +5159,15 @@
         <v>1</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="28" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C23" s="13">
         <v>0.33333333333333331</v>
@@ -5188,7 +5185,7 @@
         <v>1</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J23" s="1">
         <v>6</v>
@@ -5204,15 +5201,15 @@
         <v>1</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C24" s="13">
         <v>0.83333333333333337</v>
@@ -5230,7 +5227,7 @@
         <v>1</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J24" s="1">
         <v>6</v>
@@ -5246,15 +5243,15 @@
         <v>1</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="28" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C25" s="13">
         <v>0.83333333333333337</v>
@@ -5272,7 +5269,7 @@
         <v>1</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J25" s="1">
         <v>6</v>
@@ -5288,15 +5285,15 @@
         <v>1</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="28" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C26" s="13">
         <v>0.83333333333333337</v>
@@ -5314,7 +5311,7 @@
         <v>1</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J26" s="1">
         <v>6</v>
@@ -5330,15 +5327,15 @@
         <v>1</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="28" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C27" s="13">
         <v>0.33333333333333331</v>
@@ -5356,7 +5353,7 @@
         <v>1</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J27" s="1">
         <v>6</v>
@@ -5372,15 +5369,15 @@
         <v>1</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="28" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C28" s="13">
         <v>0.83333333333333337</v>
@@ -5398,7 +5395,7 @@
         <v>0</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J28" s="1">
         <v>5</v>
@@ -5414,15 +5411,15 @@
         <v>1</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="28" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C29" s="13">
         <v>0.83333333333333337</v>
@@ -5440,7 +5437,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J29" s="1">
         <v>5</v>
@@ -5456,15 +5453,15 @@
         <v>0</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="28" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C30" s="13">
         <v>0.83333333333333337</v>
@@ -5482,7 +5479,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J30" s="1">
         <v>5</v>
@@ -5498,15 +5495,15 @@
         <v>1</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="28" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C31" s="13">
         <v>0.33333333333333331</v>
@@ -5524,7 +5521,7 @@
         <v>0</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -5538,15 +5535,15 @@
         <v>0</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C32" s="13">
         <v>0.33333333333333331</v>
@@ -5564,7 +5561,7 @@
         <v>0</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -5578,15 +5575,15 @@
         <v>0</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="28" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C33" s="13">
         <v>0.33333333333333331</v>
@@ -5604,7 +5601,7 @@
         <v>0</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -5618,15 +5615,15 @@
         <v>0</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="28" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C34" s="13">
         <v>0.83333333333333337</v>
@@ -5645,7 +5642,7 @@
         <v>0</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -5659,15 +5656,15 @@
         <v>0</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="28" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C35" s="13">
         <v>0.83333333333333337</v>
@@ -5686,7 +5683,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -5700,15 +5697,15 @@
         <v>0</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C36" s="13">
         <v>0.83333333333333337</v>
@@ -5727,7 +5724,7 @@
         <v>0</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -5741,15 +5738,15 @@
         <v>0</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="28" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C37" s="13">
         <v>0.33333333333333331</v>
@@ -5768,7 +5765,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -5782,7 +5779,7 @@
         <v>0</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6771,18 +6768,18 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I1" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>268</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I2" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K2" s="4">
         <v>4.4000000000000004</v>
@@ -6790,10 +6787,10 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I3" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K3" s="17">
         <v>5.4</v>
@@ -6801,10 +6798,10 @@
     </row>
     <row r="4" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I4" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K4" s="4">
         <v>6.4</v>
@@ -6812,10 +6809,10 @@
     </row>
     <row r="5" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I5" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K5" s="4">
         <v>7.4</v>
@@ -6823,10 +6820,10 @@
     </row>
     <row r="6" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I6" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="J6" s="8" t="s">
         <v>270</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>271</v>
       </c>
       <c r="K6" s="4">
         <v>8.4</v>
@@ -6842,10 +6839,10 @@
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
       <c r="I7" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K7" s="20">
         <v>9.4</v>
@@ -6876,10 +6873,10 @@
       <c r="G8" s="18"/>
       <c r="H8" s="18"/>
       <c r="I8" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K8" s="20">
         <v>10.4</v>
@@ -6902,10 +6899,10 @@
     </row>
     <row r="9" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I9" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="J9" s="7" t="s">
         <v>270</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>271</v>
       </c>
       <c r="K9" s="4">
         <v>11.4</v>
@@ -6913,10 +6910,10 @@
     </row>
     <row r="10" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I10" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K10" s="4">
         <v>12.4</v>
@@ -6924,10 +6921,10 @@
     </row>
     <row r="11" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I11" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="J11" s="7" t="s">
         <v>270</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>271</v>
       </c>
       <c r="K11" s="4">
         <v>13.4</v>
@@ -6943,10 +6940,10 @@
       <c r="G12" s="21"/>
       <c r="H12" s="21"/>
       <c r="I12" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K12" s="20">
         <v>14.4</v>
@@ -6977,10 +6974,10 @@
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K13" s="20">
         <v>15.4</v>
@@ -7011,10 +7008,10 @@
       <c r="G14" s="18"/>
       <c r="H14" s="18"/>
       <c r="I14" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J14" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K14" s="20">
         <v>16.399999999999999</v>
@@ -7045,10 +7042,10 @@
       <c r="G15" s="18"/>
       <c r="H15" s="18"/>
       <c r="I15" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J15" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K15" s="20">
         <v>17.399999999999999</v>
@@ -7079,10 +7076,10 @@
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
       <c r="I16" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="J16" s="23" t="s">
         <v>270</v>
-      </c>
-      <c r="J16" s="23" t="s">
-        <v>271</v>
       </c>
       <c r="K16" s="24">
         <v>18.399999999999999</v>
@@ -7113,10 +7110,10 @@
       <c r="G17" s="22"/>
       <c r="H17" s="22"/>
       <c r="I17" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="J17" s="23" t="s">
         <v>270</v>
-      </c>
-      <c r="J17" s="23" t="s">
-        <v>271</v>
       </c>
       <c r="K17" s="24">
         <v>19.399999999999999</v>
@@ -7139,10 +7136,10 @@
     </row>
     <row r="18" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I18" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="J18" s="7" t="s">
         <v>270</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>271</v>
       </c>
       <c r="K18" s="4">
         <v>20.399999999999999</v>
@@ -7150,10 +7147,10 @@
     </row>
     <row r="19" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I19" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="J19" s="7" t="s">
         <v>270</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>271</v>
       </c>
       <c r="K19" s="4">
         <v>21.4</v>
@@ -7161,10 +7158,10 @@
     </row>
     <row r="20" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I20" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="J20" s="7" t="s">
         <v>270</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>271</v>
       </c>
       <c r="K20" s="4">
         <v>22.4</v>
@@ -7180,10 +7177,10 @@
       <c r="G21" s="25"/>
       <c r="H21" s="25"/>
       <c r="I21" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J21" s="26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K21" s="27">
         <v>23.4</v>
@@ -7214,10 +7211,10 @@
       <c r="G22" s="25"/>
       <c r="H22" s="25"/>
       <c r="I22" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J22" s="26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K22" s="27">
         <v>24.4</v>
@@ -7240,10 +7237,10 @@
     </row>
     <row r="23" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I23" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="J23" s="7" t="s">
         <v>270</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>271</v>
       </c>
       <c r="K23" s="4">
         <v>25.4</v>
@@ -7251,10 +7248,10 @@
     </row>
     <row r="24" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I24" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K24" s="4">
         <v>26.4</v>
@@ -7262,10 +7259,10 @@
     </row>
     <row r="25" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I25" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K25" s="4">
         <v>27.4</v>
@@ -7273,10 +7270,10 @@
     </row>
     <row r="26" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I26" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K26" s="4">
         <v>28.4</v>
@@ -7284,10 +7281,10 @@
     </row>
     <row r="27" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I27" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K27" s="4">
         <v>29.4</v>
@@ -7303,10 +7300,10 @@
       <c r="G28" s="18"/>
       <c r="H28" s="18"/>
       <c r="I28" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J28" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K28" s="20">
         <v>30.4</v>
@@ -7337,10 +7334,10 @@
       <c r="G29" s="18"/>
       <c r="H29" s="18"/>
       <c r="I29" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K29" s="20">
         <v>1.5</v>
@@ -7370,8 +7367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.09765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7395,75 +7392,75 @@
         <v>199</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="H1" t="s">
         <v>297</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>298</v>
       </c>
-      <c r="I1" t="s">
-        <v>299</v>
-      </c>
       <c r="J1" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="F2" s="17" t="s">
         <v>302</v>
       </c>
-      <c r="F2" s="17" t="s">
-        <v>303</v>
-      </c>
       <c r="G2" t="s">
+        <v>361</v>
+      </c>
+      <c r="H2" t="s">
+        <v>378</v>
+      </c>
+      <c r="I2" t="s">
         <v>362</v>
-      </c>
-      <c r="H2" t="s">
-        <v>379</v>
-      </c>
-      <c r="I2" t="s">
-        <v>363</v>
       </c>
       <c r="J2">
         <v>16</v>
@@ -8510,12 +8507,12 @@
         <v>1</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B2" s="29">
         <v>1</v>
@@ -8523,7 +8520,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B3" s="29">
         <v>2</v>
@@ -8531,7 +8528,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B4" s="29">
         <v>2</v>
@@ -8546,18 +8543,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F1F3A4-F739-4A89-BCC3-9CBCDA8AC30A}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -9049,34 +9046,34 @@
   <sheetData>
     <row r="2" spans="9:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I2" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>273</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="3" spans="9:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I3" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="9:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I4" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>276</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="5" spans="9:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I5" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>278</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wv equipment is not compatible with bakut added #TODO to fix weeks calculation - affects balancing shifts between the weeks
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitza\Desktop\automated shifts assignment\Automated-shifts-assignment\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667F6994-2B45-457B-B970-51FD5C758E5C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAC96F5-71CF-4F79-81A5-86F1FB933453}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4163,7 +4163,7 @@
   <dimension ref="A1:AB1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4291,7 +4291,7 @@
         <v>1</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4336,7 +4336,7 @@
         <v>0</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added option to request a task in a list of days
</commit_message>
<xml_diff>
--- a/DATA/DB.xlsx
+++ b/DATA/DB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitza\Desktop\automated shifts assignment\Automated-shifts-assignment\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAC96F5-71CF-4F79-81A5-86F1FB933453}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A027280F-6E85-487B-9982-4D3E8AD2135A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="תורנויות" sheetId="7" state="hidden" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Operators!$A$1:$L$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Operators!$A$1:$M$46</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="402">
   <si>
     <t>id</t>
   </si>
@@ -956,24 +956,9 @@
     <t>6,7,8,12,13</t>
   </si>
   <si>
-    <t>3,6,10,17,24,31</t>
-  </si>
-  <si>
     <t>2,20</t>
   </si>
   <si>
-    <t>14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31</t>
-  </si>
-  <si>
-    <t>2,3,4,5,6,7,8,9,10,11,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31</t>
-  </si>
-  <si>
-    <t>2,3,10,11,12,13,19,20,23,24,25,27,30,31</t>
-  </si>
-  <si>
-    <t>2,3,4,7,8,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31</t>
-  </si>
-  <si>
     <t>13,14,15,16,17,21,22</t>
   </si>
   <si>
@@ -998,24 +983,6 @@
     <t>13,14,15,16,17,18,19,21,22</t>
   </si>
   <si>
-    <t>6,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31</t>
-  </si>
-  <si>
-    <t>9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31</t>
-  </si>
-  <si>
-    <t>6,7,8,9,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31</t>
-  </si>
-  <si>
-    <t>2,5,10,11,12,13,19,20,23,24,25,27,30,31</t>
-  </si>
-  <si>
-    <t>6,11,31,14,15,21,22</t>
-  </si>
-  <si>
-    <t>6, 18</t>
-  </si>
-  <si>
     <t>5,13,26,14,15,7,8</t>
   </si>
   <si>
@@ -1031,33 +998,12 @@
     <t>5,9,16,23,30,28,29</t>
   </si>
   <si>
-    <t>20,31,21,22,14,15</t>
-  </si>
-  <si>
-    <t>4,13,19,25,31,14,15,28,29</t>
-  </si>
-  <si>
-    <t>4,11,20,31,14,15,21,22</t>
-  </si>
-  <si>
     <t>18,20</t>
   </si>
   <si>
-    <t>4,10,20,31,28,29,14,15</t>
-  </si>
-  <si>
-    <t>10,20,31,14,15,28,29</t>
-  </si>
-  <si>
     <t>3,10,20,24,14,15,21,22</t>
   </si>
   <si>
-    <t>3,11,20,31,14,15,21,22</t>
-  </si>
-  <si>
-    <t>3,11,20,25,31,7,8,14,15</t>
-  </si>
-  <si>
     <t>2,13,21,22</t>
   </si>
   <si>
@@ -1076,9 +1022,6 @@
     <t>13,21,22,23</t>
   </si>
   <si>
-    <t>11,18,25,31,14,15</t>
-  </si>
-  <si>
     <t>13,14,15,18,19,20,24,26</t>
   </si>
   <si>
@@ -1118,9 +1061,6 @@
     <t>20,21,22,23</t>
   </si>
   <si>
-    <t>2,6,7,8,13,18,19,20,21,22,23,24,25,26,27,28,29,30,31</t>
-  </si>
-  <si>
     <t>2,3,4,5,6,9,10,11,12,13,18,19,20,23,24,25,26,27</t>
   </si>
   <si>
@@ -1227,6 +1167,81 @@
   </si>
   <si>
     <t>dates</t>
+  </si>
+  <si>
+    <t>6,18</t>
+  </si>
+  <si>
+    <t>2,9,13,30</t>
+  </si>
+  <si>
+    <t>4,12,16,17,18</t>
+  </si>
+  <si>
+    <t>6,7,8,9,10</t>
+  </si>
+  <si>
+    <t>4,25,26</t>
+  </si>
+  <si>
+    <t>Preferred days</t>
+  </si>
+  <si>
+    <t>6,11,14,15,21,22</t>
+  </si>
+  <si>
+    <t>20,21,22,14,15</t>
+  </si>
+  <si>
+    <t>4,13,19,25,14,15,28,29</t>
+  </si>
+  <si>
+    <t>4,11,20,14,15,21,22</t>
+  </si>
+  <si>
+    <t>4,10,20,28,29,14,15</t>
+  </si>
+  <si>
+    <t>10,20,14,15,28,29</t>
+  </si>
+  <si>
+    <t>3,11,20,14,15,21,22</t>
+  </si>
+  <si>
+    <t>11,18,25,14,15</t>
+  </si>
+  <si>
+    <t>3,11,20,25,7,8,14,15</t>
+  </si>
+  <si>
+    <t>2,3,10,11,12,13,19,20,23,24,25,27,30</t>
+  </si>
+  <si>
+    <t>2,5,10,11,12,13,19,20,23,24,25,27,30</t>
+  </si>
+  <si>
+    <t>2,6,7,8,13,18,19,20,21,22,23,24,25,26,27,28,29,30</t>
+  </si>
+  <si>
+    <t>2,3,4,7,8,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30</t>
+  </si>
+  <si>
+    <t>2,3,4,5,6,7,8,9,10,11,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30</t>
+  </si>
+  <si>
+    <t>6,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30</t>
+  </si>
+  <si>
+    <t>9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30</t>
+  </si>
+  <si>
+    <t>14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30</t>
+  </si>
+  <si>
+    <t>6,7,8,9,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30</t>
+  </si>
+  <si>
+    <t>3,6,10,17,24</t>
   </si>
 </sst>
 </file>
@@ -1637,29 +1652,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1002"/>
+  <dimension ref="A1:M1002"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.09765625" customWidth="1"/>
-    <col min="3" max="3" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.09765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.69921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.59765625" customWidth="1"/>
-    <col min="9" max="9" width="26.796875" customWidth="1"/>
-    <col min="10" max="10" width="74.19921875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="64.09765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="26" width="8.59765625" customWidth="1"/>
+    <col min="7" max="7" width="12.296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="62.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.796875" customWidth="1"/>
+    <col min="11" max="11" width="65.8984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="67.69921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="27" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1687,14 +1703,17 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>279</v>
       </c>
@@ -1717,19 +1736,22 @@
         <v>10</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>324</v>
+        <v>383</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>364</v>
+        <v>377</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>378</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1752,17 +1774,18 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="I3" s="7"/>
-      <c r="J3" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="J3" s="7"/>
+      <c r="K3" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1785,17 +1808,18 @@
         <v>10</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="I4" s="7"/>
-      <c r="J4" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="J4" s="7"/>
+      <c r="K4" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1818,17 +1842,20 @@
         <v>10</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="I5" s="7"/>
-      <c r="J5" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="J5" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1851,17 +1878,18 @@
         <v>10</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="I6" s="7"/>
-      <c r="J6" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="K6" s="1" t="s">
+      <c r="J6" s="7"/>
+      <c r="K6" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1884,19 +1912,22 @@
         <v>10</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="I7" s="7">
         <v>13</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="K7" s="1" t="s">
+      <c r="J7" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1922,14 +1953,17 @@
         <v>5</v>
       </c>
       <c r="I8" s="7"/>
-      <c r="J8" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="K8" s="1" t="s">
+      <c r="J8" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1952,17 +1986,18 @@
         <v>10</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>331</v>
+        <v>384</v>
       </c>
       <c r="I9" s="7"/>
-      <c r="J9" s="1" t="s">
-        <v>364</v>
-      </c>
+      <c r="J9" s="7"/>
       <c r="K9" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1985,17 +2020,18 @@
         <v>10</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>332</v>
+        <v>385</v>
       </c>
       <c r="I10" s="7"/>
-      <c r="J10" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="K10" s="1" t="s">
+      <c r="J10" s="7"/>
+      <c r="K10" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -2018,17 +2054,18 @@
         <v>10</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>333</v>
+        <v>386</v>
       </c>
       <c r="I11" s="7"/>
-      <c r="J11" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="K11" s="1" t="s">
+      <c r="J11" s="7"/>
+      <c r="K11" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -2051,19 +2088,20 @@
         <v>10</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>335</v>
+        <v>387</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>371</v>
-      </c>
+        <v>320</v>
+      </c>
+      <c r="J12" s="7"/>
       <c r="K12" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -2086,20 +2124,21 @@
         <v>10</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>336</v>
+        <v>388</v>
       </c>
       <c r="I13" s="7">
         <v>2</v>
       </c>
-      <c r="J13" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="K13" s="1" t="s">
+      <c r="J13" s="7"/>
+      <c r="K13" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L13" s="3"/>
-    </row>
-    <row r="14" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -2122,17 +2161,18 @@
         <v>10</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="I14" s="7"/>
-      <c r="J14" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="K14" s="1" t="s">
+      <c r="J14" s="7"/>
+      <c r="K14" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -2155,17 +2195,18 @@
         <v>10</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>338</v>
+        <v>389</v>
       </c>
       <c r="I15" s="7"/>
-      <c r="J15" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="K15" s="1" t="s">
+      <c r="J15" s="7"/>
+      <c r="K15" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -2188,17 +2229,18 @@
         <v>10</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>346</v>
+        <v>390</v>
       </c>
       <c r="I16" s="7"/>
-      <c r="J16" s="1" t="s">
-        <v>364</v>
-      </c>
+      <c r="J16" s="7"/>
       <c r="K16" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="L16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -2221,17 +2263,18 @@
         <v>10</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>339</v>
+        <v>391</v>
       </c>
       <c r="I17" s="7"/>
-      <c r="J17" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="K17" s="1" t="s">
+      <c r="J17" s="7"/>
+      <c r="K17" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="L17" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -2254,19 +2297,20 @@
         <v>8</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>348</v>
+        <v>329</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>365</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="J18" s="7"/>
       <c r="K18" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="L18" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -2289,19 +2333,20 @@
         <v>8</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>350</v>
+        <v>331</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>365</v>
-      </c>
+        <v>330</v>
+      </c>
+      <c r="J19" s="7"/>
       <c r="K19" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="L19" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -2324,19 +2369,20 @@
         <v>8</v>
       </c>
       <c r="H20" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="J20" s="7"/>
+      <c r="K20" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="I20" s="7" t="s">
-        <v>351</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -2359,19 +2405,20 @@
         <v>8</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="K21" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="J21" s="7"/>
+      <c r="K21" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -2394,19 +2441,20 @@
         <v>0</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="I22" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="J22" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="K22" s="1" t="s">
+      <c r="J22" s="7"/>
+      <c r="K22" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="L22" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>71</v>
       </c>
@@ -2429,19 +2477,20 @@
         <v>0</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>345</v>
+        <v>327</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="K23" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="J23" s="7"/>
+      <c r="K23" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="L23" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -2465,16 +2514,17 @@
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="K24" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="J24" s="7"/>
+      <c r="K24" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="L24" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -2498,16 +2548,17 @@
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="K25" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="J25" s="7"/>
+      <c r="K25" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="L25" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>78</v>
       </c>
@@ -2530,19 +2581,20 @@
         <v>8</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>356</v>
-      </c>
-      <c r="J26" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="J26" s="7"/>
+      <c r="K26" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -2565,19 +2617,20 @@
         <v>8</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>359</v>
+        <v>340</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>358</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="K27" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="J27" s="7"/>
+      <c r="K27" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="L27" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -2601,14 +2654,15 @@
       </c>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
-      <c r="J28" s="3" t="s">
+      <c r="J28" s="7"/>
+      <c r="K28" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -2631,19 +2685,20 @@
         <v>0</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>341</v>
+        <v>323</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="K29" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="J29" s="7"/>
+      <c r="K29" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="L29" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -2666,19 +2721,20 @@
         <v>0</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>343</v>
+        <v>325</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="K30" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="J30" s="7"/>
+      <c r="K30" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="L30" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>92</v>
       </c>
@@ -2704,16 +2760,17 @@
         <v>304</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="J31" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="J31" s="7"/>
+      <c r="K31" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>95</v>
       </c>
@@ -2739,16 +2796,17 @@
         <v>6</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="J32" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="J32" s="7"/>
+      <c r="K32" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="L32" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>98</v>
       </c>
@@ -2772,16 +2830,17 @@
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="J33" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="J33" s="7"/>
+      <c r="K33" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="L33" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>101</v>
       </c>
@@ -2807,16 +2866,17 @@
         <v>20</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="K34" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="J34" s="7"/>
+      <c r="K34" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="L34" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>104</v>
       </c>
@@ -2839,19 +2899,20 @@
         <v>2</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="K35" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="J35" s="7"/>
+      <c r="K35" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="L35" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>106</v>
       </c>
@@ -2874,19 +2935,20 @@
         <v>2</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="K36" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="J36" s="7"/>
+      <c r="K36" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="L36" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>107</v>
       </c>
@@ -2912,16 +2974,17 @@
         <v>20</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>317</v>
-      </c>
-      <c r="J37" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="K37" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="J37" s="7"/>
+      <c r="K37" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="L37" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>108</v>
       </c>
@@ -2944,19 +3007,20 @@
         <v>0</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="K38" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="J38" s="7"/>
+      <c r="K38" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="L38" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>109</v>
       </c>
@@ -2984,14 +3048,15 @@
       <c r="I39" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="J39" s="1" t="s">
-        <v>366</v>
-      </c>
+      <c r="J39" s="7"/>
       <c r="K39" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="L39" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>112</v>
       </c>
@@ -3017,16 +3082,17 @@
         <v>3</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="J40" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="J40" s="7"/>
+      <c r="K40" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="L40" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>115</v>
       </c>
@@ -3049,16 +3115,17 @@
         <v>0</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>321</v>
-      </c>
-      <c r="J41" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="J41" s="7"/>
+      <c r="K41" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="K41" s="1" t="s">
+      <c r="L41" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>280</v>
       </c>
@@ -3084,16 +3151,17 @@
         <v>5</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>368</v>
-      </c>
+        <v>399</v>
+      </c>
+      <c r="J42" s="7"/>
       <c r="K42" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="L42" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>117</v>
       </c>
@@ -3116,16 +3184,17 @@
         <v>0</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>322</v>
-      </c>
-      <c r="J43" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="J43" s="7"/>
+      <c r="K43" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="L43" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>281</v>
       </c>
@@ -3148,19 +3217,20 @@
         <v>0</v>
       </c>
       <c r="H44" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>368</v>
-      </c>
+        <v>401</v>
+      </c>
+      <c r="J44" s="7"/>
       <c r="K44" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="L44" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>282</v>
       </c>
@@ -3183,19 +3253,20 @@
         <v>0</v>
       </c>
       <c r="I45" s="7"/>
-      <c r="J45" s="1" t="s">
+      <c r="J45" s="7"/>
+      <c r="K45" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="K45" s="1" t="s">
+      <c r="L45" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
-      <c r="J46" s="3"/>
-    </row>
-    <row r="47" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4151,7 +4222,7 @@
     <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:L46" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:M46" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4162,7 +4233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
@@ -4219,7 +4290,7 @@
         <v>182</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>395</v>
+        <v>375</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>183</v>
@@ -4279,7 +4350,7 @@
         <v>189</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>190</v>
@@ -4368,7 +4439,7 @@
         <v>197</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>190</v>
@@ -4530,7 +4601,7 @@
         <v>189</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>209</v>
@@ -4574,7 +4645,7 @@
         <v>197</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>209</v>
@@ -4621,7 +4692,7 @@
         <v>189</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>213</v>
@@ -4665,7 +4736,7 @@
         <v>189</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>217</v>
@@ -4885,7 +4956,7 @@
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
-        <v>369</v>
+        <v>349</v>
       </c>
       <c r="M16" s="3">
         <v>0</v>
@@ -4930,7 +5001,7 @@
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1" t="s">
-        <v>370</v>
+        <v>350</v>
       </c>
       <c r="M17" s="3">
         <v>0</v>
@@ -5500,10 +5571,10 @@
     </row>
     <row r="31" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="28" t="s">
-        <v>386</v>
+        <v>366</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>379</v>
+        <v>359</v>
       </c>
       <c r="C31" s="13">
         <v>0.33333333333333331</v>
@@ -5540,10 +5611,10 @@
     </row>
     <row r="32" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
-        <v>387</v>
+        <v>367</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>380</v>
+        <v>360</v>
       </c>
       <c r="C32" s="13">
         <v>0.33333333333333331</v>
@@ -5580,10 +5651,10 @@
     </row>
     <row r="33" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="28" t="s">
-        <v>388</v>
+        <v>368</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>381</v>
+        <v>361</v>
       </c>
       <c r="C33" s="13">
         <v>0.33333333333333331</v>
@@ -5620,10 +5691,10 @@
     </row>
     <row r="34" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="28" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>382</v>
+        <v>362</v>
       </c>
       <c r="C34" s="13">
         <v>0.83333333333333337</v>
@@ -5661,10 +5732,10 @@
     </row>
     <row r="35" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="28" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>383</v>
+        <v>363</v>
       </c>
       <c r="C35" s="13">
         <v>0.83333333333333337</v>
@@ -5702,10 +5773,10 @@
     </row>
     <row r="36" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="28" t="s">
-        <v>391</v>
+        <v>371</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>384</v>
+        <v>364</v>
       </c>
       <c r="C36" s="13">
         <v>0.83333333333333337</v>
@@ -5743,10 +5814,10 @@
     </row>
     <row r="37" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="28" t="s">
-        <v>392</v>
+        <v>372</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>385</v>
+        <v>365</v>
       </c>
       <c r="C37" s="13">
         <v>0.33333333333333331</v>
@@ -7413,33 +7484,33 @@
         <v>298</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>379</v>
+        <v>359</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>380</v>
+        <v>360</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>381</v>
+        <v>361</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>382</v>
+        <v>362</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>383</v>
+        <v>363</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>384</v>
+        <v>364</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>385</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>362</v>
+        <v>342</v>
       </c>
       <c r="B2" t="s">
-        <v>393</v>
+        <v>373</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>299</v>
@@ -7454,13 +7525,13 @@
         <v>302</v>
       </c>
       <c r="G2" t="s">
-        <v>361</v>
+        <v>341</v>
       </c>
       <c r="H2" t="s">
-        <v>378</v>
+        <v>358</v>
       </c>
       <c r="I2" t="s">
-        <v>362</v>
+        <v>342</v>
       </c>
       <c r="J2">
         <v>16</v>
@@ -8549,12 +8620,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>396</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>